<commit_message>
Practice & new checklist added
</commit_message>
<xml_diff>
--- a/JavaPrograms/Work Done.xlsx
+++ b/JavaPrograms/Work Done.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" activeTab="4"/>
+    <workbookView windowWidth="23040" windowHeight="8280" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Python" sheetId="5" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="83">
   <si>
     <t>Questions</t>
   </si>
@@ -857,6 +857,22 @@
 Is arr[2] == 1? → 7 == 1 ❌
 Is arr[3] == 1? → 1 == 1 ✅ found at index 3
 Stop searching.</t>
+  </si>
+  <si>
+    <t>Math in Java</t>
+  </si>
+  <si>
+    <t>Summary Table
+Function Meaning Example
+Math.abs(x) absolute value abs(-10) → 10
+Math.min(a,b) smaller number min(4,9) → 4
+Math.max(a,b) bigger number max(4,9) → 9
+Math.ceil(x) round up ceil(4.2) → 5.0
+Math.floor(x) round down floor(4.8) → 4.0
+Math.round(x) nearest integer round(4.5) → 5
+Math.pow(a,b) a to the power b pow(2,3) → 8.0
+Math.sqrt(x) square root sqrt(16) → 4.0
+Math.random() random 0–1 random() → 0.53</t>
   </si>
   <si>
     <t>Sorting Algorithm</t>
@@ -2635,7 +2651,7 @@
   <dimension ref="A1:F114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B8"/>
+      <selection activeCell="A9" sqref="A9:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -3781,7 +3797,7 @@
   <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -3803,7 +3819,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" ht="144" spans="1:3">
+    <row r="2" ht="201.6" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>41</v>
       </c>
@@ -3814,7 +3830,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" ht="86.4" spans="1:3">
+    <row r="3" ht="100.8" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>44</v>
       </c>
@@ -3834,7 +3850,7 @@
       </c>
       <c r="C4" s="6"/>
     </row>
-    <row r="5" ht="115.2" spans="1:3">
+    <row r="5" ht="129.6" spans="1:3">
       <c r="A5" s="7" t="s">
         <v>49</v>
       </c>
@@ -3870,7 +3886,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" ht="86.4" spans="1:3">
+    <row r="8" ht="115.2" spans="1:3">
       <c r="A8" s="8" t="s">
         <v>59</v>
       </c>
@@ -3913,7 +3929,7 @@
       <c r="B12" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="7" t="s">
         <v>69</v>
       </c>
     </row>
@@ -3922,40 +3938,44 @@
       <c r="B13" s="8"/>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="6"/>
+    <row r="14" ht="158.4" spans="1:3">
+      <c r="A14" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="12"/>
     </row>
     <row r="15" ht="43.2" spans="1:3">
       <c r="A15" s="11" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C15" s="7"/>
     </row>
     <row r="16" ht="129.6" spans="1:3">
       <c r="A16" s="11" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="17" ht="187.2" spans="1:3">
       <c r="A17" s="11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -4255,7 +4275,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4270,7 +4290,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
@@ -4512,7 +4532,7 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>

</xml_diff>

<commit_message>
18-11-25 MergeSort CountInversions & Work Done
</commit_message>
<xml_diff>
--- a/JavaPrograms/Work Done.xlsx
+++ b/JavaPrograms/Work Done.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="113">
   <si>
     <r>
       <rPr>
@@ -1141,6 +1141,13 @@
   </si>
   <si>
     <t>Merge Two Sorted Arrays Using Merge Technique</t>
+  </si>
+  <si>
+    <t>Problem 1 — Count Inversions (classic MergeSort problem)
+Input: [2, 4, 1, 3, 5]
+Output: 3
+(Because (2,1), (4,1), (4,3) are inversions)
+👉 This uses the merge logic with one small modification.</t>
   </si>
   <si>
     <t>https://www.notion.so/DSA-PATTERN-ROADMAP-2a285e32939580ff8596d7c9fbb7e0b3</t>
@@ -4864,8 +4871,8 @@
   <sheetPr/>
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
@@ -4967,8 +4974,10 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="11"/>
+    <row r="19" ht="72" spans="1:1">
+      <c r="A19" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="11"/>
@@ -4992,17 +5001,17 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -5043,7 +5052,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5058,7 +5067,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
@@ -5300,7 +5309,7 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -5486,7 +5495,7 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -15083,10 +15092,10 @@
   <sheetData>
     <row r="1" ht="409" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:1">

</xml_diff>

<commit_message>
20-11-25 QuickSort Dutch National FLag Pattern
</commit_message>
<xml_diff>
--- a/JavaPrograms/Work Done.xlsx
+++ b/JavaPrograms/Work Done.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8280" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="8280" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="DSA plan" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="118">
   <si>
     <r>
       <rPr>
@@ -630,6 +630,12 @@
     <t>Quick Sort</t>
   </si>
   <si>
+    <t xml:space="preserve">QuickSort with Middle Pivot </t>
+  </si>
+  <si>
+    <t>Quick sort Duplicate &amp; descending order</t>
+  </si>
+  <si>
     <t>Recall</t>
   </si>
   <si>
@@ -1118,6 +1124,57 @@
 Partition returns the pivot’s final correct index.                                                                                          It has 2 brains:
 quickSort() → splits
 partition() → does the heavy rearranging</t>
+  </si>
+  <si>
+    <t>Quick Sort Pattern Rec</t>
+  </si>
+  <si>
+    <t>✅ 1. Lomuto Partition (pivot = last element)
+Use this when:
+Array has no duplicates or very few duplicates
+Simpler problems
+Teaching / basic implementations
+Cleanest code (your standard QuickSort)
+Why?
+Because Lomuto does terrible when many items are the same. It moves them one-by-one → becomes slow.
+Pattern recognition:
+If constraints look easy…
+If array values look random…
+If no emphasis on duplicates…
+→ Lomuto is fine.
+✅ 2. Hoare Partition (pivot = middle element)
+Use this when:
+Array is large
+You want fast average performance
+Input may be partially sorted
+You want fewer swaps
+Why?
+Hoare partition is faster (fewer swaps, better partitioning), but trickier to implement.
+Pattern recognition:
+If problem says:
+Use middle pivot OR
+Avoid worst-case OR
+Do in-place with fewer swaps OR
+"Partition until left pointer &gt; right pointer"
+→ That’s Hoare.
+✅ 3. Dutch National Flag Partition (3-way partition)
+Use this when:
+Array contains a lot of duplicates
+Pivot duplicates must be grouped together
+Problem says “sort colors” or “group 0s,1s,2s”
+Classic example:
+LeetCode 75. Sort Colors
+QuickSort on array with many repeated numbers
+Pattern recognition:
+If problem has ANY of these phrases:
+"0, 1, 2"
+"colors"
+"group equal elements"
+"many duplicates"
+"3-way partitioning"
+“DNF” / “Dutch flag”
+“avoid worst-case when many are equal”
+→ Use DNF QuickSort.</t>
   </si>
   <si>
     <t>3 Merge Sort Problems (Simple → Medium)
@@ -3966,8 +4023,8 @@
   <sheetPr/>
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C9" sqref="C2:C9"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="4"/>
@@ -4230,19 +4287,35 @@
       <c r="C16" s="30">
         <v>45982</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="40"/>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
+      <c r="A17" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="30">
+        <v>45980</v>
+      </c>
+      <c r="C17" s="30">
+        <v>45982</v>
+      </c>
       <c r="D17" s="8"/>
-      <c r="E17" s="40"/>
+      <c r="E17" s="39" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
+      <c r="A18" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="30">
+        <v>45981</v>
+      </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="40"/>
@@ -4337,7 +4410,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B1" s="14"/>
     </row>
@@ -4349,26 +4422,26 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="14" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4379,10 +4452,10 @@
     </row>
     <row r="7" s="21" customFormat="1" ht="57.6" spans="1:2">
       <c r="A7" s="25" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -4396,8 +4469,8 @@
   <sheetPr/>
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -4410,155 +4483,155 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" ht="201.6" spans="1:3">
       <c r="A2" s="14" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" ht="100.8" spans="1:3">
       <c r="A3" s="14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" ht="72" spans="1:3">
       <c r="A4" s="16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C4" s="14"/>
     </row>
     <row r="5" ht="129.6" spans="1:3">
       <c r="A5" s="15" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" ht="86.4" spans="1:4">
       <c r="A6" s="15" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" ht="158.4" spans="1:3">
       <c r="A7" s="8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" ht="115.2" spans="1:3">
       <c r="A8" s="10" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C8" s="14"/>
     </row>
     <row r="9" ht="129.6" spans="1:3">
       <c r="A9" s="10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C9" s="14"/>
     </row>
     <row r="10" ht="129.6" spans="1:3">
       <c r="A10" s="8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C10" s="14"/>
     </row>
     <row r="11" ht="158.4" spans="1:3">
       <c r="A11" s="8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C11" s="14"/>
     </row>
     <row r="12" ht="115.2" spans="1:3">
       <c r="A12" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" ht="158.4" spans="1:3">
       <c r="A13" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" ht="158.4" spans="1:3">
       <c r="A14" s="8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C14" s="15"/>
     </row>
     <row r="15" ht="43.2" spans="1:3">
       <c r="A15" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C15" s="15"/>
     </row>
@@ -4567,10 +4640,10 @@
         <v>34</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" ht="187.2" spans="1:3">
@@ -4578,10 +4651,10 @@
         <v>36</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" ht="273.6" spans="1:4">
@@ -4589,13 +4662,13 @@
         <v>37</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" ht="158.4" spans="1:4">
@@ -4603,13 +4676,13 @@
         <v>38</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" ht="302.4" spans="1:4">
@@ -4617,18 +4690,22 @@
         <v>41</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" ht="409.5" spans="1:3">
+      <c r="A21" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>106</v>
+      </c>
       <c r="C21" s="14"/>
     </row>
     <row r="22" spans="1:3">
@@ -4912,72 +4989,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="10" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:1">
@@ -4995,7 +5072,7 @@
         <v>38</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -5005,7 +5082,7 @@
     </row>
     <row r="19" ht="72" spans="1:1">
       <c r="A19" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:1">
@@ -5030,17 +5107,17 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -5081,7 +5158,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="3" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5096,7 +5173,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="5" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
@@ -5338,7 +5415,7 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="3" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -5524,7 +5601,7 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="4" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -15121,10 +15198,10 @@
   <sheetData>
     <row r="1" ht="409" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:1">

</xml_diff>

<commit_message>
24-11-25  Sliding Window MaxSumSubarrayK
</commit_message>
<xml_diff>
--- a/JavaPrograms/Work Done.xlsx
+++ b/JavaPrograms/Work Done.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="139">
   <si>
     <r>
       <rPr>
@@ -1289,10 +1289,40 @@
 You update the sum without recounting all cookies again</t>
   </si>
   <si>
-    <t>So if last window sum was:
-[2,1,5] = 8
-Slide → [1,5,1]
-New sum = 8 - 2 + 1 = 7</t>
+    <t>Sliding Window — Animation Style (Your Example)
+Array:[3, 5, 1, 5, 1, 2]
+k = 3
+We want max sum of any 3 continuous elements.
+Step 1: Build the first window
+Take first 3 values
+[ 3, 5, 1 ] 5 1 2
+   ↑  ↑  ↑
+sum = 3 + 5 + 1 = 9  
+maxSum = 9
+Step 2: Slide the window right by 1
+Window moves one step → drop left value, add next value
+Old: 3
+New entering: 5
+3 [ 5, 1, 5 ] 1 2
+      ↑  ↑  ↑
+windowSum = 9 - 3 + 5 = 11  
+maxSum = 11
+Step 3: Slide again
+Drop 5, add 1
+3 5 [ 1, 5, 1 ] 2
+         ↑  ↑  ↑
+windowSum = 11 - 5 + 1 = 7  
+maxSum = 11
+Step 4: Slide again
+Drop 1, add 2
+3 5 1 [ 5, 1, 2 ]
+            ↑  ↑  ↑
+windowSum = 7 - 1 + 2 = 8  
+maxSum = 11</t>
+  </si>
+  <si>
+    <t>Quick rule to remember
+If the question says “longest / max / min / count / sum of subarray” with continuous elements, think Sliding Window.</t>
   </si>
   <si>
     <t>QuickSelect</t>
@@ -2602,7 +2632,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2661,6 +2691,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3369,246 +3402,246 @@
   </cols>
   <sheetData>
     <row r="1" ht="90" customHeight="1" spans="1:6">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="44" t="s">
+      <c r="B1" s="44"/>
+      <c r="C1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="46" t="s">
+      <c r="D1" s="46"/>
+      <c r="E1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="46"/>
+      <c r="F1" s="47"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="48" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="8"/>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="48" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="10"/>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="55"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
     </row>
     <row r="15" ht="15" customHeight="1" spans="1:6">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
-      <c r="C16" s="60" t="s">
+      <c r="C16" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="61"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="48" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="8"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="63"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="64"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="65"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="66"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
-      <c r="C24" s="66" t="s">
+      <c r="C24" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="67"/>
+      <c r="D24" s="68"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
-      <c r="C25" s="68"/>
-      <c r="D25" s="69"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="70"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
-      <c r="C26" s="68"/>
-      <c r="D26" s="69"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="70"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
-      <c r="C27" s="68"/>
-      <c r="D27" s="69"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="70"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
-      <c r="C28" s="70"/>
-      <c r="D28" s="71"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="72"/>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="8"/>
@@ -3623,7 +3656,7 @@
       <c r="D30" s="14"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="48" t="s">
         <v>10</v>
       </c>
       <c r="B31" s="10"/>
@@ -3679,7 +3712,7 @@
       <c r="D39" s="14"/>
     </row>
     <row r="40" ht="18" customHeight="1" spans="1:4">
-      <c r="A40" s="47" t="s">
+      <c r="A40" s="48" t="s">
         <v>11</v>
       </c>
       <c r="B40" s="10"/>
@@ -3741,7 +3774,7 @@
       <c r="D49" s="14"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="47" t="s">
+      <c r="A50" s="48" t="s">
         <v>12</v>
       </c>
       <c r="B50" s="10"/>
@@ -3797,7 +3830,7 @@
       <c r="D58" s="14"/>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="47" t="s">
+      <c r="A59" s="48" t="s">
         <v>13</v>
       </c>
       <c r="B59" s="8"/>
@@ -3853,7 +3886,7 @@
       <c r="D67" s="14"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="47" t="s">
+      <c r="A68" s="48" t="s">
         <v>14</v>
       </c>
       <c r="B68" s="8"/>
@@ -3915,7 +3948,7 @@
       <c r="D77" s="14"/>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="47" t="s">
+      <c r="A78" s="48" t="s">
         <v>15</v>
       </c>
       <c r="B78" s="8"/>
@@ -3977,7 +4010,7 @@
       <c r="D87" s="14"/>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="47" t="s">
+      <c r="A88" s="48" t="s">
         <v>16</v>
       </c>
       <c r="B88" s="8"/>
@@ -4033,7 +4066,7 @@
       <c r="D96" s="14"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="47" t="s">
+      <c r="A97" s="48" t="s">
         <v>17</v>
       </c>
       <c r="B97" s="10"/>
@@ -4089,7 +4122,7 @@
       <c r="D105" s="14"/>
     </row>
     <row r="106" spans="1:4">
-      <c r="A106" s="47" t="s">
+      <c r="A106" s="48" t="s">
         <v>18</v>
       </c>
       <c r="B106" s="8"/>
@@ -4202,7 +4235,7 @@
       <c r="D1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="30" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4210,31 +4243,31 @@
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="30">
+      <c r="B2" s="31">
         <v>45976</v>
       </c>
-      <c r="C2" s="31">
+      <c r="C2" s="32">
         <v>45983</v>
       </c>
       <c r="D2" s="8">
         <v>4</v>
       </c>
-      <c r="E2" s="32"/>
+      <c r="E2" s="33"/>
     </row>
     <row r="3" ht="115.2" spans="1:5">
       <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="31">
         <v>45976</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="32">
         <v>45983</v>
       </c>
       <c r="D3" s="8">
         <v>4</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="34" t="s">
         <v>26</v>
       </c>
     </row>
@@ -4242,16 +4275,16 @@
       <c r="A4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="31">
         <v>45976</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="32">
         <v>45983</v>
       </c>
       <c r="D4" s="8">
         <v>3</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="35" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4259,125 +4292,125 @@
       <c r="A5" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="31">
         <v>45976</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="32">
         <v>45983</v>
       </c>
       <c r="D5" s="8">
         <v>2</v>
       </c>
-      <c r="E5" s="35"/>
+      <c r="E5" s="36"/>
     </row>
     <row r="6" ht="115.2" spans="1:5">
       <c r="A6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="31">
         <v>45976</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="32">
         <v>45983</v>
       </c>
       <c r="D6" s="8">
         <v>2</v>
       </c>
-      <c r="E6" s="35"/>
+      <c r="E6" s="36"/>
     </row>
     <row r="7" ht="129.6" spans="1:5">
       <c r="A7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="30">
+      <c r="B7" s="31">
         <v>45976</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="32">
         <v>45983</v>
       </c>
       <c r="D7" s="8">
         <v>2</v>
       </c>
-      <c r="E7" s="35"/>
-    </row>
-    <row r="8" s="28" customFormat="1" ht="144" spans="1:5">
-      <c r="A8" s="36" t="s">
+      <c r="E7" s="36"/>
+    </row>
+    <row r="8" s="29" customFormat="1" ht="144" spans="1:5">
+      <c r="A8" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="31">
+      <c r="B8" s="32">
         <v>45976</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="32">
         <v>45983</v>
       </c>
-      <c r="D8" s="37">
+      <c r="D8" s="38">
         <v>2</v>
       </c>
-      <c r="E8" s="38"/>
-    </row>
-    <row r="9" s="28" customFormat="1" ht="158.4" spans="1:5">
-      <c r="A9" s="36" t="s">
+      <c r="E8" s="39"/>
+    </row>
+    <row r="9" s="29" customFormat="1" ht="158.4" spans="1:5">
+      <c r="A9" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="31">
+      <c r="B9" s="32">
         <v>45976</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="32">
         <v>45983</v>
       </c>
-      <c r="D9" s="37">
+      <c r="D9" s="38">
         <v>1</v>
       </c>
-      <c r="E9" s="39"/>
-    </row>
-    <row r="10" s="28" customFormat="1" spans="1:5">
-      <c r="A10" s="37" t="s">
+      <c r="E9" s="40"/>
+    </row>
+    <row r="10" s="29" customFormat="1" spans="1:5">
+      <c r="A10" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="31">
+      <c r="B10" s="32">
         <v>45976</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="32">
         <v>45983</v>
       </c>
-      <c r="D10" s="37">
+      <c r="D10" s="38">
         <v>1</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" s="28" customFormat="1" spans="1:5">
-      <c r="A11" s="37" t="s">
+    <row r="11" s="29" customFormat="1" spans="1:5">
+      <c r="A11" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="31">
+      <c r="B11" s="32">
         <v>45976</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="32">
         <v>45983</v>
       </c>
-      <c r="D11" s="37">
+      <c r="D11" s="38">
         <v>1</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" s="28" customFormat="1" spans="1:5">
-      <c r="A12" s="37" t="s">
+    <row r="12" s="29" customFormat="1" spans="1:5">
+      <c r="A12" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="31">
+      <c r="B12" s="32">
         <v>45976</v>
       </c>
-      <c r="C12" s="31">
+      <c r="C12" s="32">
         <v>45983</v>
       </c>
-      <c r="D12" s="37">
+      <c r="D12" s="38">
         <v>1</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4385,14 +4418,14 @@
       <c r="A13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="31">
+      <c r="B13" s="32">
         <v>45977</v>
       </c>
-      <c r="C13" s="31">
+      <c r="C13" s="32">
         <v>45982</v>
       </c>
       <c r="D13" s="8"/>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4400,16 +4433,16 @@
       <c r="A14" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="31">
+      <c r="B14" s="32">
         <v>45980</v>
       </c>
-      <c r="C14" s="31">
+      <c r="C14" s="32">
         <v>45982</v>
       </c>
       <c r="D14" s="8">
         <v>1</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4417,16 +4450,16 @@
       <c r="A15" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="31">
+      <c r="B15" s="32">
         <v>45980</v>
       </c>
-      <c r="C15" s="31">
+      <c r="C15" s="32">
         <v>45982</v>
       </c>
       <c r="D15" s="8">
         <v>1</v>
       </c>
-      <c r="E15" s="40" t="s">
+      <c r="E15" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4434,16 +4467,16 @@
       <c r="A16" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="31">
+      <c r="B16" s="32">
         <v>45980</v>
       </c>
-      <c r="C16" s="31">
+      <c r="C16" s="32">
         <v>45982</v>
       </c>
       <c r="D16" s="8">
         <v>1</v>
       </c>
-      <c r="E16" s="40" t="s">
+      <c r="E16" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4451,14 +4484,14 @@
       <c r="A17" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="31">
+      <c r="B17" s="32">
         <v>45980</v>
       </c>
-      <c r="C17" s="31">
+      <c r="C17" s="32">
         <v>45982</v>
       </c>
       <c r="D17" s="8"/>
-      <c r="E17" s="40" t="s">
+      <c r="E17" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4466,75 +4499,75 @@
       <c r="A18" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="31">
+      <c r="B18" s="32">
         <v>45981</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="41"/>
+      <c r="E18" s="42"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="41"/>
+      <c r="E19" s="42"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="41"/>
+      <c r="E20" s="42"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="41"/>
+      <c r="E21" s="42"/>
     </row>
     <row r="22" ht="14" customHeight="1" spans="1:5">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="41"/>
+      <c r="E22" s="42"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="41"/>
+      <c r="E23" s="42"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
-      <c r="E24" s="41"/>
+      <c r="E24" s="42"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="41"/>
+      <c r="E25" s="42"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="41"/>
+      <c r="E26" s="42"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="41"/>
+      <c r="E27" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4568,7 +4601,7 @@
       <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="23">
+      <c r="A2" s="24">
         <v>45962</v>
       </c>
       <c r="B2" s="14"/>
@@ -4577,7 +4610,7 @@
       <c r="A3" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="25" t="s">
         <v>46</v>
       </c>
     </row>
@@ -4585,7 +4618,7 @@
       <c r="A4" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="25" t="s">
         <v>48</v>
       </c>
     </row>
@@ -4593,21 +4626,21 @@
       <c r="A5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="25" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="25">
+      <c r="A6" s="26">
         <v>45969</v>
       </c>
       <c r="B6" s="14"/>
     </row>
-    <row r="7" s="22" customFormat="1" ht="57.6" spans="1:2">
-      <c r="A7" s="26" t="s">
+    <row r="7" s="23" customFormat="1" ht="57.6" spans="1:2">
+      <c r="A7" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="28" t="s">
         <v>52</v>
       </c>
     </row>
@@ -4623,7 +4656,7 @@
   <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -4917,7 +4950,7 @@
       </c>
       <c r="C27" s="14"/>
     </row>
-    <row r="28" ht="100.8" spans="1:3">
+    <row r="28" ht="409.5" spans="1:4">
       <c r="A28" s="8" t="s">
         <v>120</v>
       </c>
@@ -4927,16 +4960,19 @@
       <c r="C28" s="15" t="s">
         <v>122</v>
       </c>
+      <c r="D28" s="20" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="29" ht="244.8" spans="1:3">
       <c r="A29" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="C29" s="20" t="s">
         <v>125</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -5055,8 +5091,8 @@
       <c r="C52" s="14"/>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="21"/>
-      <c r="B53" s="21"/>
+      <c r="A53" s="22"/>
+      <c r="B53" s="22"/>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="8"/>
@@ -5268,7 +5304,7 @@
         <v>38</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -5278,12 +5314,12 @@
     </row>
     <row r="19" ht="72" spans="1:1">
       <c r="A19" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" ht="72" spans="1:1">
       <c r="A20" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -5305,17 +5341,17 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -5356,7 +5392,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5371,7 +5407,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
@@ -5613,7 +5649,7 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -5799,7 +5835,7 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -15396,10 +15432,10 @@
   <sheetData>
     <row r="1" ht="409" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:1">

</xml_diff>

<commit_message>
28-11-25  Updated with prefix sum + HashMap
</commit_message>
<xml_diff>
--- a/JavaPrograms/Work Done.xlsx
+++ b/JavaPrograms/Work Done.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="160">
   <si>
     <r>
       <rPr>
@@ -1409,6 +1409,800 @@
 So when you code, you should already know 2 is coming.</t>
   </si>
   <si>
+    <t>Prefix Sum</t>
+  </si>
+  <si>
+    <t>Imagine you're walking on tiles where each tile has a number.
+Step Tile Value Total sum so far
+Step1 +2 2
+Step2 +5 7
+Step3 -3 4
+Step4 +1 5
+This running sum is the prefix sum.
+If at step 2 sum=7 and at step 4 sum=5,
+then between step(2→4) we lost 2.
+Because → 5 - 7 = -2
+So any subarray sum can be obtained by:
+prefix[j] - prefix[i] = subarray sum(i+1 to j)
+🔥 That’s the entire prefix concept.</t>
+  </si>
+  <si>
+    <t>HashMap</t>
+  </si>
+  <si>
+    <r>
+      <t>What EVEN is a HashMap?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Imagine a drawer cabinet.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>You place something in drawer 5 → you can get it back instantly by opening drawer 5.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>You don’t search all drawers like in a list.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>You know exactly where to look.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>In Java terms:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Drawer No. Inside item</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Key Value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>So:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Map&lt;Integer,Integer&gt; map = new HashMap&lt;&gt;();</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>map.put(5, 10); // keep item 10 in drawer key 5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>map.get(5);</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>// instantly retrieves 10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>You don't search — you access in O(1) time.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>HashMap does two things for us:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>✔ Stores Key -&gt; Value pairs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>✔ Retrieves value instantly if key exists</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Think:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>“I’ve seen this number before — how many times?”</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prefix</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1) What is prefix[i] actually storing?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Correct version:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>prefix[i] stores the sum of all elements from arr[0] to arr[i].</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Example:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>i=2 → prefix[2] = arr[0] + arr[1] + arr[2]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2) Why does prefix[3] - prefix[0] give sum of arr[1..3]?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Your reasoning was half correct, but here is the clean logic:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>prefix[3] = arr[0] + arr[1] + arr[2] + arr[3]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>prefix[0] = arr[0]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Subtracting removes arr[0]:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>prefix[3] - prefix[0] = (arr[0]+arr[1]+arr[2]+arr[3]) - arr[0]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">                     </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>= arr[1]+arr[2]+arr[3]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>This is why we use prefix for subarray sum.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3) Difference between arr[] and prefix[]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>arr[] prefix[]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>original values running total of array</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>arr[i] = just one number prefix[i] = sum from index 0 → i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>no computation used to compute range sums fast</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Perfect one-liner:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>arr = raw data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>prefix = cumulative sum of that data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>You got it.</t>
+    </r>
+  </si>
+  <si>
     <t>3 Merge Sort Problems (Simple → Medium)
 Problem 1 — Sort an array using merge sort
 (You already did this, but repeat until you can write it without peeking.)
@@ -1910,7 +2704,7 @@
     <numFmt numFmtId="180" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="181" formatCode="dd/mmm/yy"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1940,6 +2734,12 @@
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2321,7 +3121,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -2341,6 +3141,21 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2561,16 +3376,13 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2579,119 +3391,122 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2752,10 +3567,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2767,16 +3588,16 @@
     <xf numFmtId="180" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2785,16 +3606,16 @@
     <xf numFmtId="181" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2803,10 +3624,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2830,11 +3651,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2848,11 +3666,11 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2866,11 +3684,11 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2884,11 +3702,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2900,6 +3718,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3452,246 +4273,246 @@
   </cols>
   <sheetData>
     <row r="1" ht="90" customHeight="1" spans="1:6">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="42" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="44" t="s">
+      <c r="D1" s="45"/>
+      <c r="E1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="44"/>
+      <c r="F1" s="46"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="47" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="8"/>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="47" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="10"/>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="53"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
     </row>
     <row r="15" ht="15" customHeight="1" spans="1:6">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
-      <c r="C16" s="58" t="s">
+      <c r="C16" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="59"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="47" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="8"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="61"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="44"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="61"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="63"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="63"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="65"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
-      <c r="C24" s="64" t="s">
+      <c r="C24" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="65"/>
+      <c r="D24" s="67"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
-      <c r="C25" s="66"/>
-      <c r="D25" s="67"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="69"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
-      <c r="C26" s="66"/>
-      <c r="D26" s="67"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="69"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
-      <c r="C27" s="66"/>
-      <c r="D27" s="67"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="69"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
-      <c r="C28" s="68"/>
-      <c r="D28" s="69"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="71"/>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="8"/>
@@ -3706,7 +4527,7 @@
       <c r="D30" s="14"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="47" t="s">
         <v>10</v>
       </c>
       <c r="B31" s="10"/>
@@ -3762,7 +4583,7 @@
       <c r="D39" s="14"/>
     </row>
     <row r="40" ht="18" customHeight="1" spans="1:4">
-      <c r="A40" s="45" t="s">
+      <c r="A40" s="47" t="s">
         <v>11</v>
       </c>
       <c r="B40" s="10"/>
@@ -3824,7 +4645,7 @@
       <c r="D49" s="14"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="45" t="s">
+      <c r="A50" s="47" t="s">
         <v>12</v>
       </c>
       <c r="B50" s="10"/>
@@ -3880,7 +4701,7 @@
       <c r="D58" s="14"/>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="45" t="s">
+      <c r="A59" s="47" t="s">
         <v>13</v>
       </c>
       <c r="B59" s="8"/>
@@ -3936,7 +4757,7 @@
       <c r="D67" s="14"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="45" t="s">
+      <c r="A68" s="47" t="s">
         <v>14</v>
       </c>
       <c r="B68" s="8"/>
@@ -3998,7 +4819,7 @@
       <c r="D77" s="14"/>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="45" t="s">
+      <c r="A78" s="47" t="s">
         <v>15</v>
       </c>
       <c r="B78" s="8"/>
@@ -4060,7 +4881,7 @@
       <c r="D87" s="14"/>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="45" t="s">
+      <c r="A88" s="47" t="s">
         <v>16</v>
       </c>
       <c r="B88" s="8"/>
@@ -4116,7 +4937,7 @@
       <c r="D96" s="14"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="45" t="s">
+      <c r="A97" s="47" t="s">
         <v>17</v>
       </c>
       <c r="B97" s="10"/>
@@ -4172,7 +4993,7 @@
       <c r="D105" s="14"/>
     </row>
     <row r="106" spans="1:4">
-      <c r="A106" s="45" t="s">
+      <c r="A106" s="47" t="s">
         <v>18</v>
       </c>
       <c r="B106" s="8"/>
@@ -4285,7 +5106,7 @@
       <c r="D1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="30" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4293,31 +5114,31 @@
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="29">
+      <c r="B2" s="31">
         <v>45976</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="32">
         <v>45983</v>
       </c>
       <c r="D2" s="8">
         <v>4</v>
       </c>
-      <c r="E2" s="31"/>
+      <c r="E2" s="33"/>
     </row>
     <row r="3" ht="115.2" spans="1:5">
       <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="31">
         <v>45976</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="32">
         <v>45983</v>
       </c>
       <c r="D3" s="8">
         <v>4</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="34" t="s">
         <v>26</v>
       </c>
     </row>
@@ -4325,16 +5146,16 @@
       <c r="A4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4" s="31">
         <v>45976</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="32">
         <v>45983</v>
       </c>
       <c r="D4" s="8">
         <v>3</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="35" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4342,125 +5163,125 @@
       <c r="A5" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="31">
         <v>45976</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="32">
         <v>45983</v>
       </c>
       <c r="D5" s="8">
         <v>2</v>
       </c>
-      <c r="E5" s="34"/>
+      <c r="E5" s="36"/>
     </row>
     <row r="6" ht="115.2" spans="1:5">
       <c r="A6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="31">
         <v>45976</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="32">
         <v>45983</v>
       </c>
       <c r="D6" s="8">
         <v>2</v>
       </c>
-      <c r="E6" s="34"/>
+      <c r="E6" s="36"/>
     </row>
     <row r="7" ht="129.6" spans="1:5">
       <c r="A7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="31">
         <v>45976</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="32">
         <v>45983</v>
       </c>
       <c r="D7" s="8">
         <v>2</v>
       </c>
-      <c r="E7" s="34"/>
-    </row>
-    <row r="8" s="27" customFormat="1" ht="144" spans="1:5">
-      <c r="A8" s="35" t="s">
+      <c r="E7" s="36"/>
+    </row>
+    <row r="8" s="29" customFormat="1" ht="144" spans="1:5">
+      <c r="A8" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="30">
+      <c r="B8" s="32">
         <v>45976</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="32">
         <v>45983</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8" s="38">
         <v>2</v>
       </c>
-      <c r="E8" s="37"/>
-    </row>
-    <row r="9" s="27" customFormat="1" ht="158.4" spans="1:5">
-      <c r="A9" s="35" t="s">
+      <c r="E8" s="39"/>
+    </row>
+    <row r="9" s="29" customFormat="1" ht="158.4" spans="1:5">
+      <c r="A9" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B9" s="32">
         <v>45976</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="32">
         <v>45983</v>
       </c>
-      <c r="D9" s="36">
+      <c r="D9" s="38">
         <v>1</v>
       </c>
-      <c r="E9" s="38"/>
-    </row>
-    <row r="10" s="27" customFormat="1" spans="1:5">
-      <c r="A10" s="36" t="s">
+      <c r="E9" s="40"/>
+    </row>
+    <row r="10" s="29" customFormat="1" spans="1:5">
+      <c r="A10" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="30">
+      <c r="B10" s="32">
         <v>45976</v>
       </c>
-      <c r="C10" s="30">
+      <c r="C10" s="32">
         <v>45983</v>
       </c>
-      <c r="D10" s="36">
+      <c r="D10" s="38">
         <v>1</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" s="27" customFormat="1" spans="1:5">
-      <c r="A11" s="36" t="s">
+    <row r="11" s="29" customFormat="1" spans="1:5">
+      <c r="A11" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="30">
+      <c r="B11" s="32">
         <v>45976</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C11" s="32">
         <v>45983</v>
       </c>
-      <c r="D11" s="36">
+      <c r="D11" s="38">
         <v>1</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" s="27" customFormat="1" spans="1:5">
-      <c r="A12" s="36" t="s">
+    <row r="12" s="29" customFormat="1" spans="1:5">
+      <c r="A12" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="30">
+      <c r="B12" s="32">
         <v>45976</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="32">
         <v>45983</v>
       </c>
-      <c r="D12" s="36">
+      <c r="D12" s="38">
         <v>1</v>
       </c>
-      <c r="E12" s="39" t="s">
+      <c r="E12" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4468,16 +5289,16 @@
       <c r="A13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="30">
+      <c r="B13" s="32">
         <v>45977</v>
       </c>
-      <c r="C13" s="30">
+      <c r="C13" s="32">
         <v>45982</v>
       </c>
       <c r="D13" s="8">
         <v>1</v>
       </c>
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4485,16 +5306,16 @@
       <c r="A14" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="30">
+      <c r="B14" s="32">
         <v>45980</v>
       </c>
-      <c r="C14" s="30">
+      <c r="C14" s="32">
         <v>45982</v>
       </c>
       <c r="D14" s="8">
         <v>1</v>
       </c>
-      <c r="E14" s="39" t="s">
+      <c r="E14" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4502,16 +5323,16 @@
       <c r="A15" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="30">
+      <c r="B15" s="32">
         <v>45980</v>
       </c>
-      <c r="C15" s="30">
+      <c r="C15" s="32">
         <v>45982</v>
       </c>
       <c r="D15" s="8">
         <v>1</v>
       </c>
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4519,16 +5340,16 @@
       <c r="A16" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="30">
+      <c r="B16" s="32">
         <v>45980</v>
       </c>
-      <c r="C16" s="30">
+      <c r="C16" s="32">
         <v>45982</v>
       </c>
       <c r="D16" s="8">
         <v>1</v>
       </c>
-      <c r="E16" s="39" t="s">
+      <c r="E16" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4536,16 +5357,16 @@
       <c r="A17" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="30">
+      <c r="B17" s="32">
         <v>45980</v>
       </c>
-      <c r="C17" s="30">
+      <c r="C17" s="32">
         <v>45982</v>
       </c>
       <c r="D17" s="8">
         <v>1</v>
       </c>
-      <c r="E17" s="39" t="s">
+      <c r="E17" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4553,16 +5374,16 @@
       <c r="A18" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="30">
+      <c r="B18" s="32">
         <v>45981</v>
       </c>
-      <c r="C18" s="30">
+      <c r="C18" s="32">
         <v>45983</v>
       </c>
       <c r="D18" s="8">
         <v>1</v>
       </c>
-      <c r="E18" s="39" t="s">
+      <c r="E18" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4570,16 +5391,16 @@
       <c r="A19" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="30">
+      <c r="B19" s="32">
         <v>45982</v>
       </c>
-      <c r="C19" s="30">
+      <c r="C19" s="32">
         <v>45984</v>
       </c>
       <c r="D19" s="8">
         <v>1</v>
       </c>
-      <c r="E19" s="39" t="s">
+      <c r="E19" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4587,16 +5408,16 @@
       <c r="A20" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="30">
+      <c r="B20" s="32">
         <v>45983</v>
       </c>
-      <c r="C20" s="30">
+      <c r="C20" s="32">
         <v>45985</v>
       </c>
       <c r="D20" s="8">
         <v>1</v>
       </c>
-      <c r="E20" s="39" t="s">
+      <c r="E20" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4604,16 +5425,16 @@
       <c r="A21" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="30">
+      <c r="B21" s="32">
         <v>45986</v>
       </c>
-      <c r="C21" s="30">
+      <c r="C21" s="32">
         <v>45987</v>
       </c>
       <c r="D21" s="8">
         <v>1</v>
       </c>
-      <c r="E21" s="39" t="s">
+      <c r="E21" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4621,16 +5442,16 @@
       <c r="A22" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="30">
+      <c r="B22" s="32">
         <v>45986</v>
       </c>
-      <c r="C22" s="30">
+      <c r="C22" s="32">
         <v>45987</v>
       </c>
       <c r="D22" s="8">
         <v>1</v>
       </c>
-      <c r="E22" s="39" t="s">
+      <c r="E22" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4638,16 +5459,16 @@
       <c r="A23" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="30">
+      <c r="B23" s="32">
         <v>45986</v>
       </c>
-      <c r="C23" s="30">
+      <c r="C23" s="32">
         <v>45987</v>
       </c>
       <c r="D23" s="8">
         <v>1</v>
       </c>
-      <c r="E23" s="39" t="s">
+      <c r="E23" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4655,16 +5476,16 @@
       <c r="A24" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="30">
+      <c r="B24" s="32">
         <v>45986</v>
       </c>
-      <c r="C24" s="30">
+      <c r="C24" s="32">
         <v>45987</v>
       </c>
       <c r="D24" s="8">
         <v>1</v>
       </c>
-      <c r="E24" s="39" t="s">
+      <c r="E24" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4672,16 +5493,16 @@
       <c r="A25" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="30">
+      <c r="B25" s="32">
         <v>45986</v>
       </c>
-      <c r="C25" s="30">
+      <c r="C25" s="32">
         <v>45987</v>
       </c>
       <c r="D25" s="8">
         <v>1</v>
       </c>
-      <c r="E25" s="39" t="s">
+      <c r="E25" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4689,16 +5510,16 @@
       <c r="A26" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="30">
+      <c r="B26" s="32">
         <v>45986</v>
       </c>
-      <c r="C26" s="30">
+      <c r="C26" s="32">
         <v>45987</v>
       </c>
       <c r="D26" s="8">
         <v>1</v>
       </c>
-      <c r="E26" s="39" t="s">
+      <c r="E26" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4706,16 +5527,16 @@
       <c r="A27" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="30">
+      <c r="B27" s="32">
         <v>45986</v>
       </c>
-      <c r="C27" s="30">
+      <c r="C27" s="32">
         <v>45987</v>
       </c>
       <c r="D27" s="8">
         <v>1</v>
       </c>
-      <c r="E27" s="39" t="s">
+      <c r="E27" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4723,16 +5544,16 @@
       <c r="A28" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="30">
+      <c r="B28" s="32">
         <v>45986</v>
       </c>
-      <c r="C28" s="30">
+      <c r="C28" s="32">
         <v>45987</v>
       </c>
       <c r="D28" s="8">
         <v>1</v>
       </c>
-      <c r="E28" s="39" t="s">
+      <c r="E28" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4740,16 +5561,16 @@
       <c r="A29" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="30">
+      <c r="B29" s="32">
         <v>45986</v>
       </c>
-      <c r="C29" s="30">
+      <c r="C29" s="32">
         <v>45987</v>
       </c>
       <c r="D29" s="8">
         <v>1</v>
       </c>
-      <c r="E29" s="39" t="s">
+      <c r="E29" s="41" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4757,22 +5578,22 @@
       <c r="A30" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="30">
+      <c r="B30" s="32">
         <v>45986</v>
       </c>
-      <c r="C30" s="30">
+      <c r="C30" s="32">
         <v>45987</v>
       </c>
       <c r="D30" s="8">
         <v>1</v>
       </c>
-      <c r="E30" s="39" t="s">
+      <c r="E30" s="41" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="8"/>
-      <c r="B31" s="30"/>
+      <c r="B31" s="32"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
@@ -5418,7 +6239,7 @@
       <c r="B1" s="14"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="22">
+      <c r="A2" s="24">
         <v>45962</v>
       </c>
       <c r="B2" s="14"/>
@@ -5427,7 +6248,7 @@
       <c r="A3" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="25" t="s">
         <v>58</v>
       </c>
     </row>
@@ -5435,7 +6256,7 @@
       <c r="A4" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="25" t="s">
         <v>60</v>
       </c>
     </row>
@@ -5443,21 +6264,21 @@
       <c r="A5" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="25" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="24">
+      <c r="A6" s="26">
         <v>45969</v>
       </c>
       <c r="B6" s="14"/>
     </row>
-    <row r="7" s="21" customFormat="1" ht="57.6" spans="1:2">
-      <c r="A7" s="25" t="s">
+    <row r="7" s="23" customFormat="1" ht="57.6" spans="1:2">
+      <c r="A7" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="28" t="s">
         <v>64</v>
       </c>
     </row>
@@ -5472,8 +6293,8 @@
   <sheetPr/>
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -5801,19 +6622,31 @@
       </c>
       <c r="C30" s="14"/>
     </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
+    <row r="31" ht="187.2" spans="1:3">
+      <c r="A31" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>143</v>
+      </c>
       <c r="C31" s="14"/>
     </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
+    <row r="32" ht="259.2" spans="1:3">
+      <c r="A32" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>145</v>
+      </c>
       <c r="C32" s="14"/>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
+    <row r="33" ht="345.6" spans="1:3">
+      <c r="A33" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>147</v>
+      </c>
       <c r="C33" s="14"/>
     </row>
     <row r="34" spans="1:3">
@@ -5912,8 +6745,8 @@
       <c r="C52" s="14"/>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="20"/>
-      <c r="B53" s="20"/>
+      <c r="A53" s="22"/>
+      <c r="B53" s="22"/>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="8"/>
@@ -6125,7 +6958,7 @@
         <v>38</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -6135,12 +6968,12 @@
     </row>
     <row r="19" ht="72" spans="1:1">
       <c r="A19" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" ht="72" spans="1:1">
       <c r="A20" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -6162,17 +6995,17 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -6213,7 +7046,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="3" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6228,7 +7061,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="5" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
@@ -6470,7 +7303,7 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="3" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -6656,7 +7489,7 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="4" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -16253,10 +17086,10 @@
   <sheetData>
     <row r="1" ht="409" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:1">

</xml_diff>

<commit_message>
30-11-25  Binary Search on Answer Updated
</commit_message>
<xml_diff>
--- a/JavaPrograms/Work Done.xlsx
+++ b/JavaPrograms/Work Done.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="169">
   <si>
     <r>
       <rPr>
@@ -2281,6 +2281,16 @@
 Pattern 3 — Find in Rotated Sorted Array</t>
   </si>
   <si>
+    <t>Binary Search on Answer</t>
+  </si>
+  <si>
+    <t>Idea is simple:
+We don’t search in the array.
+We search for the answer itself.
+We guess an answer → check if it’s possible → adjust high/low.
+Treat it like "hot–warm–cold".</t>
+  </si>
+  <si>
     <t>3 Merge Sort Problems (Simple → Medium)
 Problem 1 — Sort an array using merge sort
 (You already did this, but repeat until you can write it without peeking.)
@@ -5179,10 +5189,10 @@
   <sheetData>
     <row r="1" ht="409" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -6830,7 +6840,7 @@
   <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -7194,9 +7204,13 @@
       </c>
       <c r="C34" s="14"/>
     </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
+    <row r="35" ht="72" spans="1:3">
+      <c r="A35" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>156</v>
+      </c>
       <c r="C35" s="14"/>
     </row>
     <row r="36" spans="1:3">
@@ -7498,7 +7512,7 @@
         <v>38</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -7508,12 +7522,12 @@
     </row>
     <row r="19" ht="72" spans="1:1">
       <c r="A19" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" ht="72" spans="1:1">
       <c r="A20" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -7535,17 +7549,17 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -7586,7 +7600,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="3" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -7601,7 +7615,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="5" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
@@ -7843,7 +7857,7 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -8029,7 +8043,7 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="4" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>

</xml_diff>

<commit_message>
30-11-25  Python Functions def
</commit_message>
<xml_diff>
--- a/JavaPrograms/Work Done.xlsx
+++ b/JavaPrograms/Work Done.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8280" activeTab="4"/>
+    <workbookView windowWidth="23040" windowHeight="8280" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DSA plan" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="171">
   <si>
     <r>
       <rPr>
@@ -721,6 +721,13 @@
 # "Give me the NAME for every emp in employees if DEPT is Tech"
 tech_names = [emp["name"] for emp in employees if emp["dept"] == "Tech"]
 # Result: ['Neha', 'Raj']</t>
+  </si>
+  <si>
+    <t>Functions (def)</t>
+  </si>
+  <si>
+    <t>Imagine you are a Wizard in Harry Potter.
+1. Defining (def) is WRITING the spell. You are writing a new spell in your spellbook. You give it a name, and you decide what it does.             2. Calling is CASTING the spell. This is when you actually wave your wand and say the name.</t>
   </si>
   <si>
     <t>Recall</t>
@@ -3594,7 +3601,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3690,6 +3697,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
@@ -4370,246 +4380,246 @@
   </cols>
   <sheetData>
     <row r="1" ht="90" customHeight="1" spans="1:6">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="47" t="s">
+      <c r="B1" s="47"/>
+      <c r="C1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="48"/>
-      <c r="E1" s="49" t="s">
+      <c r="D1" s="49"/>
+      <c r="E1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="49"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="51" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="8"/>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="51" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="10"/>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="58"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
     </row>
     <row r="15" ht="15" customHeight="1" spans="1:6">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
-      <c r="C16" s="63" t="s">
+      <c r="C16" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="64"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="66"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="65"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="51" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="8"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
+      <c r="C20" s="66"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
+      <c r="C21" s="66"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="66"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="67"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
-      <c r="C23" s="67"/>
-      <c r="D23" s="68"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="69"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
-      <c r="C24" s="69" t="s">
+      <c r="C24" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="70"/>
+      <c r="D24" s="71"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
-      <c r="C25" s="71"/>
-      <c r="D25" s="72"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="73"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
-      <c r="C26" s="71"/>
-      <c r="D26" s="72"/>
+      <c r="C26" s="72"/>
+      <c r="D26" s="73"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
-      <c r="C27" s="71"/>
-      <c r="D27" s="72"/>
+      <c r="C27" s="72"/>
+      <c r="D27" s="73"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
-      <c r="C28" s="73"/>
-      <c r="D28" s="74"/>
+      <c r="C28" s="74"/>
+      <c r="D28" s="75"/>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="8"/>
@@ -4624,7 +4634,7 @@
       <c r="D30" s="14"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="50" t="s">
+      <c r="A31" s="51" t="s">
         <v>10</v>
       </c>
       <c r="B31" s="10"/>
@@ -4680,7 +4690,7 @@
       <c r="D39" s="14"/>
     </row>
     <row r="40" ht="18" customHeight="1" spans="1:4">
-      <c r="A40" s="50" t="s">
+      <c r="A40" s="51" t="s">
         <v>11</v>
       </c>
       <c r="B40" s="10"/>
@@ -4742,7 +4752,7 @@
       <c r="D49" s="14"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="50" t="s">
+      <c r="A50" s="51" t="s">
         <v>12</v>
       </c>
       <c r="B50" s="10"/>
@@ -4798,7 +4808,7 @@
       <c r="D58" s="14"/>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="50" t="s">
+      <c r="A59" s="51" t="s">
         <v>13</v>
       </c>
       <c r="B59" s="8"/>
@@ -4854,7 +4864,7 @@
       <c r="D67" s="14"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="50" t="s">
+      <c r="A68" s="51" t="s">
         <v>14</v>
       </c>
       <c r="B68" s="8"/>
@@ -4916,7 +4926,7 @@
       <c r="D77" s="14"/>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="50" t="s">
+      <c r="A78" s="51" t="s">
         <v>15</v>
       </c>
       <c r="B78" s="8"/>
@@ -4978,7 +4988,7 @@
       <c r="D87" s="14"/>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="50" t="s">
+      <c r="A88" s="51" t="s">
         <v>16</v>
       </c>
       <c r="B88" s="8"/>
@@ -5034,7 +5044,7 @@
       <c r="D96" s="14"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="50" t="s">
+      <c r="A97" s="51" t="s">
         <v>17</v>
       </c>
       <c r="B97" s="10"/>
@@ -5090,7 +5100,7 @@
       <c r="D105" s="14"/>
     </row>
     <row r="106" spans="1:4">
-      <c r="A106" s="50" t="s">
+      <c r="A106" s="51" t="s">
         <v>18</v>
       </c>
       <c r="B106" s="8"/>
@@ -5189,10 +5199,10 @@
   <sheetData>
     <row r="1" ht="409" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -5348,7 +5358,7 @@
       <c r="D1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="34" t="s">
         <v>23</v>
       </c>
     </row>
@@ -5356,31 +5366,31 @@
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="34">
+      <c r="B2" s="35">
         <v>45976</v>
       </c>
-      <c r="C2" s="35">
+      <c r="C2" s="36">
         <v>45983</v>
       </c>
       <c r="D2" s="8">
         <v>4</v>
       </c>
-      <c r="E2" s="36"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" ht="115.2" spans="1:5">
       <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="34">
+      <c r="B3" s="35">
         <v>45976</v>
       </c>
-      <c r="C3" s="35">
+      <c r="C3" s="36">
         <v>45983</v>
       </c>
       <c r="D3" s="8">
         <v>4</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="38" t="s">
         <v>26</v>
       </c>
     </row>
@@ -5388,16 +5398,16 @@
       <c r="A4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="34">
+      <c r="B4" s="35">
         <v>45976</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="36">
         <v>45983</v>
       </c>
       <c r="D4" s="8">
         <v>3</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="39" t="s">
         <v>28</v>
       </c>
     </row>
@@ -5405,125 +5415,125 @@
       <c r="A5" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="34">
+      <c r="B5" s="35">
         <v>45976</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="36">
         <v>45983</v>
       </c>
       <c r="D5" s="8">
         <v>2</v>
       </c>
-      <c r="E5" s="39"/>
+      <c r="E5" s="40"/>
     </row>
     <row r="6" ht="115.2" spans="1:5">
       <c r="A6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="34">
+      <c r="B6" s="35">
         <v>45976</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="36">
         <v>45983</v>
       </c>
       <c r="D6" s="8">
         <v>2</v>
       </c>
-      <c r="E6" s="39"/>
+      <c r="E6" s="40"/>
     </row>
     <row r="7" ht="129.6" spans="1:5">
       <c r="A7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="34">
+      <c r="B7" s="35">
         <v>45976</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="36">
         <v>45983</v>
       </c>
       <c r="D7" s="8">
         <v>2</v>
       </c>
-      <c r="E7" s="39"/>
-    </row>
-    <row r="8" s="32" customFormat="1" ht="144" spans="1:5">
-      <c r="A8" s="40" t="s">
+      <c r="E7" s="40"/>
+    </row>
+    <row r="8" s="33" customFormat="1" ht="144" spans="1:5">
+      <c r="A8" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="35">
+      <c r="B8" s="36">
         <v>45976</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="36">
         <v>45983</v>
       </c>
-      <c r="D8" s="41">
+      <c r="D8" s="42">
         <v>2</v>
       </c>
-      <c r="E8" s="42"/>
-    </row>
-    <row r="9" s="32" customFormat="1" ht="158.4" spans="1:5">
-      <c r="A9" s="40" t="s">
+      <c r="E8" s="43"/>
+    </row>
+    <row r="9" s="33" customFormat="1" ht="158.4" spans="1:5">
+      <c r="A9" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="35">
+      <c r="B9" s="36">
         <v>45976</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="36">
         <v>45983</v>
       </c>
-      <c r="D9" s="41">
+      <c r="D9" s="42">
         <v>1</v>
       </c>
-      <c r="E9" s="43"/>
-    </row>
-    <row r="10" s="32" customFormat="1" spans="1:5">
-      <c r="A10" s="41" t="s">
+      <c r="E9" s="44"/>
+    </row>
+    <row r="10" s="33" customFormat="1" spans="1:5">
+      <c r="A10" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="35">
+      <c r="B10" s="36">
         <v>45976</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="36">
         <v>45983</v>
       </c>
-      <c r="D10" s="41">
+      <c r="D10" s="42">
         <v>1</v>
       </c>
-      <c r="E10" s="44" t="s">
+      <c r="E10" s="45" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" s="32" customFormat="1" spans="1:5">
-      <c r="A11" s="41" t="s">
+    <row r="11" s="33" customFormat="1" spans="1:5">
+      <c r="A11" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="35">
+      <c r="B11" s="36">
         <v>45976</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="36">
         <v>45983</v>
       </c>
-      <c r="D11" s="41">
+      <c r="D11" s="42">
         <v>1</v>
       </c>
-      <c r="E11" s="44" t="s">
+      <c r="E11" s="45" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" s="32" customFormat="1" spans="1:5">
-      <c r="A12" s="41" t="s">
+    <row r="12" s="33" customFormat="1" spans="1:5">
+      <c r="A12" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="35">
+      <c r="B12" s="36">
         <v>45976</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="36">
         <v>45983</v>
       </c>
-      <c r="D12" s="41">
+      <c r="D12" s="42">
         <v>1</v>
       </c>
-      <c r="E12" s="44" t="s">
+      <c r="E12" s="45" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5531,16 +5541,16 @@
       <c r="A13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="35">
+      <c r="B13" s="36">
         <v>45977</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C13" s="36">
         <v>45982</v>
       </c>
       <c r="D13" s="8">
         <v>1</v>
       </c>
-      <c r="E13" s="44" t="s">
+      <c r="E13" s="45" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5548,16 +5558,16 @@
       <c r="A14" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="35">
+      <c r="B14" s="36">
         <v>45980</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="36">
         <v>45982</v>
       </c>
       <c r="D14" s="8">
         <v>1</v>
       </c>
-      <c r="E14" s="44" t="s">
+      <c r="E14" s="45" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5565,16 +5575,16 @@
       <c r="A15" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="35">
+      <c r="B15" s="36">
         <v>45980</v>
       </c>
-      <c r="C15" s="35">
+      <c r="C15" s="36">
         <v>45982</v>
       </c>
       <c r="D15" s="8">
         <v>1</v>
       </c>
-      <c r="E15" s="44" t="s">
+      <c r="E15" s="45" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5582,16 +5592,16 @@
       <c r="A16" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="35">
+      <c r="B16" s="36">
         <v>45980</v>
       </c>
-      <c r="C16" s="35">
+      <c r="C16" s="36">
         <v>45982</v>
       </c>
       <c r="D16" s="8">
         <v>1</v>
       </c>
-      <c r="E16" s="44" t="s">
+      <c r="E16" s="45" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5599,16 +5609,16 @@
       <c r="A17" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="35">
+      <c r="B17" s="36">
         <v>45980</v>
       </c>
-      <c r="C17" s="35">
+      <c r="C17" s="36">
         <v>45982</v>
       </c>
       <c r="D17" s="8">
         <v>1</v>
       </c>
-      <c r="E17" s="44" t="s">
+      <c r="E17" s="45" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5616,16 +5626,16 @@
       <c r="A18" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="35">
+      <c r="B18" s="36">
         <v>45981</v>
       </c>
-      <c r="C18" s="35">
+      <c r="C18" s="36">
         <v>45983</v>
       </c>
       <c r="D18" s="8">
         <v>1</v>
       </c>
-      <c r="E18" s="44" t="s">
+      <c r="E18" s="45" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5633,16 +5643,16 @@
       <c r="A19" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="35">
+      <c r="B19" s="36">
         <v>45982</v>
       </c>
-      <c r="C19" s="35">
+      <c r="C19" s="36">
         <v>45984</v>
       </c>
       <c r="D19" s="8">
         <v>1</v>
       </c>
-      <c r="E19" s="44" t="s">
+      <c r="E19" s="45" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5650,16 +5660,16 @@
       <c r="A20" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="35">
+      <c r="B20" s="36">
         <v>45983</v>
       </c>
-      <c r="C20" s="35">
+      <c r="C20" s="36">
         <v>45985</v>
       </c>
       <c r="D20" s="8">
         <v>1</v>
       </c>
-      <c r="E20" s="44" t="s">
+      <c r="E20" s="45" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5667,16 +5677,16 @@
       <c r="A21" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="35">
+      <c r="B21" s="36">
         <v>45986</v>
       </c>
-      <c r="C21" s="35">
+      <c r="C21" s="36">
         <v>45987</v>
       </c>
       <c r="D21" s="8">
         <v>1</v>
       </c>
-      <c r="E21" s="44" t="s">
+      <c r="E21" s="45" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5684,16 +5694,16 @@
       <c r="A22" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="35">
+      <c r="B22" s="36">
         <v>45986</v>
       </c>
-      <c r="C22" s="35">
+      <c r="C22" s="36">
         <v>45987</v>
       </c>
       <c r="D22" s="8">
         <v>1</v>
       </c>
-      <c r="E22" s="44" t="s">
+      <c r="E22" s="45" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5701,16 +5711,16 @@
       <c r="A23" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="35">
+      <c r="B23" s="36">
         <v>45986</v>
       </c>
-      <c r="C23" s="35">
+      <c r="C23" s="36">
         <v>45987</v>
       </c>
       <c r="D23" s="8">
         <v>1</v>
       </c>
-      <c r="E23" s="44" t="s">
+      <c r="E23" s="45" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5718,16 +5728,16 @@
       <c r="A24" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="35">
+      <c r="B24" s="36">
         <v>45986</v>
       </c>
-      <c r="C24" s="35">
+      <c r="C24" s="36">
         <v>45987</v>
       </c>
       <c r="D24" s="8">
         <v>1</v>
       </c>
-      <c r="E24" s="44" t="s">
+      <c r="E24" s="45" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5735,16 +5745,16 @@
       <c r="A25" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="35">
+      <c r="B25" s="36">
         <v>45986</v>
       </c>
-      <c r="C25" s="35">
+      <c r="C25" s="36">
         <v>45987</v>
       </c>
       <c r="D25" s="8">
         <v>1</v>
       </c>
-      <c r="E25" s="44" t="s">
+      <c r="E25" s="45" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5752,16 +5762,16 @@
       <c r="A26" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="35">
+      <c r="B26" s="36">
         <v>45986</v>
       </c>
-      <c r="C26" s="35">
+      <c r="C26" s="36">
         <v>45987</v>
       </c>
       <c r="D26" s="8">
         <v>1</v>
       </c>
-      <c r="E26" s="44" t="s">
+      <c r="E26" s="45" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5769,16 +5779,16 @@
       <c r="A27" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="35">
+      <c r="B27" s="36">
         <v>45986</v>
       </c>
-      <c r="C27" s="35">
+      <c r="C27" s="36">
         <v>45987</v>
       </c>
       <c r="D27" s="8">
         <v>1</v>
       </c>
-      <c r="E27" s="44" t="s">
+      <c r="E27" s="45" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5786,16 +5796,16 @@
       <c r="A28" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="35">
+      <c r="B28" s="36">
         <v>45986</v>
       </c>
-      <c r="C28" s="35">
+      <c r="C28" s="36">
         <v>45987</v>
       </c>
       <c r="D28" s="8">
         <v>1</v>
       </c>
-      <c r="E28" s="44" t="s">
+      <c r="E28" s="45" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5803,16 +5813,16 @@
       <c r="A29" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="35">
+      <c r="B29" s="36">
         <v>45986</v>
       </c>
-      <c r="C29" s="35">
+      <c r="C29" s="36">
         <v>45987</v>
       </c>
       <c r="D29" s="8">
         <v>1</v>
       </c>
-      <c r="E29" s="44" t="s">
+      <c r="E29" s="45" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5820,22 +5830,22 @@
       <c r="A30" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="35">
+      <c r="B30" s="36">
         <v>45986</v>
       </c>
-      <c r="C30" s="35">
+      <c r="C30" s="36">
         <v>45987</v>
       </c>
       <c r="D30" s="8">
         <v>1</v>
       </c>
-      <c r="E30" s="44" t="s">
+      <c r="E30" s="45" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="8"/>
-      <c r="B31" s="35"/>
+      <c r="B31" s="36"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
@@ -6464,8 +6474,8 @@
   <sheetPr/>
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -6497,9 +6507,13 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
+    <row r="3" ht="86.4" spans="1:3">
+      <c r="A3" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>63</v>
+      </c>
       <c r="C3" s="14"/>
     </row>
     <row r="4" spans="1:3">
@@ -6780,7 +6794,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B1" s="14"/>
     </row>
@@ -6792,26 +6806,26 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="14" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6822,10 +6836,10 @@
     </row>
     <row r="7" s="23" customFormat="1" ht="57.6" spans="1:2">
       <c r="A7" s="27" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -6839,7 +6853,7 @@
   <sheetPr/>
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -6853,10 +6867,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>58</v>
@@ -6864,144 +6878,144 @@
     </row>
     <row r="2" ht="201.6" spans="1:3">
       <c r="A2" s="14" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" ht="100.8" spans="1:3">
       <c r="A3" s="14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" ht="72" spans="1:3">
       <c r="A4" s="16" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C4" s="14"/>
     </row>
     <row r="5" ht="129.6" spans="1:3">
       <c r="A5" s="15" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" ht="86.4" spans="1:4">
       <c r="A6" s="15" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" ht="158.4" spans="1:3">
       <c r="A7" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" ht="115.2" spans="1:3">
       <c r="A8" s="10" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C8" s="14"/>
     </row>
     <row r="9" ht="129.6" spans="1:3">
       <c r="A9" s="10" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C9" s="14"/>
     </row>
     <row r="10" ht="129.6" spans="1:3">
       <c r="A10" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C10" s="14"/>
     </row>
     <row r="11" ht="158.4" spans="1:3">
       <c r="A11" s="8" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C11" s="14"/>
     </row>
     <row r="12" ht="115.2" spans="1:3">
       <c r="A12" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" ht="158.4" spans="1:3">
       <c r="A13" s="8" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" ht="158.4" spans="1:3">
       <c r="A14" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C14" s="15"/>
     </row>
     <row r="15" ht="43.2" spans="1:3">
       <c r="A15" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C15" s="15"/>
     </row>
@@ -7010,10 +7024,10 @@
         <v>34</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" ht="187.2" spans="1:3">
@@ -7021,10 +7035,10 @@
         <v>36</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" ht="273.6" spans="1:4">
@@ -7032,13 +7046,13 @@
         <v>37</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" ht="158.4" spans="1:4">
@@ -7046,170 +7060,170 @@
         <v>38</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" ht="302.4" spans="1:4">
       <c r="A20" s="8" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" ht="174" customHeight="1" spans="1:3">
       <c r="A21" s="8" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C21" s="14"/>
     </row>
     <row r="22" ht="187.2" spans="1:3">
       <c r="A22" s="8" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C22" s="14"/>
     </row>
     <row r="23" ht="244.8" spans="1:3">
       <c r="A23" s="8" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C23" s="14"/>
     </row>
     <row r="24" ht="172.8" spans="1:3">
       <c r="A24" s="8" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C24" s="14"/>
     </row>
     <row r="25" ht="100.8" spans="1:3">
       <c r="A25" s="8" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C25" s="14"/>
     </row>
     <row r="26" ht="409" customHeight="1" spans="1:3">
       <c r="A26" s="8" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" ht="57.6" spans="1:3">
       <c r="A27" s="8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C27" s="14"/>
     </row>
     <row r="28" ht="409.5" spans="1:4">
       <c r="A28" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" ht="244.8" spans="1:3">
       <c r="A29" s="8" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" ht="244.8" spans="1:3">
       <c r="A30" s="8" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C30" s="14"/>
     </row>
     <row r="31" ht="187.2" spans="1:3">
       <c r="A31" s="8" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C31" s="14"/>
     </row>
     <row r="32" ht="259.2" spans="1:3">
       <c r="A32" s="20" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C32" s="14"/>
     </row>
     <row r="33" ht="345.6" spans="1:3">
       <c r="A33" s="20" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C33" s="14"/>
     </row>
     <row r="34" ht="100.8" spans="1:3">
       <c r="A34" s="8" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C34" s="14"/>
     </row>
     <row r="35" ht="72" spans="1:3">
       <c r="A35" s="8" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C35" s="14"/>
     </row>
@@ -7429,72 +7443,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="9" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="10" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="10" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="10" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="8" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="8" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:1">
@@ -7512,7 +7526,7 @@
         <v>38</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -7522,12 +7536,12 @@
     </row>
     <row r="19" ht="72" spans="1:1">
       <c r="A19" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" ht="72" spans="1:1">
       <c r="A20" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -7549,17 +7563,17 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -7600,7 +7614,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -7615,7 +7629,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
@@ -7857,7 +7871,7 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="3" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -8043,7 +8057,7 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="4" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>

</xml_diff>

<commit_message>
04-12-25   Tree topic updated
</commit_message>
<xml_diff>
--- a/JavaPrograms/Work Done.xlsx
+++ b/JavaPrograms/Work Done.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="245">
   <si>
     <r>
       <rPr>
@@ -2441,6 +2441,30 @@
         &amp;&amp; same(p.left, q.left)
         &amp;&amp; same(p.right, q.right);
 }</t>
+  </si>
+  <si>
+    <t>DFS = go deep left → go deep right
+Depth = max height of its children + 1
+Balanced tree = leftHeight and rightHeight differ ≤ 1
+We check balance bottom-up using dfs</t>
+  </si>
+  <si>
+    <t>DFS</t>
+  </si>
+  <si>
+    <t>What is DFS? (ELI5)
+DFS = Depth First Search.
+It’s just a fancy word for:
+“Go as deep as possible down one branch before coming back.”
+Like climbing a tree:
+Climb the left branch all the way down
+Come back
+Then climb the right branch all the way down
+That's it.
+Every recursion you’ve seen:
+dfs(node.left);
+dfs(node.right);
+is DFS.</t>
   </si>
   <si>
     <t>3 Merge Sort Problems (Simple → Medium)
@@ -3715,10 +3739,10 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="thin">
         <color auto="1"/>
-      </bottom>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -3728,10 +3752,10 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top/>
+      <bottom style="thin">
         <color auto="1"/>
-      </top>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -4055,7 +4079,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4141,6 +4165,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -4173,7 +4203,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -4182,13 +4212,13 @@
     <xf numFmtId="181" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4203,7 +4233,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4849,246 +4879,246 @@
   </cols>
   <sheetData>
     <row r="1" ht="90" customHeight="1" spans="1:6">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="53" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="54"/>
-      <c r="E1" s="55" t="s">
+      <c r="D1" s="56"/>
+      <c r="E1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="55"/>
+      <c r="F1" s="57"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="58" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="14"/>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="58"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="58" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="16"/>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="64"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="55"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="16"/>
       <c r="B13" s="16"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="16"/>
       <c r="B14" s="16"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
     </row>
     <row r="15" ht="15" customHeight="1" spans="1:6">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="16"/>
       <c r="B16" s="16"/>
-      <c r="C16" s="69" t="s">
+      <c r="C16" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="70"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="72"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="58" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="14"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="72"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="74"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="14"/>
       <c r="B20" s="14"/>
-      <c r="C20" s="71"/>
-      <c r="D20" s="72"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55"/>
+      <c r="C20" s="73"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="14"/>
       <c r="B22" s="14"/>
-      <c r="C22" s="71"/>
-      <c r="D22" s="72"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="74"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="74"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="76"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
-      <c r="C24" s="75" t="s">
+      <c r="C24" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="76"/>
+      <c r="D24" s="78"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
-      <c r="C25" s="77"/>
-      <c r="D25" s="78"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="80"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
-      <c r="C26" s="77"/>
-      <c r="D26" s="78"/>
+      <c r="C26" s="79"/>
+      <c r="D26" s="80"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="14"/>
       <c r="B27" s="14"/>
-      <c r="C27" s="77"/>
-      <c r="D27" s="78"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="80"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="14"/>
       <c r="B28" s="14"/>
-      <c r="C28" s="79"/>
-      <c r="D28" s="80"/>
+      <c r="C28" s="81"/>
+      <c r="D28" s="82"/>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="14"/>
@@ -5103,7 +5133,7 @@
       <c r="D30" s="20"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="58" t="s">
         <v>10</v>
       </c>
       <c r="B31" s="16"/>
@@ -5159,7 +5189,7 @@
       <c r="D39" s="20"/>
     </row>
     <row r="40" ht="18" customHeight="1" spans="1:4">
-      <c r="A40" s="56" t="s">
+      <c r="A40" s="58" t="s">
         <v>11</v>
       </c>
       <c r="B40" s="16"/>
@@ -5221,7 +5251,7 @@
       <c r="D49" s="20"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="56" t="s">
+      <c r="A50" s="58" t="s">
         <v>12</v>
       </c>
       <c r="B50" s="16"/>
@@ -5277,7 +5307,7 @@
       <c r="D58" s="20"/>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="56" t="s">
+      <c r="A59" s="58" t="s">
         <v>13</v>
       </c>
       <c r="B59" s="14"/>
@@ -5333,7 +5363,7 @@
       <c r="D67" s="20"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="56" t="s">
+      <c r="A68" s="58" t="s">
         <v>14</v>
       </c>
       <c r="B68" s="14"/>
@@ -5395,7 +5425,7 @@
       <c r="D77" s="20"/>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="56" t="s">
+      <c r="A78" s="58" t="s">
         <v>15</v>
       </c>
       <c r="B78" s="14"/>
@@ -5457,7 +5487,7 @@
       <c r="D87" s="20"/>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="56" t="s">
+      <c r="A88" s="58" t="s">
         <v>16</v>
       </c>
       <c r="B88" s="14"/>
@@ -5513,7 +5543,7 @@
       <c r="D96" s="20"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="56" t="s">
+      <c r="A97" s="58" t="s">
         <v>17</v>
       </c>
       <c r="B97" s="16"/>
@@ -5569,7 +5599,7 @@
       <c r="D105" s="20"/>
     </row>
     <row r="106" spans="1:4">
-      <c r="A106" s="56" t="s">
+      <c r="A106" s="58" t="s">
         <v>18</v>
       </c>
       <c r="B106" s="14"/>
@@ -5668,10 +5698,10 @@
   <sheetData>
     <row r="1" ht="409" customHeight="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -5827,7 +5857,7 @@
       <c r="D1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="41" t="s">
         <v>23</v>
       </c>
     </row>
@@ -5835,31 +5865,31 @@
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="40">
+      <c r="B2" s="42">
         <v>45976</v>
       </c>
-      <c r="C2" s="41">
+      <c r="C2" s="43">
         <v>45983</v>
       </c>
       <c r="D2" s="14">
         <v>4</v>
       </c>
-      <c r="E2" s="42"/>
+      <c r="E2" s="44"/>
     </row>
     <row r="3" ht="115.2" spans="1:5">
       <c r="A3" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="40">
+      <c r="B3" s="42">
         <v>45976</v>
       </c>
-      <c r="C3" s="41">
+      <c r="C3" s="43">
         <v>45983</v>
       </c>
       <c r="D3" s="14">
         <v>4</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="45" t="s">
         <v>26</v>
       </c>
     </row>
@@ -5867,16 +5897,16 @@
       <c r="A4" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="40">
+      <c r="B4" s="42">
         <v>45976</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="43">
         <v>45983</v>
       </c>
       <c r="D4" s="14">
         <v>3</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="46" t="s">
         <v>28</v>
       </c>
     </row>
@@ -5884,125 +5914,125 @@
       <c r="A5" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="40">
+      <c r="B5" s="42">
         <v>45976</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="43">
         <v>45983</v>
       </c>
       <c r="D5" s="14">
         <v>2</v>
       </c>
-      <c r="E5" s="45"/>
+      <c r="E5" s="47"/>
     </row>
     <row r="6" ht="115.2" spans="1:5">
       <c r="A6" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="40">
+      <c r="B6" s="42">
         <v>45976</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C6" s="43">
         <v>45983</v>
       </c>
       <c r="D6" s="14">
         <v>2</v>
       </c>
-      <c r="E6" s="45"/>
+      <c r="E6" s="47"/>
     </row>
     <row r="7" ht="129.6" spans="1:5">
       <c r="A7" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="40">
+      <c r="B7" s="42">
         <v>45976</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="43">
         <v>45983</v>
       </c>
       <c r="D7" s="14">
         <v>2</v>
       </c>
-      <c r="E7" s="45"/>
-    </row>
-    <row r="8" s="38" customFormat="1" ht="144" spans="1:5">
-      <c r="A8" s="46" t="s">
+      <c r="E7" s="47"/>
+    </row>
+    <row r="8" s="40" customFormat="1" ht="144" spans="1:5">
+      <c r="A8" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="41">
+      <c r="B8" s="43">
         <v>45976</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="43">
         <v>45983</v>
       </c>
-      <c r="D8" s="47">
+      <c r="D8" s="49">
         <v>2</v>
       </c>
-      <c r="E8" s="48"/>
-    </row>
-    <row r="9" s="38" customFormat="1" ht="158.4" spans="1:5">
-      <c r="A9" s="46" t="s">
+      <c r="E8" s="50"/>
+    </row>
+    <row r="9" s="40" customFormat="1" ht="158.4" spans="1:5">
+      <c r="A9" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="41">
+      <c r="B9" s="43">
         <v>45976</v>
       </c>
-      <c r="C9" s="41">
+      <c r="C9" s="43">
         <v>45983</v>
       </c>
-      <c r="D9" s="47">
+      <c r="D9" s="49">
         <v>1</v>
       </c>
-      <c r="E9" s="49"/>
-    </row>
-    <row r="10" s="38" customFormat="1" spans="1:5">
-      <c r="A10" s="47" t="s">
+      <c r="E9" s="51"/>
+    </row>
+    <row r="10" s="40" customFormat="1" spans="1:5">
+      <c r="A10" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="41">
+      <c r="B10" s="43">
         <v>45976</v>
       </c>
-      <c r="C10" s="41">
+      <c r="C10" s="43">
         <v>45983</v>
       </c>
-      <c r="D10" s="47">
+      <c r="D10" s="49">
         <v>1</v>
       </c>
-      <c r="E10" s="50" t="s">
+      <c r="E10" s="52" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" s="38" customFormat="1" spans="1:5">
-      <c r="A11" s="47" t="s">
+    <row r="11" s="40" customFormat="1" spans="1:5">
+      <c r="A11" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="41">
+      <c r="B11" s="43">
         <v>45976</v>
       </c>
-      <c r="C11" s="41">
+      <c r="C11" s="43">
         <v>45983</v>
       </c>
-      <c r="D11" s="47">
+      <c r="D11" s="49">
         <v>1</v>
       </c>
-      <c r="E11" s="50" t="s">
+      <c r="E11" s="52" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" s="38" customFormat="1" spans="1:5">
-      <c r="A12" s="47" t="s">
+    <row r="12" s="40" customFormat="1" spans="1:5">
+      <c r="A12" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="41">
+      <c r="B12" s="43">
         <v>45976</v>
       </c>
-      <c r="C12" s="41">
+      <c r="C12" s="43">
         <v>45983</v>
       </c>
-      <c r="D12" s="47">
+      <c r="D12" s="49">
         <v>1</v>
       </c>
-      <c r="E12" s="50" t="s">
+      <c r="E12" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6010,16 +6040,16 @@
       <c r="A13" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="41">
+      <c r="B13" s="43">
         <v>45977</v>
       </c>
-      <c r="C13" s="41">
+      <c r="C13" s="43">
         <v>45982</v>
       </c>
       <c r="D13" s="14">
         <v>1</v>
       </c>
-      <c r="E13" s="50" t="s">
+      <c r="E13" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6027,16 +6057,16 @@
       <c r="A14" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="41">
+      <c r="B14" s="43">
         <v>45980</v>
       </c>
-      <c r="C14" s="41">
+      <c r="C14" s="43">
         <v>45982</v>
       </c>
       <c r="D14" s="14">
         <v>1</v>
       </c>
-      <c r="E14" s="50" t="s">
+      <c r="E14" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6044,16 +6074,16 @@
       <c r="A15" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="41">
+      <c r="B15" s="43">
         <v>45980</v>
       </c>
-      <c r="C15" s="41">
+      <c r="C15" s="43">
         <v>45982</v>
       </c>
       <c r="D15" s="14">
         <v>1</v>
       </c>
-      <c r="E15" s="50" t="s">
+      <c r="E15" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6061,16 +6091,16 @@
       <c r="A16" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="41">
+      <c r="B16" s="43">
         <v>45980</v>
       </c>
-      <c r="C16" s="41">
+      <c r="C16" s="43">
         <v>45982</v>
       </c>
       <c r="D16" s="14">
         <v>1</v>
       </c>
-      <c r="E16" s="50" t="s">
+      <c r="E16" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6078,16 +6108,16 @@
       <c r="A17" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="41">
+      <c r="B17" s="43">
         <v>45980</v>
       </c>
-      <c r="C17" s="41">
+      <c r="C17" s="43">
         <v>45982</v>
       </c>
       <c r="D17" s="14">
         <v>1</v>
       </c>
-      <c r="E17" s="50" t="s">
+      <c r="E17" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6095,16 +6125,16 @@
       <c r="A18" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="41">
+      <c r="B18" s="43">
         <v>45981</v>
       </c>
-      <c r="C18" s="41">
+      <c r="C18" s="43">
         <v>45983</v>
       </c>
       <c r="D18" s="14">
         <v>1</v>
       </c>
-      <c r="E18" s="50" t="s">
+      <c r="E18" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6112,16 +6142,16 @@
       <c r="A19" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="41">
+      <c r="B19" s="43">
         <v>45982</v>
       </c>
-      <c r="C19" s="41">
+      <c r="C19" s="43">
         <v>45984</v>
       </c>
       <c r="D19" s="14">
         <v>1</v>
       </c>
-      <c r="E19" s="50" t="s">
+      <c r="E19" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6129,16 +6159,16 @@
       <c r="A20" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="41">
+      <c r="B20" s="43">
         <v>45983</v>
       </c>
-      <c r="C20" s="41">
+      <c r="C20" s="43">
         <v>45985</v>
       </c>
       <c r="D20" s="14">
         <v>1</v>
       </c>
-      <c r="E20" s="50" t="s">
+      <c r="E20" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6146,16 +6176,16 @@
       <c r="A21" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="41">
+      <c r="B21" s="43">
         <v>45986</v>
       </c>
-      <c r="C21" s="41">
+      <c r="C21" s="43">
         <v>45987</v>
       </c>
       <c r="D21" s="14">
         <v>1</v>
       </c>
-      <c r="E21" s="50" t="s">
+      <c r="E21" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6163,16 +6193,16 @@
       <c r="A22" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="41">
+      <c r="B22" s="43">
         <v>45986</v>
       </c>
-      <c r="C22" s="41">
+      <c r="C22" s="43">
         <v>45987</v>
       </c>
       <c r="D22" s="14">
         <v>1</v>
       </c>
-      <c r="E22" s="50" t="s">
+      <c r="E22" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6180,16 +6210,16 @@
       <c r="A23" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="41">
+      <c r="B23" s="43">
         <v>45986</v>
       </c>
-      <c r="C23" s="41">
+      <c r="C23" s="43">
         <v>45987</v>
       </c>
       <c r="D23" s="14">
         <v>1</v>
       </c>
-      <c r="E23" s="50" t="s">
+      <c r="E23" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6197,16 +6227,16 @@
       <c r="A24" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="41">
+      <c r="B24" s="43">
         <v>45986</v>
       </c>
-      <c r="C24" s="41">
+      <c r="C24" s="43">
         <v>45987</v>
       </c>
       <c r="D24" s="14">
         <v>1</v>
       </c>
-      <c r="E24" s="50" t="s">
+      <c r="E24" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6214,16 +6244,16 @@
       <c r="A25" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="41">
+      <c r="B25" s="43">
         <v>45986</v>
       </c>
-      <c r="C25" s="41">
+      <c r="C25" s="43">
         <v>45987</v>
       </c>
       <c r="D25" s="14">
         <v>1</v>
       </c>
-      <c r="E25" s="50" t="s">
+      <c r="E25" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6231,16 +6261,16 @@
       <c r="A26" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="41">
+      <c r="B26" s="43">
         <v>45986</v>
       </c>
-      <c r="C26" s="41">
+      <c r="C26" s="43">
         <v>45987</v>
       </c>
       <c r="D26" s="14">
         <v>1</v>
       </c>
-      <c r="E26" s="50" t="s">
+      <c r="E26" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6248,16 +6278,16 @@
       <c r="A27" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="41">
+      <c r="B27" s="43">
         <v>45986</v>
       </c>
-      <c r="C27" s="41">
+      <c r="C27" s="43">
         <v>45987</v>
       </c>
       <c r="D27" s="14">
         <v>1</v>
       </c>
-      <c r="E27" s="50" t="s">
+      <c r="E27" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6265,16 +6295,16 @@
       <c r="A28" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="41">
+      <c r="B28" s="43">
         <v>45986</v>
       </c>
-      <c r="C28" s="41">
+      <c r="C28" s="43">
         <v>45987</v>
       </c>
       <c r="D28" s="14">
         <v>1</v>
       </c>
-      <c r="E28" s="50" t="s">
+      <c r="E28" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6282,16 +6312,16 @@
       <c r="A29" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="41">
+      <c r="B29" s="43">
         <v>45986</v>
       </c>
-      <c r="C29" s="41">
+      <c r="C29" s="43">
         <v>45987</v>
       </c>
       <c r="D29" s="14">
         <v>1</v>
       </c>
-      <c r="E29" s="50" t="s">
+      <c r="E29" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6299,16 +6329,16 @@
       <c r="A30" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="41">
+      <c r="B30" s="43">
         <v>45986</v>
       </c>
-      <c r="C30" s="41">
+      <c r="C30" s="43">
         <v>45987</v>
       </c>
       <c r="D30" s="14">
         <v>1</v>
       </c>
-      <c r="E30" s="50" t="s">
+      <c r="E30" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6316,16 +6346,16 @@
       <c r="A31" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="41">
+      <c r="B31" s="43">
         <v>45992</v>
       </c>
-      <c r="C31" s="41">
+      <c r="C31" s="43">
         <v>45993</v>
       </c>
       <c r="D31" s="14">
         <v>1</v>
       </c>
-      <c r="E31" s="50" t="s">
+      <c r="E31" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6333,16 +6363,16 @@
       <c r="A32" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="41">
+      <c r="B32" s="43">
         <v>45992</v>
       </c>
-      <c r="C32" s="41">
+      <c r="C32" s="43">
         <v>45993</v>
       </c>
       <c r="D32" s="14">
         <v>1</v>
       </c>
-      <c r="E32" s="50" t="s">
+      <c r="E32" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6350,16 +6380,16 @@
       <c r="A33" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="41">
+      <c r="B33" s="43">
         <v>45992</v>
       </c>
-      <c r="C33" s="41">
+      <c r="C33" s="43">
         <v>45993</v>
       </c>
       <c r="D33" s="14">
         <v>1</v>
       </c>
-      <c r="E33" s="50" t="s">
+      <c r="E33" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6367,16 +6397,16 @@
       <c r="A34" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="41">
+      <c r="B34" s="43">
         <v>45993</v>
       </c>
-      <c r="C34" s="41">
+      <c r="C34" s="43">
         <v>45993</v>
       </c>
       <c r="D34" s="14">
         <v>1</v>
       </c>
-      <c r="E34" s="50" t="s">
+      <c r="E34" s="52" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6995,21 +7025,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="37" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" ht="409.5" spans="1:3">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="39" t="s">
         <v>64</v>
       </c>
       <c r="C2" s="21" t="s">
@@ -7316,7 +7346,7 @@
       <c r="B1" s="20"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="30">
+      <c r="A2" s="32">
         <v>45962</v>
       </c>
       <c r="B2" s="20"/>
@@ -7325,7 +7355,7 @@
       <c r="A3" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="33" t="s">
         <v>74</v>
       </c>
     </row>
@@ -7333,7 +7363,7 @@
       <c r="A4" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="33" t="s">
         <v>76</v>
       </c>
     </row>
@@ -7341,21 +7371,21 @@
       <c r="A5" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="33" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="32">
+      <c r="A6" s="34">
         <v>45969</v>
       </c>
       <c r="B6" s="20"/>
     </row>
-    <row r="7" s="29" customFormat="1" ht="57.6" spans="1:2">
-      <c r="A7" s="33" t="s">
+    <row r="7" s="31" customFormat="1" ht="57.6" spans="1:2">
+      <c r="A7" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="36" t="s">
         <v>80</v>
       </c>
     </row>
@@ -7371,7 +7401,7 @@
   <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -7751,12 +7781,18 @@
       <c r="B36" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="C36" s="20"/>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="20"/>
+      <c r="C36" s="28" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="37" ht="187.2" spans="1:3">
+      <c r="A37" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="C37" s="29"/>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="14"/>
@@ -7834,8 +7870,8 @@
       <c r="C52" s="20"/>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="28"/>
-      <c r="B53" s="28"/>
+      <c r="A53" s="30"/>
+      <c r="B53" s="30"/>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="14"/>
@@ -7942,6 +7978,9 @@
       <c r="B79" s="14"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C36:C37"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -8047,7 +8086,7 @@
         <v>38</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -8057,12 +8096,12 @@
     </row>
     <row r="19" ht="72" spans="1:1">
       <c r="A19" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" ht="72" spans="1:1">
       <c r="A20" s="1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -8084,17 +8123,17 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" s="13" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -8123,302 +8162,302 @@
   <sheetData>
     <row r="1" spans="2:3">
       <c r="B1" s="7" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="2:3">
       <c r="B2" s="8" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="8" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="8" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="6" spans="2:3">
       <c r="B6" s="8" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="8" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" ht="43.2" spans="2:3">
       <c r="B8" s="8" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" s="9" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" ht="23.4" spans="2:2">
       <c r="B11" s="10" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="2:2">
       <c r="B12" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" s="11" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" s="11" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="2:2">
       <c r="B16" s="11" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="11" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="11" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="11" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="11" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" s="11" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" s="11" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" s="11" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" ht="23.4" spans="2:2">
       <c r="B26" s="10" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" s="11" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" s="11" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" s="11" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" s="11" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" s="11" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" s="11" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="11" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" s="11" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" s="11" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" s="11" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" s="11" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="40" spans="2:2">
       <c r="B40" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" ht="23.4" spans="2:2">
       <c r="B41" s="10" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="42" spans="2:2">
       <c r="B42" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" spans="2:2">
       <c r="B43" s="11" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44" spans="2:2">
       <c r="B44" s="11" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="45" spans="2:2">
       <c r="B45" s="11" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46" spans="2:2">
       <c r="B46" s="11" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" spans="2:2">
       <c r="B47" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="48" spans="2:2">
       <c r="B48" s="12" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="49" spans="2:2">
       <c r="B49" s="12" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50" s="12" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="51" spans="2:2">
       <c r="B51" s="12" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="52" spans="2:2">
       <c r="B52" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="54" ht="13" customHeight="1"/>
     <row r="55" ht="22" customHeight="1" spans="2:2">
       <c r="B55" s="10" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="56" spans="2:2">
       <c r="B56" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="57" spans="2:2">
       <c r="B57" s="11" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="58" spans="2:2">
@@ -8433,17 +8472,17 @@
     </row>
     <row r="60" spans="2:2">
       <c r="B60" s="11" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="61" spans="2:2">
       <c r="B61" s="11" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="62" spans="2:2">
       <c r="B62" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -8465,7 +8504,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="3" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -8480,7 +8519,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="5" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
@@ -8722,7 +8761,7 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="3" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -8908,7 +8947,7 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="4" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>

</xml_diff>

<commit_message>
07-12-25 BFS          Queue          Understand LinkedList as a Queue
</commit_message>
<xml_diff>
--- a/JavaPrograms/Work Done.xlsx
+++ b/JavaPrograms/Work Done.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" firstSheet="3" activeTab="10"/>
+    <workbookView windowWidth="23040" windowHeight="9000" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="DSA plan" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="360">
   <si>
     <r>
       <rPr>
@@ -2447,7 +2447,17 @@
     <t>DFS = go deep left → go deep right
 Depth = max height of its children + 1
 Balanced tree = leftHeight and rightHeight differ ≤ 1
-We check balance bottom-up using dfs</t>
+We check balance bottom-up using dfs
+BFS vs DFS – TL;DR
+BFS
+Uses queue
+Explores level by level
+Good for: shortest path, level order, “first time you reach something”
+DFS
+Uses recursion or stack
+Explores one path fully before trying another
+Good for: depth, diameter, tree shape checks, backtracking
+Both are just different ways of walking the same structure.</t>
   </si>
   <si>
     <t>DFS</t>
@@ -2466,6 +2476,60 @@
 dfs(node.left);
 dfs(node.right);
 is DFS.</t>
+  </si>
+  <si>
+    <t>BFS</t>
+  </si>
+  <si>
+    <t>What is BFS?
+BFS = Breadth-First Search.
+Super simple idea:
+You explore a tree level by level.
+First you visit depth 0 (root),
+then all nodes at depth 1,
+then all nodes at depth 2,
+and so on.
+Real-life analogy:
+You’re on floor 0 in a building. You visit everyone on floor 0,
+then floor 1,
+then floor 2…
+You don’t randomly go up/down.
+In code, BFS is almost always done with a queue:
+Put starting node in queue
+While queue not empty:
+Remove front
+Add its children
+For trees, this gives level order naturally.</t>
+  </si>
+  <si>
+    <t>Queue</t>
+  </si>
+  <si>
+    <t>Queue = First-In First-Out (FIFO)
+Real-life example:
+People stand in line.
+The first person who enters the line is the first to exit.
+In Java:
+Queue&lt;TreeNode&gt; q = new LinkedList&lt;&gt;();
+q.add(root);  // push
+q.poll();     // remove first
+You don't have to memorize the syntax.
+Just understand:
+Stack → DFS
+Queue → BFS
+That's the entire idea.</t>
+  </si>
+  <si>
+    <t>Understand LinkedList as a Queue</t>
+  </si>
+  <si>
+    <t>Java doesn't have a separate queue class with its own constructor.
+Instead:
+Queue&lt;TreeNode&gt; q = new LinkedList&lt;&gt;();
+LinkedList implements the Queue interface.
+We use it only because Java requires it.
+If Java had a Queue() constructor, we’d use that instead.
+You don't need to know internal implementation right now.</t>
   </si>
   <si>
     <t>3 Merge Sort Problems (Simple → Medium)
@@ -3590,7 +3654,7 @@
     <numFmt numFmtId="181" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="182" formatCode="dd/mmm/yy"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3649,6 +3713,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4097,9 +4168,7 @@
         <color auto="1"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -4110,7 +4179,9 @@
         <color auto="1"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -4293,7 +4364,7 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4302,128 +4373,128 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4529,13 +4600,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="181" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4547,10 +4624,10 @@
     <xf numFmtId="181" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
@@ -4574,7 +4651,7 @@
     <xf numFmtId="182" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4583,7 +4660,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4592,10 +4669,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5241,246 +5318,246 @@
   </cols>
   <sheetData>
     <row r="1" ht="90" customHeight="1" spans="1:6">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="62"/>
-      <c r="E1" s="63" t="s">
+      <c r="D1" s="64"/>
+      <c r="E1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="63"/>
+      <c r="F1" s="65"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="21"/>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="66"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="21"/>
       <c r="B3" s="21"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="21"/>
       <c r="B4" s="21"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="21"/>
       <c r="B5" s="21"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="21"/>
       <c r="B6" s="21"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="21"/>
       <c r="B8" s="21"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="64" t="s">
+      <c r="A9" s="66" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="23"/>
-      <c r="C9" s="71" t="s">
+      <c r="C9" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="72"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="23"/>
       <c r="B10" s="23"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="23"/>
       <c r="B11" s="23"/>
-      <c r="C11" s="73"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="23"/>
       <c r="B12" s="23"/>
-      <c r="C12" s="73"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="23"/>
       <c r="B13" s="23"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="23"/>
       <c r="B14" s="23"/>
-      <c r="C14" s="73"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
     </row>
     <row r="15" ht="15" customHeight="1" spans="1:6">
       <c r="A15" s="23"/>
       <c r="B15" s="23"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="23"/>
       <c r="B16" s="23"/>
-      <c r="C16" s="77" t="s">
+      <c r="C16" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="78"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="23"/>
       <c r="B17" s="23"/>
-      <c r="C17" s="79"/>
-      <c r="D17" s="80"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
+      <c r="C17" s="81"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="23"/>
       <c r="B18" s="23"/>
-      <c r="C18" s="79"/>
-      <c r="D18" s="80"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="65"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="64" t="s">
+      <c r="A19" s="66" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="21"/>
-      <c r="C19" s="79"/>
-      <c r="D19" s="80"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="63"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="21"/>
       <c r="B20" s="21"/>
-      <c r="C20" s="79"/>
-      <c r="D20" s="80"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="65"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="21"/>
       <c r="B21" s="21"/>
-      <c r="C21" s="79"/>
-      <c r="D21" s="80"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="65"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
-      <c r="C22" s="79"/>
-      <c r="D22" s="80"/>
+      <c r="C22" s="81"/>
+      <c r="D22" s="82"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="21"/>
       <c r="B23" s="21"/>
-      <c r="C23" s="81"/>
-      <c r="D23" s="82"/>
+      <c r="C23" s="83"/>
+      <c r="D23" s="84"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="21"/>
       <c r="B24" s="21"/>
-      <c r="C24" s="83" t="s">
+      <c r="C24" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="84"/>
+      <c r="D24" s="86"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="21"/>
       <c r="B25" s="21"/>
-      <c r="C25" s="85"/>
-      <c r="D25" s="86"/>
+      <c r="C25" s="87"/>
+      <c r="D25" s="88"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
-      <c r="C26" s="85"/>
-      <c r="D26" s="86"/>
+      <c r="C26" s="87"/>
+      <c r="D26" s="88"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="21"/>
       <c r="B27" s="21"/>
-      <c r="C27" s="85"/>
-      <c r="D27" s="86"/>
+      <c r="C27" s="87"/>
+      <c r="D27" s="88"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="21"/>
       <c r="B28" s="21"/>
-      <c r="C28" s="87"/>
-      <c r="D28" s="88"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="90"/>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="21"/>
@@ -5495,7 +5572,7 @@
       <c r="D30" s="27"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="64" t="s">
+      <c r="A31" s="66" t="s">
         <v>10</v>
       </c>
       <c r="B31" s="23"/>
@@ -5551,7 +5628,7 @@
       <c r="D39" s="27"/>
     </row>
     <row r="40" ht="18" customHeight="1" spans="1:4">
-      <c r="A40" s="64" t="s">
+      <c r="A40" s="66" t="s">
         <v>11</v>
       </c>
       <c r="B40" s="23"/>
@@ -5613,7 +5690,7 @@
       <c r="D49" s="27"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="64" t="s">
+      <c r="A50" s="66" t="s">
         <v>12</v>
       </c>
       <c r="B50" s="23"/>
@@ -5669,7 +5746,7 @@
       <c r="D58" s="27"/>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="64" t="s">
+      <c r="A59" s="66" t="s">
         <v>13</v>
       </c>
       <c r="B59" s="21"/>
@@ -5725,7 +5802,7 @@
       <c r="D67" s="27"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="64" t="s">
+      <c r="A68" s="66" t="s">
         <v>14</v>
       </c>
       <c r="B68" s="21"/>
@@ -5787,7 +5864,7 @@
       <c r="D77" s="27"/>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="64" t="s">
+      <c r="A78" s="66" t="s">
         <v>15</v>
       </c>
       <c r="B78" s="21"/>
@@ -5849,7 +5926,7 @@
       <c r="D87" s="27"/>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="64" t="s">
+      <c r="A88" s="66" t="s">
         <v>16</v>
       </c>
       <c r="B88" s="21"/>
@@ -5905,7 +5982,7 @@
       <c r="D96" s="27"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="64" t="s">
+      <c r="A97" s="66" t="s">
         <v>17</v>
       </c>
       <c r="B97" s="23"/>
@@ -5961,7 +6038,7 @@
       <c r="D105" s="27"/>
     </row>
     <row r="106" spans="1:4">
-      <c r="A106" s="64" t="s">
+      <c r="A106" s="66" t="s">
         <v>18</v>
       </c>
       <c r="B106" s="21"/>
@@ -6060,10 +6137,10 @@
   <sheetData>
     <row r="1" ht="409" customHeight="1" spans="1:2">
       <c r="A1" s="8" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -6193,7 +6270,7 @@
   <sheetPr/>
   <dimension ref="A1:C223"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -6214,12 +6291,12 @@
     </row>
     <row r="2" ht="31.2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:1">
@@ -6229,7 +6306,7 @@
     </row>
     <row r="8" ht="23.4" spans="1:1">
       <c r="A8" s="6" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:1">
@@ -6244,7 +6321,7 @@
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
     </row>
     <row r="16" spans="1:1">
@@ -6254,52 +6331,52 @@
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="1" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="1" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="1" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="1" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="1" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="1" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="7" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="1" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
     </row>
     <row r="36" ht="23.4" spans="1:1">
@@ -6307,177 +6384,177 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="1" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="1" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="1" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="1" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="1" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="1" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="1" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="1" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="1" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="7" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="1" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
     </row>
     <row r="60" ht="23.4" spans="1:1">
       <c r="A60" s="6" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="1" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="1" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="1" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="1" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="1" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="1" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="1" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="1" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="1" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="1" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="7" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="1" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
     </row>
     <row r="86" ht="23.4" spans="1:1">
       <c r="A86" s="6" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="1" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="1" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="1" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="1" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" s="1" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" s="1" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="1" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" s="1" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="1" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
     </row>
     <row r="103" spans="1:1">
@@ -6487,12 +6564,12 @@
     </row>
     <row r="105" spans="1:1">
       <c r="A105" s="1" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" s="1" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
     </row>
     <row r="108" spans="1:1">
@@ -6500,12 +6577,12 @@
     </row>
     <row r="109" spans="1:1">
       <c r="A109" s="1" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" s="1" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
     </row>
     <row r="112" ht="23.4" spans="1:1">
@@ -6513,42 +6590,42 @@
     </row>
     <row r="113" spans="1:1">
       <c r="A113" s="1" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" s="1" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" s="1" t="s">
-        <v>300</v>
+        <v>306</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" s="1" t="s">
-        <v>301</v>
+        <v>307</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" s="1" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" s="1" t="s">
-        <v>303</v>
+        <v>309</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" s="1" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" s="1" t="s">
-        <v>305</v>
+        <v>311</v>
       </c>
     </row>
     <row r="128" spans="1:1">
@@ -6556,12 +6633,12 @@
     </row>
     <row r="129" spans="1:1">
       <c r="A129" s="1" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" s="1" t="s">
-        <v>307</v>
+        <v>313</v>
       </c>
     </row>
     <row r="132" ht="23.4" spans="1:1">
@@ -6569,62 +6646,62 @@
     </row>
     <row r="133" spans="1:1">
       <c r="A133" s="1" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" s="1" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" s="1" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" s="1" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" s="1" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" s="1" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" s="1" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" s="1" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" s="1" t="s">
-        <v>316</v>
+        <v>322</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" s="7" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" s="1" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" s="1" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
     </row>
     <row r="154" ht="23.4" spans="1:1">
@@ -6632,62 +6709,62 @@
     </row>
     <row r="156" spans="1:1">
       <c r="A156" s="1" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" s="1" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" s="1" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" s="1" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" s="1" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" s="1" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" s="1" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" s="1" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" s="1" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" s="7" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" s="1" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" s="1" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
     </row>
     <row r="180" spans="1:1">
@@ -6697,7 +6774,7 @@
     </row>
     <row r="182" spans="1:1">
       <c r="A182" s="1" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
     </row>
     <row r="184" spans="1:1">
@@ -6707,122 +6784,122 @@
     </row>
     <row r="186" spans="1:1">
       <c r="A186" s="1" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" s="1" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" s="1" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" s="1" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" s="1" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" s="1" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" s="1" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" s="1" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" s="1" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" s="1" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" s="1" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" s="1" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" s="1" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" s="1" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" s="1" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" s="1" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" s="1" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" s="1" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" s="1" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" s="1" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" s="1" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" s="1" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" s="1" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" s="1" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -6862,7 +6939,7 @@
       <c r="D1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="49" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6870,31 +6947,31 @@
       <c r="A2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="48">
+      <c r="B2" s="50">
         <v>45976</v>
       </c>
-      <c r="C2" s="49">
+      <c r="C2" s="51">
         <v>45983</v>
       </c>
       <c r="D2" s="21">
         <v>4</v>
       </c>
-      <c r="E2" s="50"/>
+      <c r="E2" s="52"/>
     </row>
     <row r="3" ht="115.2" spans="1:5">
       <c r="A3" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="48">
+      <c r="B3" s="50">
         <v>45976</v>
       </c>
-      <c r="C3" s="49">
+      <c r="C3" s="51">
         <v>45983</v>
       </c>
       <c r="D3" s="21">
         <v>4</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="53" t="s">
         <v>26</v>
       </c>
     </row>
@@ -6902,16 +6979,16 @@
       <c r="A4" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="48">
+      <c r="B4" s="50">
         <v>45976</v>
       </c>
-      <c r="C4" s="49">
+      <c r="C4" s="51">
         <v>45983</v>
       </c>
       <c r="D4" s="21">
         <v>3</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="54" t="s">
         <v>28</v>
       </c>
     </row>
@@ -6919,125 +6996,125 @@
       <c r="A5" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="48">
+      <c r="B5" s="50">
         <v>45976</v>
       </c>
-      <c r="C5" s="49">
+      <c r="C5" s="51">
         <v>45983</v>
       </c>
       <c r="D5" s="21">
         <v>2</v>
       </c>
-      <c r="E5" s="53"/>
+      <c r="E5" s="55"/>
     </row>
     <row r="6" ht="115.2" spans="1:5">
       <c r="A6" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="48">
+      <c r="B6" s="50">
         <v>45976</v>
       </c>
-      <c r="C6" s="49">
+      <c r="C6" s="51">
         <v>45983</v>
       </c>
       <c r="D6" s="21">
         <v>2</v>
       </c>
-      <c r="E6" s="53"/>
+      <c r="E6" s="55"/>
     </row>
     <row r="7" ht="129.6" spans="1:5">
       <c r="A7" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="48">
+      <c r="B7" s="50">
         <v>45976</v>
       </c>
-      <c r="C7" s="49">
+      <c r="C7" s="51">
         <v>45983</v>
       </c>
       <c r="D7" s="21">
         <v>2</v>
       </c>
-      <c r="E7" s="53"/>
-    </row>
-    <row r="8" s="46" customFormat="1" ht="144" spans="1:5">
-      <c r="A8" s="54" t="s">
+      <c r="E7" s="55"/>
+    </row>
+    <row r="8" s="48" customFormat="1" ht="144" spans="1:5">
+      <c r="A8" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="49">
+      <c r="B8" s="51">
         <v>45976</v>
       </c>
-      <c r="C8" s="49">
+      <c r="C8" s="51">
         <v>45983</v>
       </c>
-      <c r="D8" s="55">
+      <c r="D8" s="57">
         <v>2</v>
       </c>
-      <c r="E8" s="56"/>
-    </row>
-    <row r="9" s="46" customFormat="1" ht="158.4" spans="1:5">
-      <c r="A9" s="54" t="s">
+      <c r="E8" s="58"/>
+    </row>
+    <row r="9" s="48" customFormat="1" ht="158.4" spans="1:5">
+      <c r="A9" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="49">
+      <c r="B9" s="51">
         <v>45976</v>
       </c>
-      <c r="C9" s="49">
+      <c r="C9" s="51">
         <v>45983</v>
       </c>
-      <c r="D9" s="55">
+      <c r="D9" s="57">
         <v>1</v>
       </c>
-      <c r="E9" s="57"/>
-    </row>
-    <row r="10" s="46" customFormat="1" spans="1:5">
-      <c r="A10" s="55" t="s">
+      <c r="E9" s="59"/>
+    </row>
+    <row r="10" s="48" customFormat="1" spans="1:5">
+      <c r="A10" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="49">
+      <c r="B10" s="51">
         <v>45976</v>
       </c>
-      <c r="C10" s="49">
+      <c r="C10" s="51">
         <v>45983</v>
       </c>
-      <c r="D10" s="55">
+      <c r="D10" s="57">
         <v>1</v>
       </c>
-      <c r="E10" s="58" t="s">
+      <c r="E10" s="60" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" s="46" customFormat="1" spans="1:5">
-      <c r="A11" s="55" t="s">
+    <row r="11" s="48" customFormat="1" spans="1:5">
+      <c r="A11" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="49">
+      <c r="B11" s="51">
         <v>45976</v>
       </c>
-      <c r="C11" s="49">
+      <c r="C11" s="51">
         <v>45983</v>
       </c>
-      <c r="D11" s="55">
+      <c r="D11" s="57">
         <v>1</v>
       </c>
-      <c r="E11" s="58" t="s">
+      <c r="E11" s="60" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" s="46" customFormat="1" spans="1:5">
-      <c r="A12" s="55" t="s">
+    <row r="12" s="48" customFormat="1" spans="1:5">
+      <c r="A12" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="49">
+      <c r="B12" s="51">
         <v>45976</v>
       </c>
-      <c r="C12" s="49">
+      <c r="C12" s="51">
         <v>45983</v>
       </c>
-      <c r="D12" s="55">
+      <c r="D12" s="57">
         <v>1</v>
       </c>
-      <c r="E12" s="58" t="s">
+      <c r="E12" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7045,16 +7122,16 @@
       <c r="A13" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="49">
+      <c r="B13" s="51">
         <v>45977</v>
       </c>
-      <c r="C13" s="49">
+      <c r="C13" s="51">
         <v>45982</v>
       </c>
       <c r="D13" s="21">
         <v>1</v>
       </c>
-      <c r="E13" s="58" t="s">
+      <c r="E13" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7062,16 +7139,16 @@
       <c r="A14" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="49">
+      <c r="B14" s="51">
         <v>45980</v>
       </c>
-      <c r="C14" s="49">
+      <c r="C14" s="51">
         <v>45982</v>
       </c>
       <c r="D14" s="21">
         <v>1</v>
       </c>
-      <c r="E14" s="58" t="s">
+      <c r="E14" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7079,16 +7156,16 @@
       <c r="A15" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="49">
+      <c r="B15" s="51">
         <v>45980</v>
       </c>
-      <c r="C15" s="49">
+      <c r="C15" s="51">
         <v>45982</v>
       </c>
       <c r="D15" s="21">
         <v>1</v>
       </c>
-      <c r="E15" s="58" t="s">
+      <c r="E15" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7096,16 +7173,16 @@
       <c r="A16" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="49">
+      <c r="B16" s="51">
         <v>45980</v>
       </c>
-      <c r="C16" s="49">
+      <c r="C16" s="51">
         <v>45982</v>
       </c>
       <c r="D16" s="21">
         <v>1</v>
       </c>
-      <c r="E16" s="58" t="s">
+      <c r="E16" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7113,16 +7190,16 @@
       <c r="A17" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="49">
+      <c r="B17" s="51">
         <v>45980</v>
       </c>
-      <c r="C17" s="49">
+      <c r="C17" s="51">
         <v>45982</v>
       </c>
       <c r="D17" s="21">
         <v>1</v>
       </c>
-      <c r="E17" s="58" t="s">
+      <c r="E17" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7130,16 +7207,16 @@
       <c r="A18" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="49">
+      <c r="B18" s="51">
         <v>45981</v>
       </c>
-      <c r="C18" s="49">
+      <c r="C18" s="51">
         <v>45983</v>
       </c>
       <c r="D18" s="21">
         <v>1</v>
       </c>
-      <c r="E18" s="58" t="s">
+      <c r="E18" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7147,16 +7224,16 @@
       <c r="A19" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="49">
+      <c r="B19" s="51">
         <v>45982</v>
       </c>
-      <c r="C19" s="49">
+      <c r="C19" s="51">
         <v>45984</v>
       </c>
       <c r="D19" s="21">
         <v>1</v>
       </c>
-      <c r="E19" s="58" t="s">
+      <c r="E19" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7164,16 +7241,16 @@
       <c r="A20" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="49">
+      <c r="B20" s="51">
         <v>45983</v>
       </c>
-      <c r="C20" s="49">
+      <c r="C20" s="51">
         <v>45985</v>
       </c>
       <c r="D20" s="21">
         <v>1</v>
       </c>
-      <c r="E20" s="58" t="s">
+      <c r="E20" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7181,16 +7258,16 @@
       <c r="A21" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="49">
+      <c r="B21" s="51">
         <v>45986</v>
       </c>
-      <c r="C21" s="49">
+      <c r="C21" s="51">
         <v>45987</v>
       </c>
       <c r="D21" s="21">
         <v>1</v>
       </c>
-      <c r="E21" s="58" t="s">
+      <c r="E21" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7198,16 +7275,16 @@
       <c r="A22" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="49">
+      <c r="B22" s="51">
         <v>45986</v>
       </c>
-      <c r="C22" s="49">
+      <c r="C22" s="51">
         <v>45987</v>
       </c>
       <c r="D22" s="21">
         <v>1</v>
       </c>
-      <c r="E22" s="58" t="s">
+      <c r="E22" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7215,16 +7292,16 @@
       <c r="A23" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="49">
+      <c r="B23" s="51">
         <v>45986</v>
       </c>
-      <c r="C23" s="49">
+      <c r="C23" s="51">
         <v>45987</v>
       </c>
       <c r="D23" s="21">
         <v>1</v>
       </c>
-      <c r="E23" s="58" t="s">
+      <c r="E23" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7232,16 +7309,16 @@
       <c r="A24" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="49">
+      <c r="B24" s="51">
         <v>45986</v>
       </c>
-      <c r="C24" s="49">
+      <c r="C24" s="51">
         <v>45987</v>
       </c>
       <c r="D24" s="21">
         <v>1</v>
       </c>
-      <c r="E24" s="58" t="s">
+      <c r="E24" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7249,16 +7326,16 @@
       <c r="A25" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="49">
+      <c r="B25" s="51">
         <v>45986</v>
       </c>
-      <c r="C25" s="49">
+      <c r="C25" s="51">
         <v>45987</v>
       </c>
       <c r="D25" s="21">
         <v>1</v>
       </c>
-      <c r="E25" s="58" t="s">
+      <c r="E25" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7266,16 +7343,16 @@
       <c r="A26" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="49">
+      <c r="B26" s="51">
         <v>45986</v>
       </c>
-      <c r="C26" s="49">
+      <c r="C26" s="51">
         <v>45987</v>
       </c>
       <c r="D26" s="21">
         <v>1</v>
       </c>
-      <c r="E26" s="58" t="s">
+      <c r="E26" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7283,16 +7360,16 @@
       <c r="A27" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="49">
+      <c r="B27" s="51">
         <v>45986</v>
       </c>
-      <c r="C27" s="49">
+      <c r="C27" s="51">
         <v>45987</v>
       </c>
       <c r="D27" s="21">
         <v>1</v>
       </c>
-      <c r="E27" s="58" t="s">
+      <c r="E27" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7300,16 +7377,16 @@
       <c r="A28" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="49">
+      <c r="B28" s="51">
         <v>45986</v>
       </c>
-      <c r="C28" s="49">
+      <c r="C28" s="51">
         <v>45987</v>
       </c>
       <c r="D28" s="21">
         <v>1</v>
       </c>
-      <c r="E28" s="58" t="s">
+      <c r="E28" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7317,16 +7394,16 @@
       <c r="A29" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="49">
+      <c r="B29" s="51">
         <v>45986</v>
       </c>
-      <c r="C29" s="49">
+      <c r="C29" s="51">
         <v>45987</v>
       </c>
       <c r="D29" s="21">
         <v>1</v>
       </c>
-      <c r="E29" s="58" t="s">
+      <c r="E29" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7334,16 +7411,16 @@
       <c r="A30" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="49">
+      <c r="B30" s="51">
         <v>45986</v>
       </c>
-      <c r="C30" s="49">
+      <c r="C30" s="51">
         <v>45987</v>
       </c>
       <c r="D30" s="21">
         <v>1</v>
       </c>
-      <c r="E30" s="58" t="s">
+      <c r="E30" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7351,16 +7428,16 @@
       <c r="A31" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="49">
+      <c r="B31" s="51">
         <v>45992</v>
       </c>
-      <c r="C31" s="49">
+      <c r="C31" s="51">
         <v>45993</v>
       </c>
       <c r="D31" s="21">
         <v>1</v>
       </c>
-      <c r="E31" s="58" t="s">
+      <c r="E31" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7368,16 +7445,16 @@
       <c r="A32" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="49">
+      <c r="B32" s="51">
         <v>45992</v>
       </c>
-      <c r="C32" s="49">
+      <c r="C32" s="51">
         <v>45993</v>
       </c>
       <c r="D32" s="21">
         <v>1</v>
       </c>
-      <c r="E32" s="58" t="s">
+      <c r="E32" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7385,16 +7462,16 @@
       <c r="A33" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="49">
+      <c r="B33" s="51">
         <v>45992</v>
       </c>
-      <c r="C33" s="49">
+      <c r="C33" s="51">
         <v>45993</v>
       </c>
       <c r="D33" s="21">
         <v>1</v>
       </c>
-      <c r="E33" s="58" t="s">
+      <c r="E33" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7402,16 +7479,16 @@
       <c r="A34" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="49">
+      <c r="B34" s="51">
         <v>45993</v>
       </c>
-      <c r="C34" s="49">
+      <c r="C34" s="51">
         <v>45993</v>
       </c>
       <c r="D34" s="21">
         <v>1</v>
       </c>
-      <c r="E34" s="58" t="s">
+      <c r="E34" s="60" t="s">
         <v>35</v>
       </c>
     </row>
@@ -8030,21 +8107,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="45" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" ht="409.5" spans="1:3">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="47" t="s">
         <v>64</v>
       </c>
       <c r="C2" s="28" t="s">
@@ -8351,7 +8428,7 @@
       <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="38">
+      <c r="A2" s="40">
         <v>45962</v>
       </c>
       <c r="B2" s="27"/>
@@ -8360,7 +8437,7 @@
       <c r="A3" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="41" t="s">
         <v>74</v>
       </c>
     </row>
@@ -8368,7 +8445,7 @@
       <c r="A4" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="41" t="s">
         <v>76</v>
       </c>
     </row>
@@ -8376,21 +8453,21 @@
       <c r="A5" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="41" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="40">
+      <c r="A6" s="42">
         <v>45969</v>
       </c>
       <c r="B6" s="27"/>
     </row>
-    <row r="7" s="37" customFormat="1" ht="57.6" spans="1:2">
-      <c r="A7" s="41" t="s">
+    <row r="7" s="39" customFormat="1" ht="57.6" spans="1:2">
+      <c r="A7" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="44" t="s">
         <v>80</v>
       </c>
     </row>
@@ -8405,8 +8482,8 @@
   <sheetPr/>
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A37"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -8799,19 +8876,31 @@
       </c>
       <c r="C37" s="36"/>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="21"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="27"/>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="21"/>
-      <c r="B39" s="21"/>
+    <row r="38" ht="288" spans="1:3">
+      <c r="A38" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="C38" s="37"/>
+    </row>
+    <row r="39" ht="216" spans="1:3">
+      <c r="A39" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>175</v>
+      </c>
       <c r="C39" s="27"/>
     </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="21"/>
-      <c r="B40" s="21"/>
+    <row r="40" ht="100.8" spans="1:3">
+      <c r="A40" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>177</v>
+      </c>
       <c r="C40" s="27"/>
     </row>
     <row r="41" spans="1:3">
@@ -8875,8 +8964,8 @@
       <c r="C52" s="27"/>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="36"/>
-      <c r="B53" s="36"/>
+      <c r="A53" s="38"/>
+      <c r="B53" s="38"/>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="21"/>
@@ -8984,7 +9073,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C36:C38"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -9091,7 +9180,7 @@
         <v>38</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -9101,12 +9190,12 @@
     </row>
     <row r="19" ht="72" spans="1:1">
       <c r="A19" s="8" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" ht="72" spans="1:1">
       <c r="A20" s="8" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -9128,17 +9217,17 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" s="20" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -9167,302 +9256,302 @@
   <sheetData>
     <row r="1" spans="2:3">
       <c r="B1" s="14" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="2:3">
       <c r="B2" s="15" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="15" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="15" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" s="15" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="2:3">
       <c r="B6" s="15" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="15" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" ht="43.2" spans="2:3">
       <c r="B8" s="15" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" s="16" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" ht="23.4" spans="2:2">
       <c r="B11" s="17" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="2:2">
       <c r="B12" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" s="18" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" s="18" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="2:2">
       <c r="B16" s="18" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="18" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="18" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="18" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="18" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" s="18" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" s="18" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" s="18" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26" ht="23.4" spans="2:2">
       <c r="B26" s="17" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" s="18" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" s="18" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" s="18" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" s="18" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" s="18" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" s="18" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="18" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" s="18" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" s="18" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" s="18" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" s="18" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row r="40" spans="2:2">
       <c r="B40" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
     </row>
     <row r="41" ht="23.4" spans="2:2">
       <c r="B41" s="17" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="42" spans="2:2">
       <c r="B42" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
     </row>
     <row r="43" spans="2:2">
       <c r="B43" s="18" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
     </row>
     <row r="44" spans="2:2">
       <c r="B44" s="18" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
     </row>
     <row r="45" spans="2:2">
       <c r="B45" s="18" t="s">
-        <v>225</v>
+        <v>231</v>
       </c>
     </row>
     <row r="46" spans="2:2">
       <c r="B46" s="18" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
     </row>
     <row r="47" spans="2:2">
       <c r="B47" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
     </row>
     <row r="48" spans="2:2">
       <c r="B48" s="19" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
     </row>
     <row r="49" spans="2:2">
       <c r="B49" s="19" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50" s="19" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
     </row>
     <row r="51" spans="2:2">
       <c r="B51" s="19" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
     </row>
     <row r="52" spans="2:2">
       <c r="B52" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" ht="13" customHeight="1"/>
     <row r="55" ht="22" customHeight="1" spans="2:2">
       <c r="B55" s="17" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
     </row>
     <row r="56" spans="2:2">
       <c r="B56" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
     </row>
     <row r="57" spans="2:2">
       <c r="B57" s="18" t="s">
-        <v>235</v>
+        <v>241</v>
       </c>
     </row>
     <row r="58" spans="2:2">
@@ -9477,17 +9566,17 @@
     </row>
     <row r="60" spans="2:2">
       <c r="B60" s="18" t="s">
-        <v>236</v>
+        <v>242</v>
       </c>
     </row>
     <row r="61" spans="2:2">
       <c r="B61" s="18" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
     </row>
     <row r="62" spans="2:2">
       <c r="B62" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -9509,7 +9598,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="10" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -9524,7 +9613,7 @@
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
       <c r="N1" s="12" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="O1" s="13"/>
       <c r="P1" s="13"/>
@@ -9766,7 +9855,7 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="10" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -9952,7 +10041,7 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="11" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>

</xml_diff>

<commit_message>
13-12-25 updated with questions
</commit_message>
<xml_diff>
--- a/JavaPrograms/Work Done.xlsx
+++ b/JavaPrograms/Work Done.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" firstSheet="3" activeTab="10"/>
+    <workbookView windowWidth="23040" windowHeight="8280" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="DSA plan" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="375">
   <si>
     <r>
       <rPr>
@@ -2575,6 +2575,77 @@
 4️⃣ Median of Two Sorted Arrays (pivot logic thinking)</t>
   </si>
   <si>
+    <t>Binary Search Applications</t>
+  </si>
+  <si>
+    <t>First / Last Occurrence
+Search in Rotated Sorted Array
+Square ≥ N (Binary Search Answer)
+Koko Eating Bananas
+Split Array Largest Sum (410)
+Capacity to Ship Packages (1011)
+Median of Two Sorted Arrays (4)</t>
+  </si>
+  <si>
+    <t>Time-Based Indexing</t>
+  </si>
+  <si>
+    <t>TimeMap (981)</t>
+  </si>
+  <si>
+    <t>QuickSelect &amp; Rank Problems</t>
+  </si>
+  <si>
+    <t>Kth Largest
+Kth Smallest
+Top K Largest
+Top K Smallest</t>
+  </si>
+  <si>
+    <t>QuickSort Variants</t>
+  </si>
+  <si>
+    <t>QuickSort Lomuto
+QuickSort Hoare
+QuickSort DNF
+QuickSort Random Pivot
+QuickSort Median-of-Three</t>
+  </si>
+  <si>
+    <t>Binary Tree Fundamentals</t>
+  </si>
+  <si>
+    <t>Maximum Depth (104)
+Balanced Binary Tree (110)
+Level Order Traversal (102)
+Right Side View (199)
+Zigzag Level Order (103)
+Bottom-Up Level Order (107)</t>
+  </si>
+  <si>
+    <t>Path Problems</t>
+  </si>
+  <si>
+    <t>Path Sum (112)
+Path Sum II (113)
+Binary Tree Paths (257)</t>
+  </si>
+  <si>
+    <t>Tree Transformations</t>
+  </si>
+  <si>
+    <t>Symmetric Tree (101)
+Invert Binary Tree (226)</t>
+  </si>
+  <si>
+    <t>Traversals</t>
+  </si>
+  <si>
+    <t>Preorder
+Inorder
+Postorder</t>
+  </si>
+  <si>
     <t>https://www.notion.so/DSA-PATTERN-ROADMAP-2a285e32939580ff8596d7c9fbb7e0b3</t>
   </si>
   <si>
@@ -3593,9 +3664,6 @@
   </si>
   <si>
     <t>Divide + merge → O(n log n)</t>
-  </si>
-  <si>
-    <t>QuickSort Variants</t>
   </si>
   <si>
     <t>pick pivot</t>
@@ -4634,7 +4702,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4712,6 +4780,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5461,780 +5535,780 @@
   </cols>
   <sheetData>
     <row r="1" ht="90" customHeight="1" spans="1:6">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="64" t="s">
+      <c r="B1" s="65"/>
+      <c r="C1" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="66" t="s">
+      <c r="D1" s="67"/>
+      <c r="E1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="66"/>
+      <c r="F1" s="68"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="69" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="23"/>
-      <c r="C2" s="68" t="s">
+      <c r="C2" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="69"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="23"/>
       <c r="B4" s="23"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="23"/>
       <c r="B5" s="23"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="23"/>
       <c r="B6" s="23"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="23"/>
       <c r="B7" s="23"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="69" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="25"/>
-      <c r="C9" s="74" t="s">
+      <c r="C9" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="75"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="25"/>
       <c r="B10" s="25"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="25"/>
       <c r="B11" s="25"/>
-      <c r="C11" s="76"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="66"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="25"/>
       <c r="B12" s="25"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="68"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="25"/>
       <c r="B13" s="25"/>
-      <c r="C13" s="76"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="25"/>
       <c r="B14" s="25"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="68"/>
     </row>
     <row r="15" ht="15" customHeight="1" spans="1:6">
       <c r="A15" s="25"/>
       <c r="B15" s="25"/>
-      <c r="C15" s="78"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="68"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="25"/>
       <c r="B16" s="25"/>
-      <c r="C16" s="80" t="s">
+      <c r="C16" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="81"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
+      <c r="D16" s="83"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="68"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="25"/>
       <c r="B17" s="25"/>
-      <c r="C17" s="82"/>
-      <c r="D17" s="83"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
+      <c r="C17" s="84"/>
+      <c r="D17" s="85"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="68"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="25"/>
       <c r="B18" s="25"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="83"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
+      <c r="C18" s="84"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="68"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="67" t="s">
+      <c r="A19" s="69" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="23"/>
-      <c r="C19" s="82"/>
-      <c r="D19" s="83"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="66"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="68"/>
+      <c r="F19" s="68"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="23"/>
       <c r="B20" s="23"/>
-      <c r="C20" s="82"/>
-      <c r="D20" s="83"/>
-      <c r="E20" s="66"/>
-      <c r="F20" s="66"/>
+      <c r="C20" s="84"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="68"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="23"/>
       <c r="B21" s="23"/>
-      <c r="C21" s="82"/>
-      <c r="D21" s="83"/>
-      <c r="E21" s="66"/>
-      <c r="F21" s="66"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="85"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="68"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="23"/>
       <c r="B22" s="23"/>
-      <c r="C22" s="82"/>
-      <c r="D22" s="83"/>
+      <c r="C22" s="84"/>
+      <c r="D22" s="85"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="23"/>
       <c r="B23" s="23"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="85"/>
+      <c r="C23" s="86"/>
+      <c r="D23" s="87"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="23"/>
       <c r="B24" s="23"/>
-      <c r="C24" s="86" t="s">
+      <c r="C24" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="87"/>
+      <c r="D24" s="89"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="23"/>
       <c r="B25" s="23"/>
-      <c r="C25" s="88"/>
-      <c r="D25" s="89"/>
+      <c r="C25" s="90"/>
+      <c r="D25" s="91"/>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="23"/>
       <c r="B26" s="23"/>
-      <c r="C26" s="88"/>
-      <c r="D26" s="89"/>
+      <c r="C26" s="90"/>
+      <c r="D26" s="91"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="23"/>
       <c r="B27" s="23"/>
-      <c r="C27" s="88"/>
-      <c r="D27" s="89"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="91"/>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="23"/>
       <c r="B28" s="23"/>
-      <c r="C28" s="90"/>
-      <c r="D28" s="91"/>
+      <c r="C28" s="92"/>
+      <c r="D28" s="93"/>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="23"/>
       <c r="B29" s="23"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="23"/>
       <c r="B30" s="23"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="67" t="s">
+      <c r="A31" s="69" t="s">
         <v>10</v>
       </c>
       <c r="B31" s="25"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="25"/>
       <c r="B32" s="25"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="25"/>
       <c r="B33" s="25"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="25"/>
       <c r="B34" s="25"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="25"/>
       <c r="B35" s="25"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="25"/>
       <c r="B36" s="25"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="28"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="25"/>
       <c r="B37" s="25"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="25"/>
       <c r="B38" s="25"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="25"/>
       <c r="B39" s="25"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
     </row>
     <row r="40" ht="18" customHeight="1" spans="1:4">
-      <c r="A40" s="67" t="s">
+      <c r="A40" s="69" t="s">
         <v>11</v>
       </c>
       <c r="B40" s="25"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="25"/>
       <c r="B41" s="25"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="25"/>
       <c r="B42" s="25"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="25"/>
       <c r="B43" s="25"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="25"/>
       <c r="B44" s="25"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="25"/>
       <c r="B45" s="25"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="25"/>
       <c r="B46" s="25"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="25"/>
       <c r="B47" s="25"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="28"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="25"/>
       <c r="B48" s="25"/>
-      <c r="C48" s="28"/>
-      <c r="D48" s="28"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="25"/>
       <c r="B49" s="25"/>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="30"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="67" t="s">
+      <c r="A50" s="69" t="s">
         <v>12</v>
       </c>
       <c r="B50" s="25"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="28"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="25"/>
       <c r="B51" s="25"/>
-      <c r="C51" s="28"/>
-      <c r="D51" s="28"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="30"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="25"/>
       <c r="B52" s="25"/>
-      <c r="C52" s="28"/>
-      <c r="D52" s="28"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="25"/>
       <c r="B53" s="25"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="30"/>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="25"/>
       <c r="B54" s="25"/>
-      <c r="C54" s="28"/>
-      <c r="D54" s="28"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="25"/>
       <c r="B55" s="25"/>
-      <c r="C55" s="28"/>
-      <c r="D55" s="28"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="30"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="25"/>
       <c r="B56" s="25"/>
-      <c r="C56" s="28"/>
-      <c r="D56" s="28"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="25"/>
       <c r="B57" s="25"/>
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
+      <c r="C57" s="30"/>
+      <c r="D57" s="30"/>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="25"/>
       <c r="B58" s="25"/>
-      <c r="C58" s="28"/>
-      <c r="D58" s="28"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="30"/>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="67" t="s">
+      <c r="A59" s="69" t="s">
         <v>13</v>
       </c>
       <c r="B59" s="23"/>
-      <c r="C59" s="28"/>
-      <c r="D59" s="28"/>
+      <c r="C59" s="30"/>
+      <c r="D59" s="30"/>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="23"/>
       <c r="B60" s="23"/>
-      <c r="C60" s="28"/>
-      <c r="D60" s="28"/>
+      <c r="C60" s="30"/>
+      <c r="D60" s="30"/>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="23"/>
       <c r="B61" s="23"/>
-      <c r="C61" s="28"/>
-      <c r="D61" s="28"/>
+      <c r="C61" s="30"/>
+      <c r="D61" s="30"/>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="23"/>
       <c r="B62" s="23"/>
-      <c r="C62" s="28"/>
-      <c r="D62" s="28"/>
+      <c r="C62" s="30"/>
+      <c r="D62" s="30"/>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="23"/>
       <c r="B63" s="23"/>
-      <c r="C63" s="28"/>
-      <c r="D63" s="28"/>
+      <c r="C63" s="30"/>
+      <c r="D63" s="30"/>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="23"/>
       <c r="B64" s="23"/>
-      <c r="C64" s="28"/>
-      <c r="D64" s="28"/>
+      <c r="C64" s="30"/>
+      <c r="D64" s="30"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="23"/>
       <c r="B65" s="23"/>
-      <c r="C65" s="28"/>
-      <c r="D65" s="28"/>
+      <c r="C65" s="30"/>
+      <c r="D65" s="30"/>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="23"/>
       <c r="B66" s="23"/>
-      <c r="C66" s="28"/>
-      <c r="D66" s="28"/>
+      <c r="C66" s="30"/>
+      <c r="D66" s="30"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="23"/>
       <c r="B67" s="23"/>
-      <c r="C67" s="28"/>
-      <c r="D67" s="28"/>
+      <c r="C67" s="30"/>
+      <c r="D67" s="30"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="67" t="s">
+      <c r="A68" s="69" t="s">
         <v>14</v>
       </c>
       <c r="B68" s="23"/>
-      <c r="C68" s="28"/>
-      <c r="D68" s="28"/>
+      <c r="C68" s="30"/>
+      <c r="D68" s="30"/>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="23"/>
       <c r="B69" s="23"/>
-      <c r="C69" s="28"/>
-      <c r="D69" s="28"/>
+      <c r="C69" s="30"/>
+      <c r="D69" s="30"/>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="23"/>
       <c r="B70" s="23"/>
-      <c r="C70" s="28"/>
-      <c r="D70" s="28"/>
+      <c r="C70" s="30"/>
+      <c r="D70" s="30"/>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="23"/>
       <c r="B71" s="23"/>
-      <c r="C71" s="28"/>
-      <c r="D71" s="28"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="30"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="23"/>
       <c r="B72" s="23"/>
-      <c r="C72" s="28"/>
-      <c r="D72" s="28"/>
+      <c r="C72" s="30"/>
+      <c r="D72" s="30"/>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="23"/>
       <c r="B73" s="23"/>
-      <c r="C73" s="28"/>
-      <c r="D73" s="28"/>
+      <c r="C73" s="30"/>
+      <c r="D73" s="30"/>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="23"/>
       <c r="B74" s="23"/>
-      <c r="C74" s="28"/>
-      <c r="D74" s="28"/>
+      <c r="C74" s="30"/>
+      <c r="D74" s="30"/>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="23"/>
       <c r="B75" s="23"/>
-      <c r="C75" s="28"/>
-      <c r="D75" s="28"/>
+      <c r="C75" s="30"/>
+      <c r="D75" s="30"/>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="23"/>
       <c r="B76" s="23"/>
-      <c r="C76" s="28"/>
-      <c r="D76" s="28"/>
+      <c r="C76" s="30"/>
+      <c r="D76" s="30"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="23"/>
       <c r="B77" s="23"/>
-      <c r="C77" s="28"/>
-      <c r="D77" s="28"/>
+      <c r="C77" s="30"/>
+      <c r="D77" s="30"/>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="67" t="s">
+      <c r="A78" s="69" t="s">
         <v>15</v>
       </c>
       <c r="B78" s="23"/>
-      <c r="C78" s="28"/>
-      <c r="D78" s="28"/>
+      <c r="C78" s="30"/>
+      <c r="D78" s="30"/>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="23"/>
       <c r="B79" s="23"/>
-      <c r="C79" s="28"/>
-      <c r="D79" s="28"/>
+      <c r="C79" s="30"/>
+      <c r="D79" s="30"/>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="23"/>
       <c r="B80" s="23"/>
-      <c r="C80" s="28"/>
-      <c r="D80" s="28"/>
+      <c r="C80" s="30"/>
+      <c r="D80" s="30"/>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="23"/>
       <c r="B81" s="23"/>
-      <c r="C81" s="28"/>
-      <c r="D81" s="28"/>
+      <c r="C81" s="30"/>
+      <c r="D81" s="30"/>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="23"/>
       <c r="B82" s="23"/>
-      <c r="C82" s="28"/>
-      <c r="D82" s="28"/>
+      <c r="C82" s="30"/>
+      <c r="D82" s="30"/>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="23"/>
       <c r="B83" s="23"/>
-      <c r="C83" s="28"/>
-      <c r="D83" s="28"/>
+      <c r="C83" s="30"/>
+      <c r="D83" s="30"/>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="23"/>
       <c r="B84" s="23"/>
-      <c r="C84" s="28"/>
-      <c r="D84" s="28"/>
+      <c r="C84" s="30"/>
+      <c r="D84" s="30"/>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="23"/>
       <c r="B85" s="23"/>
-      <c r="C85" s="28"/>
-      <c r="D85" s="28"/>
+      <c r="C85" s="30"/>
+      <c r="D85" s="30"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="23"/>
       <c r="B86" s="23"/>
-      <c r="C86" s="28"/>
-      <c r="D86" s="28"/>
+      <c r="C86" s="30"/>
+      <c r="D86" s="30"/>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="23"/>
       <c r="B87" s="23"/>
-      <c r="C87" s="28"/>
-      <c r="D87" s="28"/>
+      <c r="C87" s="30"/>
+      <c r="D87" s="30"/>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="67" t="s">
+      <c r="A88" s="69" t="s">
         <v>16</v>
       </c>
       <c r="B88" s="23"/>
-      <c r="C88" s="28"/>
-      <c r="D88" s="28"/>
+      <c r="C88" s="30"/>
+      <c r="D88" s="30"/>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="23"/>
       <c r="B89" s="23"/>
-      <c r="C89" s="28"/>
-      <c r="D89" s="28"/>
+      <c r="C89" s="30"/>
+      <c r="D89" s="30"/>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="23"/>
       <c r="B90" s="23"/>
-      <c r="C90" s="28"/>
-      <c r="D90" s="28"/>
+      <c r="C90" s="30"/>
+      <c r="D90" s="30"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="23"/>
       <c r="B91" s="23"/>
-      <c r="C91" s="28"/>
-      <c r="D91" s="28"/>
+      <c r="C91" s="30"/>
+      <c r="D91" s="30"/>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="23"/>
       <c r="B92" s="23"/>
-      <c r="C92" s="28"/>
-      <c r="D92" s="28"/>
+      <c r="C92" s="30"/>
+      <c r="D92" s="30"/>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="23"/>
       <c r="B93" s="23"/>
-      <c r="C93" s="28"/>
-      <c r="D93" s="28"/>
+      <c r="C93" s="30"/>
+      <c r="D93" s="30"/>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="23"/>
       <c r="B94" s="23"/>
-      <c r="C94" s="28"/>
-      <c r="D94" s="28"/>
+      <c r="C94" s="30"/>
+      <c r="D94" s="30"/>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="23"/>
       <c r="B95" s="23"/>
-      <c r="C95" s="28"/>
-      <c r="D95" s="28"/>
+      <c r="C95" s="30"/>
+      <c r="D95" s="30"/>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="23"/>
       <c r="B96" s="23"/>
-      <c r="C96" s="28"/>
-      <c r="D96" s="28"/>
+      <c r="C96" s="30"/>
+      <c r="D96" s="30"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="67" t="s">
+      <c r="A97" s="69" t="s">
         <v>17</v>
       </c>
       <c r="B97" s="25"/>
-      <c r="C97" s="28"/>
-      <c r="D97" s="28"/>
+      <c r="C97" s="30"/>
+      <c r="D97" s="30"/>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="25"/>
       <c r="B98" s="25"/>
-      <c r="C98" s="28"/>
-      <c r="D98" s="28"/>
+      <c r="C98" s="30"/>
+      <c r="D98" s="30"/>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="25"/>
       <c r="B99" s="25"/>
-      <c r="C99" s="28"/>
-      <c r="D99" s="28"/>
+      <c r="C99" s="30"/>
+      <c r="D99" s="30"/>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="25"/>
       <c r="B100" s="25"/>
-      <c r="C100" s="28"/>
-      <c r="D100" s="28"/>
+      <c r="C100" s="30"/>
+      <c r="D100" s="30"/>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="25"/>
       <c r="B101" s="25"/>
-      <c r="C101" s="28"/>
-      <c r="D101" s="28"/>
+      <c r="C101" s="30"/>
+      <c r="D101" s="30"/>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="25"/>
       <c r="B102" s="25"/>
-      <c r="C102" s="28"/>
-      <c r="D102" s="28"/>
+      <c r="C102" s="30"/>
+      <c r="D102" s="30"/>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="25"/>
       <c r="B103" s="25"/>
-      <c r="C103" s="28"/>
-      <c r="D103" s="28"/>
+      <c r="C103" s="30"/>
+      <c r="D103" s="30"/>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="25"/>
       <c r="B104" s="25"/>
-      <c r="C104" s="28"/>
-      <c r="D104" s="28"/>
+      <c r="C104" s="30"/>
+      <c r="D104" s="30"/>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="25"/>
       <c r="B105" s="25"/>
-      <c r="C105" s="28"/>
-      <c r="D105" s="28"/>
+      <c r="C105" s="30"/>
+      <c r="D105" s="30"/>
     </row>
     <row r="106" spans="1:4">
-      <c r="A106" s="67" t="s">
+      <c r="A106" s="69" t="s">
         <v>18</v>
       </c>
       <c r="B106" s="23"/>
-      <c r="C106" s="28"/>
-      <c r="D106" s="28"/>
+      <c r="C106" s="30"/>
+      <c r="D106" s="30"/>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="23"/>
       <c r="B107" s="23"/>
-      <c r="C107" s="28"/>
-      <c r="D107" s="28"/>
+      <c r="C107" s="30"/>
+      <c r="D107" s="30"/>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="23"/>
       <c r="B108" s="23"/>
-      <c r="C108" s="28"/>
-      <c r="D108" s="28"/>
+      <c r="C108" s="30"/>
+      <c r="D108" s="30"/>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="23"/>
       <c r="B109" s="23"/>
-      <c r="C109" s="28"/>
-      <c r="D109" s="28"/>
+      <c r="C109" s="30"/>
+      <c r="D109" s="30"/>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="23"/>
       <c r="B110" s="23"/>
-      <c r="C110" s="28"/>
-      <c r="D110" s="28"/>
+      <c r="C110" s="30"/>
+      <c r="D110" s="30"/>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="23"/>
       <c r="B111" s="23"/>
-      <c r="C111" s="28"/>
-      <c r="D111" s="28"/>
+      <c r="C111" s="30"/>
+      <c r="D111" s="30"/>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="23"/>
       <c r="B112" s="23"/>
-      <c r="C112" s="28"/>
-      <c r="D112" s="28"/>
+      <c r="C112" s="30"/>
+      <c r="D112" s="30"/>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="23"/>
       <c r="B113" s="23"/>
-      <c r="C113" s="28"/>
-      <c r="D113" s="28"/>
+      <c r="C113" s="30"/>
+      <c r="D113" s="30"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="23"/>
       <c r="B114" s="23"/>
-      <c r="C114" s="28"/>
-      <c r="D114" s="28"/>
+      <c r="C114" s="30"/>
+      <c r="D114" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="19">
@@ -6280,10 +6354,10 @@
   <sheetData>
     <row r="1" ht="409" customHeight="1" spans="1:2">
       <c r="A1" s="7" t="s">
-        <v>250</v>
+        <v>266</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>251</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -6413,7 +6487,7 @@
   <sheetPr/>
   <dimension ref="A1:C223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -6434,18 +6508,18 @@
     </row>
     <row r="2" ht="409.5" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>254</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" ht="409.5" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>255</v>
+        <v>271</v>
       </c>
       <c r="C3"/>
     </row>
@@ -6494,32 +6568,32 @@
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="1" t="s">
-        <v>256</v>
+        <v>272</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="1" t="s">
-        <v>257</v>
+        <v>273</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="1" t="s">
-        <v>258</v>
+        <v>274</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="10" t="s">
-        <v>259</v>
+        <v>275</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="1" t="s">
-        <v>261</v>
+        <v>277</v>
       </c>
     </row>
     <row r="36" ht="23.4" spans="1:1">
@@ -6527,177 +6601,177 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="1" t="s">
-        <v>263</v>
+        <v>279</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="1" t="s">
-        <v>264</v>
+        <v>280</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="1" t="s">
-        <v>265</v>
+        <v>281</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="1" t="s">
-        <v>266</v>
+        <v>282</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="1" t="s">
-        <v>267</v>
+        <v>283</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="1" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="1" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="1" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="1" t="s">
-        <v>271</v>
+        <v>287</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="10" t="s">
-        <v>272</v>
+        <v>288</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="1" t="s">
-        <v>273</v>
+        <v>289</v>
       </c>
     </row>
     <row r="60" ht="23.4" spans="1:1">
       <c r="A60" s="9" t="s">
-        <v>274</v>
+        <v>290</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="1" t="s">
-        <v>275</v>
+        <v>291</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="1" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="1" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="1" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="1" t="s">
-        <v>279</v>
+        <v>295</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="1" t="s">
-        <v>280</v>
+        <v>296</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="1" t="s">
-        <v>281</v>
+        <v>297</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="1" t="s">
-        <v>282</v>
+        <v>298</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="1" t="s">
-        <v>283</v>
+        <v>299</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="1" t="s">
-        <v>284</v>
+        <v>300</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="10" t="s">
-        <v>285</v>
+        <v>301</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="1" t="s">
-        <v>286</v>
+        <v>302</v>
       </c>
     </row>
     <row r="86" ht="23.4" spans="1:1">
       <c r="A86" s="9" t="s">
-        <v>287</v>
+        <v>303</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="1" t="s">
-        <v>288</v>
+        <v>304</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="1" t="s">
-        <v>289</v>
+        <v>305</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="1" t="s">
-        <v>290</v>
+        <v>306</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="1" t="s">
-        <v>291</v>
+        <v>307</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" s="1" t="s">
-        <v>292</v>
+        <v>308</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" s="1" t="s">
-        <v>293</v>
+        <v>309</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="1" t="s">
-        <v>294</v>
+        <v>310</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" s="1" t="s">
-        <v>295</v>
+        <v>311</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="1" t="s">
-        <v>296</v>
+        <v>312</v>
       </c>
     </row>
     <row r="103" spans="1:1">
@@ -6707,12 +6781,12 @@
     </row>
     <row r="105" spans="1:1">
       <c r="A105" s="1" t="s">
-        <v>297</v>
+        <v>313</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" s="1" t="s">
-        <v>298</v>
+        <v>188</v>
       </c>
     </row>
     <row r="108" spans="1:1">
@@ -6720,12 +6794,12 @@
     </row>
     <row r="109" spans="1:1">
       <c r="A109" s="1" t="s">
-        <v>299</v>
+        <v>314</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" s="1" t="s">
-        <v>300</v>
+        <v>315</v>
       </c>
     </row>
     <row r="112" ht="23.4" spans="1:1">
@@ -6733,42 +6807,42 @@
     </row>
     <row r="113" spans="1:1">
       <c r="A113" s="1" t="s">
-        <v>301</v>
+        <v>316</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" s="1" t="s">
-        <v>302</v>
+        <v>317</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" s="1" t="s">
-        <v>303</v>
+        <v>318</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" s="1" t="s">
-        <v>304</v>
+        <v>319</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" s="1" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" s="1" t="s">
-        <v>306</v>
+        <v>321</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" s="1" t="s">
-        <v>307</v>
+        <v>322</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" s="1" t="s">
-        <v>308</v>
+        <v>323</v>
       </c>
     </row>
     <row r="128" spans="1:1">
@@ -6776,12 +6850,12 @@
     </row>
     <row r="129" spans="1:1">
       <c r="A129" s="1" t="s">
-        <v>309</v>
+        <v>324</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" s="1" t="s">
-        <v>310</v>
+        <v>325</v>
       </c>
     </row>
     <row r="132" ht="23.4" spans="1:1">
@@ -6789,62 +6863,62 @@
     </row>
     <row r="133" spans="1:1">
       <c r="A133" s="1" t="s">
-        <v>311</v>
+        <v>326</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" s="1" t="s">
-        <v>312</v>
+        <v>327</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" s="1" t="s">
-        <v>314</v>
+        <v>329</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" s="1" t="s">
-        <v>315</v>
+        <v>330</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" s="1" t="s">
-        <v>316</v>
+        <v>331</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" s="1" t="s">
-        <v>317</v>
+        <v>332</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" s="1" t="s">
-        <v>318</v>
+        <v>333</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" s="1" t="s">
-        <v>319</v>
+        <v>334</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" s="10" t="s">
-        <v>320</v>
+        <v>335</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" s="1" t="s">
-        <v>321</v>
+        <v>336</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" s="1" t="s">
-        <v>322</v>
+        <v>337</v>
       </c>
     </row>
     <row r="154" ht="23.4" spans="1:1">
@@ -6852,62 +6926,62 @@
     </row>
     <row r="156" spans="1:1">
       <c r="A156" s="1" t="s">
-        <v>323</v>
+        <v>338</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" s="1" t="s">
-        <v>324</v>
+        <v>339</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" s="1" t="s">
-        <v>325</v>
+        <v>340</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" s="1" t="s">
-        <v>326</v>
+        <v>341</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" s="1" t="s">
-        <v>327</v>
+        <v>342</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" s="1" t="s">
-        <v>328</v>
+        <v>343</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" s="1" t="s">
-        <v>329</v>
+        <v>344</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" s="1" t="s">
-        <v>330</v>
+        <v>345</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" s="1" t="s">
-        <v>331</v>
+        <v>346</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" s="10" t="s">
-        <v>332</v>
+        <v>347</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" s="1" t="s">
-        <v>333</v>
+        <v>348</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" s="1" t="s">
-        <v>334</v>
+        <v>349</v>
       </c>
     </row>
     <row r="180" spans="1:1">
@@ -6917,7 +6991,7 @@
     </row>
     <row r="182" spans="1:1">
       <c r="A182" s="1" t="s">
-        <v>335</v>
+        <v>350</v>
       </c>
     </row>
     <row r="184" spans="1:1">
@@ -6927,122 +7001,122 @@
     </row>
     <row r="186" spans="1:1">
       <c r="A186" s="1" t="s">
-        <v>336</v>
+        <v>351</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" s="1" t="s">
-        <v>337</v>
+        <v>352</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" s="1" t="s">
-        <v>338</v>
+        <v>353</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" s="1" t="s">
-        <v>339</v>
+        <v>354</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" s="1" t="s">
-        <v>340</v>
+        <v>355</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" s="1" t="s">
-        <v>341</v>
+        <v>356</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" s="1" t="s">
-        <v>342</v>
+        <v>357</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" s="1" t="s">
-        <v>343</v>
+        <v>358</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" s="1" t="s">
-        <v>344</v>
+        <v>359</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" s="1" t="s">
-        <v>345</v>
+        <v>360</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" s="1" t="s">
-        <v>346</v>
+        <v>361</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" s="1" t="s">
-        <v>347</v>
+        <v>362</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" s="1" t="s">
-        <v>348</v>
+        <v>363</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" s="1" t="s">
-        <v>349</v>
+        <v>364</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" s="1" t="s">
-        <v>350</v>
+        <v>365</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" s="1" t="s">
-        <v>351</v>
+        <v>366</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" s="1" t="s">
-        <v>352</v>
+        <v>367</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" s="1" t="s">
-        <v>353</v>
+        <v>368</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" s="1" t="s">
-        <v>354</v>
+        <v>369</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" s="1" t="s">
-        <v>355</v>
+        <v>370</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" s="1" t="s">
-        <v>356</v>
+        <v>371</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" s="1" t="s">
-        <v>357</v>
+        <v>372</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" s="1" t="s">
-        <v>358</v>
+        <v>373</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" s="1" t="s">
-        <v>359</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -7070,19 +7144,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="52" t="s">
         <v>23</v>
       </c>
     </row>
@@ -7090,31 +7164,31 @@
       <c r="A2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="51">
+      <c r="B2" s="53">
         <v>45976</v>
       </c>
-      <c r="C2" s="52">
+      <c r="C2" s="54">
         <v>45983</v>
       </c>
       <c r="D2" s="23">
         <v>4</v>
       </c>
-      <c r="E2" s="53"/>
+      <c r="E2" s="55"/>
     </row>
     <row r="3" ht="115.2" spans="1:5">
       <c r="A3" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="51">
+      <c r="B3" s="53">
         <v>45976</v>
       </c>
-      <c r="C3" s="52">
+      <c r="C3" s="54">
         <v>45983</v>
       </c>
       <c r="D3" s="23">
         <v>4</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="56" t="s">
         <v>26</v>
       </c>
     </row>
@@ -7122,16 +7196,16 @@
       <c r="A4" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="51">
+      <c r="B4" s="53">
         <v>45976</v>
       </c>
-      <c r="C4" s="52">
+      <c r="C4" s="54">
         <v>45983</v>
       </c>
       <c r="D4" s="23">
         <v>3</v>
       </c>
-      <c r="E4" s="55" t="s">
+      <c r="E4" s="57" t="s">
         <v>28</v>
       </c>
     </row>
@@ -7139,125 +7213,125 @@
       <c r="A5" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="51">
+      <c r="B5" s="53">
         <v>45976</v>
       </c>
-      <c r="C5" s="52">
+      <c r="C5" s="54">
         <v>45983</v>
       </c>
       <c r="D5" s="23">
         <v>2</v>
       </c>
-      <c r="E5" s="56"/>
+      <c r="E5" s="58"/>
     </row>
     <row r="6" ht="115.2" spans="1:5">
       <c r="A6" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="51">
+      <c r="B6" s="53">
         <v>45976</v>
       </c>
-      <c r="C6" s="52">
+      <c r="C6" s="54">
         <v>45983</v>
       </c>
       <c r="D6" s="23">
         <v>2</v>
       </c>
-      <c r="E6" s="56"/>
+      <c r="E6" s="58"/>
     </row>
     <row r="7" ht="129.6" spans="1:5">
       <c r="A7" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="51">
+      <c r="B7" s="53">
         <v>45976</v>
       </c>
-      <c r="C7" s="52">
+      <c r="C7" s="54">
         <v>45983</v>
       </c>
       <c r="D7" s="23">
         <v>2</v>
       </c>
-      <c r="E7" s="56"/>
-    </row>
-    <row r="8" s="49" customFormat="1" ht="144" spans="1:5">
-      <c r="A8" s="57" t="s">
+      <c r="E7" s="58"/>
+    </row>
+    <row r="8" s="51" customFormat="1" ht="144" spans="1:5">
+      <c r="A8" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="52">
+      <c r="B8" s="54">
         <v>45976</v>
       </c>
-      <c r="C8" s="52">
+      <c r="C8" s="54">
         <v>45983</v>
       </c>
-      <c r="D8" s="58">
+      <c r="D8" s="60">
         <v>2</v>
       </c>
-      <c r="E8" s="59"/>
-    </row>
-    <row r="9" s="49" customFormat="1" ht="158.4" spans="1:5">
-      <c r="A9" s="57" t="s">
+      <c r="E8" s="61"/>
+    </row>
+    <row r="9" s="51" customFormat="1" ht="158.4" spans="1:5">
+      <c r="A9" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="52">
+      <c r="B9" s="54">
         <v>45976</v>
       </c>
-      <c r="C9" s="52">
+      <c r="C9" s="54">
         <v>45983</v>
       </c>
-      <c r="D9" s="58">
+      <c r="D9" s="60">
         <v>1</v>
       </c>
-      <c r="E9" s="60"/>
-    </row>
-    <row r="10" s="49" customFormat="1" spans="1:5">
-      <c r="A10" s="58" t="s">
+      <c r="E9" s="62"/>
+    </row>
+    <row r="10" s="51" customFormat="1" spans="1:5">
+      <c r="A10" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="52">
+      <c r="B10" s="54">
         <v>45976</v>
       </c>
-      <c r="C10" s="52">
+      <c r="C10" s="54">
         <v>45983</v>
       </c>
-      <c r="D10" s="58">
+      <c r="D10" s="60">
         <v>1</v>
       </c>
-      <c r="E10" s="61" t="s">
+      <c r="E10" s="63" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" s="49" customFormat="1" spans="1:5">
-      <c r="A11" s="58" t="s">
+    <row r="11" s="51" customFormat="1" spans="1:5">
+      <c r="A11" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="52">
+      <c r="B11" s="54">
         <v>45976</v>
       </c>
-      <c r="C11" s="52">
+      <c r="C11" s="54">
         <v>45983</v>
       </c>
-      <c r="D11" s="58">
+      <c r="D11" s="60">
         <v>1</v>
       </c>
-      <c r="E11" s="61" t="s">
+      <c r="E11" s="63" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" s="49" customFormat="1" spans="1:5">
-      <c r="A12" s="58" t="s">
+    <row r="12" s="51" customFormat="1" spans="1:5">
+      <c r="A12" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="52">
+      <c r="B12" s="54">
         <v>45976</v>
       </c>
-      <c r="C12" s="52">
+      <c r="C12" s="54">
         <v>45983</v>
       </c>
-      <c r="D12" s="58">
+      <c r="D12" s="60">
         <v>1</v>
       </c>
-      <c r="E12" s="61" t="s">
+      <c r="E12" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7265,16 +7339,16 @@
       <c r="A13" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="52">
+      <c r="B13" s="54">
         <v>45977</v>
       </c>
-      <c r="C13" s="52">
+      <c r="C13" s="54">
         <v>45982</v>
       </c>
       <c r="D13" s="23">
         <v>1</v>
       </c>
-      <c r="E13" s="61" t="s">
+      <c r="E13" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7282,16 +7356,16 @@
       <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="52">
+      <c r="B14" s="54">
         <v>45980</v>
       </c>
-      <c r="C14" s="52">
+      <c r="C14" s="54">
         <v>45982</v>
       </c>
       <c r="D14" s="23">
         <v>1</v>
       </c>
-      <c r="E14" s="61" t="s">
+      <c r="E14" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7299,16 +7373,16 @@
       <c r="A15" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="52">
+      <c r="B15" s="54">
         <v>45980</v>
       </c>
-      <c r="C15" s="52">
+      <c r="C15" s="54">
         <v>45982</v>
       </c>
       <c r="D15" s="23">
         <v>1</v>
       </c>
-      <c r="E15" s="61" t="s">
+      <c r="E15" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7316,16 +7390,16 @@
       <c r="A16" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="52">
+      <c r="B16" s="54">
         <v>45980</v>
       </c>
-      <c r="C16" s="52">
+      <c r="C16" s="54">
         <v>45982</v>
       </c>
       <c r="D16" s="23">
         <v>1</v>
       </c>
-      <c r="E16" s="61" t="s">
+      <c r="E16" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7333,16 +7407,16 @@
       <c r="A17" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="52">
+      <c r="B17" s="54">
         <v>45980</v>
       </c>
-      <c r="C17" s="52">
+      <c r="C17" s="54">
         <v>45982</v>
       </c>
       <c r="D17" s="23">
         <v>1</v>
       </c>
-      <c r="E17" s="61" t="s">
+      <c r="E17" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7350,16 +7424,16 @@
       <c r="A18" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="52">
+      <c r="B18" s="54">
         <v>45981</v>
       </c>
-      <c r="C18" s="52">
+      <c r="C18" s="54">
         <v>45983</v>
       </c>
       <c r="D18" s="23">
         <v>1</v>
       </c>
-      <c r="E18" s="61" t="s">
+      <c r="E18" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7367,16 +7441,16 @@
       <c r="A19" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="52">
+      <c r="B19" s="54">
         <v>45982</v>
       </c>
-      <c r="C19" s="52">
+      <c r="C19" s="54">
         <v>45984</v>
       </c>
       <c r="D19" s="23">
         <v>1</v>
       </c>
-      <c r="E19" s="61" t="s">
+      <c r="E19" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7384,16 +7458,16 @@
       <c r="A20" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="52">
+      <c r="B20" s="54">
         <v>45983</v>
       </c>
-      <c r="C20" s="52">
+      <c r="C20" s="54">
         <v>45985</v>
       </c>
       <c r="D20" s="23">
         <v>1</v>
       </c>
-      <c r="E20" s="61" t="s">
+      <c r="E20" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7401,16 +7475,16 @@
       <c r="A21" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="52">
+      <c r="B21" s="54">
         <v>45986</v>
       </c>
-      <c r="C21" s="52">
+      <c r="C21" s="54">
         <v>45987</v>
       </c>
       <c r="D21" s="23">
         <v>1</v>
       </c>
-      <c r="E21" s="61" t="s">
+      <c r="E21" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7418,16 +7492,16 @@
       <c r="A22" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="52">
+      <c r="B22" s="54">
         <v>45986</v>
       </c>
-      <c r="C22" s="52">
+      <c r="C22" s="54">
         <v>45987</v>
       </c>
       <c r="D22" s="23">
         <v>1</v>
       </c>
-      <c r="E22" s="61" t="s">
+      <c r="E22" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7435,16 +7509,16 @@
       <c r="A23" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="52">
+      <c r="B23" s="54">
         <v>45986</v>
       </c>
-      <c r="C23" s="52">
+      <c r="C23" s="54">
         <v>45987</v>
       </c>
       <c r="D23" s="23">
         <v>1</v>
       </c>
-      <c r="E23" s="61" t="s">
+      <c r="E23" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7452,16 +7526,16 @@
       <c r="A24" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="52">
+      <c r="B24" s="54">
         <v>45986</v>
       </c>
-      <c r="C24" s="52">
+      <c r="C24" s="54">
         <v>45987</v>
       </c>
       <c r="D24" s="23">
         <v>1</v>
       </c>
-      <c r="E24" s="61" t="s">
+      <c r="E24" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7469,16 +7543,16 @@
       <c r="A25" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="52">
+      <c r="B25" s="54">
         <v>45986</v>
       </c>
-      <c r="C25" s="52">
+      <c r="C25" s="54">
         <v>45987</v>
       </c>
       <c r="D25" s="23">
         <v>1</v>
       </c>
-      <c r="E25" s="61" t="s">
+      <c r="E25" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7486,16 +7560,16 @@
       <c r="A26" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="52">
+      <c r="B26" s="54">
         <v>45986</v>
       </c>
-      <c r="C26" s="52">
+      <c r="C26" s="54">
         <v>45987</v>
       </c>
       <c r="D26" s="23">
         <v>1</v>
       </c>
-      <c r="E26" s="61" t="s">
+      <c r="E26" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7503,16 +7577,16 @@
       <c r="A27" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="52">
+      <c r="B27" s="54">
         <v>45986</v>
       </c>
-      <c r="C27" s="52">
+      <c r="C27" s="54">
         <v>45987</v>
       </c>
       <c r="D27" s="23">
         <v>1</v>
       </c>
-      <c r="E27" s="61" t="s">
+      <c r="E27" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7520,16 +7594,16 @@
       <c r="A28" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="52">
+      <c r="B28" s="54">
         <v>45986</v>
       </c>
-      <c r="C28" s="52">
+      <c r="C28" s="54">
         <v>45987</v>
       </c>
       <c r="D28" s="23">
         <v>1</v>
       </c>
-      <c r="E28" s="61" t="s">
+      <c r="E28" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7537,16 +7611,16 @@
       <c r="A29" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="52">
+      <c r="B29" s="54">
         <v>45986</v>
       </c>
-      <c r="C29" s="52">
+      <c r="C29" s="54">
         <v>45987</v>
       </c>
       <c r="D29" s="23">
         <v>1</v>
       </c>
-      <c r="E29" s="61" t="s">
+      <c r="E29" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7554,16 +7628,16 @@
       <c r="A30" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="52">
+      <c r="B30" s="54">
         <v>45986</v>
       </c>
-      <c r="C30" s="52">
+      <c r="C30" s="54">
         <v>45987</v>
       </c>
       <c r="D30" s="23">
         <v>1</v>
       </c>
-      <c r="E30" s="61" t="s">
+      <c r="E30" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7571,16 +7645,16 @@
       <c r="A31" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="52">
+      <c r="B31" s="54">
         <v>45992</v>
       </c>
-      <c r="C31" s="52">
+      <c r="C31" s="54">
         <v>45993</v>
       </c>
       <c r="D31" s="23">
         <v>1</v>
       </c>
-      <c r="E31" s="61" t="s">
+      <c r="E31" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7588,16 +7662,16 @@
       <c r="A32" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="52">
+      <c r="B32" s="54">
         <v>45992</v>
       </c>
-      <c r="C32" s="52">
+      <c r="C32" s="54">
         <v>45993</v>
       </c>
       <c r="D32" s="23">
         <v>1</v>
       </c>
-      <c r="E32" s="61" t="s">
+      <c r="E32" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7605,16 +7679,16 @@
       <c r="A33" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="52">
+      <c r="B33" s="54">
         <v>45992</v>
       </c>
-      <c r="C33" s="52">
+      <c r="C33" s="54">
         <v>45993</v>
       </c>
       <c r="D33" s="23">
         <v>1</v>
       </c>
-      <c r="E33" s="61" t="s">
+      <c r="E33" s="63" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7622,21 +7696,21 @@
       <c r="A34" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="52">
+      <c r="B34" s="54">
         <v>45993</v>
       </c>
-      <c r="C34" s="52">
+      <c r="C34" s="54">
         <v>45993</v>
       </c>
       <c r="D34" s="23">
         <v>1</v>
       </c>
-      <c r="E34" s="61" t="s">
+      <c r="E34" s="63" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="28"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="23"/>
       <c r="C35" s="23"/>
       <c r="D35" s="23"/>
@@ -8250,298 +8324,298 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="48" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" ht="409.5" spans="1:3">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="31" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="3" ht="86.4" spans="1:3">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="28"/>
+      <c r="C3" s="30"/>
     </row>
     <row r="4" ht="57.6" spans="1:3">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="28"/>
+      <c r="C4" s="30"/>
     </row>
     <row r="5" ht="72" spans="1:3">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="28"/>
+      <c r="C5" s="30"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="28"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="28"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="28"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="28"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="28"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="28"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="28"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="28"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="28"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="28"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="28"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="28"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="28"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="28"/>
-      <c r="B36" s="28"/>
-      <c r="C36" s="28"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="28"/>
-      <c r="B37" s="28"/>
-      <c r="C37" s="28"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="28"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="28"/>
+      <c r="A38" s="30"/>
+      <c r="B38" s="30"/>
+      <c r="C38" s="30"/>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="28"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="28"/>
-      <c r="B40" s="28"/>
-      <c r="C40" s="28"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="28"/>
-      <c r="B41" s="28"/>
-      <c r="C41" s="28"/>
+      <c r="A41" s="30"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="30"/>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" s="28"/>
-      <c r="B42" s="28"/>
-      <c r="C42" s="28"/>
+      <c r="A42" s="30"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="30"/>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="28"/>
-      <c r="B43" s="28"/>
-      <c r="C43" s="28"/>
+      <c r="A43" s="30"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="28"/>
-      <c r="B44" s="28"/>
-      <c r="C44" s="28"/>
+      <c r="A44" s="30"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="28"/>
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
+      <c r="A45" s="30"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
     </row>
     <row r="46" spans="1:3">
-      <c r="A46" s="28"/>
-      <c r="B46" s="28"/>
-      <c r="C46" s="28"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="28"/>
-      <c r="B47" s="28"/>
-      <c r="C47" s="28"/>
+      <c r="A47" s="30"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
     </row>
     <row r="48" spans="1:3">
-      <c r="A48" s="28"/>
-      <c r="B48" s="28"/>
-      <c r="C48" s="28"/>
+      <c r="A48" s="30"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="30"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" s="28"/>
-      <c r="B49" s="28"/>
-      <c r="C49" s="28"/>
+      <c r="A49" s="30"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="30"/>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="28"/>
-      <c r="B50" s="28"/>
-      <c r="C50" s="28"/>
+      <c r="A50" s="30"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="30"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="28"/>
-      <c r="B51" s="28"/>
-      <c r="C51" s="28"/>
+      <c r="A51" s="30"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="30"/>
     </row>
     <row r="52" spans="1:3">
-      <c r="A52" s="28"/>
-      <c r="B52" s="28"/>
-      <c r="C52" s="28"/>
+      <c r="A52" s="30"/>
+      <c r="B52" s="30"/>
+      <c r="C52" s="30"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="28"/>
-      <c r="B53" s="28"/>
-      <c r="C53" s="28"/>
+      <c r="A53" s="30"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="30"/>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="28"/>
-      <c r="B54" s="28"/>
-      <c r="C54" s="28"/>
+      <c r="A54" s="30"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8565,52 +8639,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="30"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="41">
+      <c r="A2" s="43">
         <v>45962</v>
       </c>
-      <c r="B2" s="28"/>
+      <c r="B2" s="30"/>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="44" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="44" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="44" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="43">
+      <c r="A6" s="45">
         <v>45969</v>
       </c>
-      <c r="B6" s="28"/>
-    </row>
-    <row r="7" s="40" customFormat="1" ht="57.6" spans="1:2">
-      <c r="A7" s="44" t="s">
+      <c r="B6" s="30"/>
+    </row>
+    <row r="7" s="42" customFormat="1" ht="57.6" spans="1:2">
+      <c r="A7" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="47" t="s">
         <v>80</v>
       </c>
     </row>
@@ -8638,66 +8712,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="29" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" ht="201.6" spans="1:3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="31" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="3" ht="100.8" spans="1:3">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="30" t="s">
         <v>86</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="31" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="4" ht="72" spans="1:3">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="32" t="s">
         <v>89</v>
       </c>
       <c r="B4" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="28"/>
+      <c r="C4" s="30"/>
     </row>
     <row r="5" ht="129.6" spans="1:3">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="31" t="s">
         <v>91</v>
       </c>
       <c r="B5" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="31" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="6" ht="86.4" spans="1:4">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="31" t="s">
         <v>94</v>
       </c>
       <c r="B6" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="31" t="s">
         <v>96</v>
       </c>
       <c r="D6" s="11" t="s">
@@ -8711,7 +8785,7 @@
       <c r="B7" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="31" t="s">
         <v>100</v>
       </c>
     </row>
@@ -8722,7 +8796,7 @@
       <c r="B8" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="28"/>
+      <c r="C8" s="30"/>
     </row>
     <row r="9" ht="129.6" spans="1:3">
       <c r="A9" s="25" t="s">
@@ -8731,7 +8805,7 @@
       <c r="B9" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="28"/>
+      <c r="C9" s="30"/>
     </row>
     <row r="10" ht="129.6" spans="1:3">
       <c r="A10" s="23" t="s">
@@ -8740,7 +8814,7 @@
       <c r="B10" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="C10" s="28"/>
+      <c r="C10" s="30"/>
     </row>
     <row r="11" ht="158.4" spans="1:3">
       <c r="A11" s="23" t="s">
@@ -8749,7 +8823,7 @@
       <c r="B11" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="28"/>
+      <c r="C11" s="30"/>
     </row>
     <row r="12" ht="115.2" spans="1:3">
       <c r="A12" s="25" t="s">
@@ -8758,7 +8832,7 @@
       <c r="B12" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="31" t="s">
         <v>111</v>
       </c>
     </row>
@@ -8769,7 +8843,7 @@
       <c r="B13" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="31" t="s">
         <v>114</v>
       </c>
     </row>
@@ -8780,7 +8854,7 @@
       <c r="B14" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="C14" s="29"/>
+      <c r="C14" s="31"/>
     </row>
     <row r="15" ht="43.2" spans="1:3">
       <c r="A15" s="23" t="s">
@@ -8789,7 +8863,7 @@
       <c r="B15" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="C15" s="29"/>
+      <c r="C15" s="31"/>
     </row>
     <row r="16" ht="129.6" spans="1:3">
       <c r="A16" s="23" t="s">
@@ -8798,7 +8872,7 @@
       <c r="B16" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="31" t="s">
         <v>120</v>
       </c>
     </row>
@@ -8809,18 +8883,18 @@
       <c r="B17" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="31" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="18" ht="273.6" spans="1:4">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="35" t="s">
         <v>124</v>
       </c>
       <c r="D18" s="11" t="s">
@@ -8834,7 +8908,7 @@
       <c r="B19" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="31" t="s">
         <v>127</v>
       </c>
       <c r="D19" s="11" t="s">
@@ -8848,7 +8922,7 @@
       <c r="B20" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="31" t="s">
         <v>131</v>
       </c>
       <c r="D20" s="11" t="s">
@@ -8862,7 +8936,7 @@
       <c r="B21" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="C21" s="28"/>
+      <c r="C21" s="30"/>
     </row>
     <row r="22" ht="187.2" spans="1:3">
       <c r="A22" s="23" t="s">
@@ -8871,7 +8945,7 @@
       <c r="B22" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="C22" s="28"/>
+      <c r="C22" s="30"/>
     </row>
     <row r="23" ht="244.8" spans="1:3">
       <c r="A23" s="23" t="s">
@@ -8880,7 +8954,7 @@
       <c r="B23" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="C23" s="28"/>
+      <c r="C23" s="30"/>
     </row>
     <row r="24" ht="172.8" spans="1:3">
       <c r="A24" s="23" t="s">
@@ -8889,7 +8963,7 @@
       <c r="B24" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="C24" s="28"/>
+      <c r="C24" s="30"/>
     </row>
     <row r="25" ht="100.8" spans="1:3">
       <c r="A25" s="23" t="s">
@@ -8898,7 +8972,7 @@
       <c r="B25" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="C25" s="28"/>
+      <c r="C25" s="30"/>
     </row>
     <row r="26" ht="409" customHeight="1" spans="1:3">
       <c r="A26" s="23" t="s">
@@ -8907,7 +8981,7 @@
       <c r="B26" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="31" t="s">
         <v>145</v>
       </c>
     </row>
@@ -8918,7 +8992,7 @@
       <c r="B27" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C27" s="28"/>
+      <c r="C27" s="30"/>
     </row>
     <row r="28" ht="409.5" spans="1:4">
       <c r="A28" s="23" t="s">
@@ -8927,7 +9001,7 @@
       <c r="B28" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="31" t="s">
         <v>150</v>
       </c>
       <c r="D28" s="11" t="s">
@@ -8941,7 +9015,7 @@
       <c r="B29" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="31" t="s">
         <v>154</v>
       </c>
     </row>
@@ -8952,7 +9026,7 @@
       <c r="B30" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="C30" s="28"/>
+      <c r="C30" s="30"/>
     </row>
     <row r="31" ht="187.2" spans="1:3">
       <c r="A31" s="23" t="s">
@@ -8961,25 +9035,25 @@
       <c r="B31" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="C31" s="28"/>
+      <c r="C31" s="30"/>
     </row>
     <row r="32" ht="259.2" spans="1:3">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="C32" s="28"/>
+      <c r="C32" s="30"/>
     </row>
     <row r="33" ht="345.6" spans="1:3">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="B33" s="35" t="s">
+      <c r="B33" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="C33" s="28"/>
+      <c r="C33" s="30"/>
     </row>
     <row r="34" ht="100.8" spans="1:3">
       <c r="A34" s="23" t="s">
@@ -8988,7 +9062,7 @@
       <c r="B34" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="C34" s="28"/>
+      <c r="C34" s="30"/>
     </row>
     <row r="35" ht="72" spans="1:3">
       <c r="A35" s="23" t="s">
@@ -8997,7 +9071,7 @@
       <c r="B35" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="C35" s="28"/>
+      <c r="C35" s="30"/>
     </row>
     <row r="36" ht="409" customHeight="1" spans="1:3">
       <c r="A36" s="23" t="s">
@@ -9006,7 +9080,7 @@
       <c r="B36" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="C36" s="36" t="s">
+      <c r="C36" s="38" t="s">
         <v>169</v>
       </c>
     </row>
@@ -9017,7 +9091,7 @@
       <c r="B37" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="C37" s="37"/>
+      <c r="C37" s="39"/>
     </row>
     <row r="38" ht="288" spans="1:3">
       <c r="A38" s="23" t="s">
@@ -9026,7 +9100,7 @@
       <c r="B38" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="C38" s="38"/>
+      <c r="C38" s="40"/>
     </row>
     <row r="39" ht="216" spans="1:3">
       <c r="A39" s="23" t="s">
@@ -9035,7 +9109,7 @@
       <c r="B39" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="C39" s="28"/>
+      <c r="C39" s="30"/>
     </row>
     <row r="40" ht="100.8" spans="1:3">
       <c r="A40" s="25" t="s">
@@ -9044,71 +9118,71 @@
       <c r="B40" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="C40" s="28"/>
+      <c r="C40" s="30"/>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="23"/>
       <c r="B41" s="23"/>
-      <c r="C41" s="28"/>
+      <c r="C41" s="30"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="23"/>
       <c r="B42" s="23"/>
-      <c r="C42" s="28"/>
+      <c r="C42" s="30"/>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="23"/>
       <c r="B43" s="23"/>
-      <c r="C43" s="28"/>
+      <c r="C43" s="30"/>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="23"/>
       <c r="B44" s="23"/>
-      <c r="C44" s="28"/>
+      <c r="C44" s="30"/>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="23"/>
       <c r="B45" s="23"/>
-      <c r="C45" s="28"/>
+      <c r="C45" s="30"/>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="23"/>
       <c r="B46" s="23"/>
-      <c r="C46" s="28"/>
+      <c r="C46" s="30"/>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="23"/>
       <c r="B47" s="23"/>
-      <c r="C47" s="28"/>
+      <c r="C47" s="30"/>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="23"/>
       <c r="B48" s="23"/>
-      <c r="C48" s="28"/>
+      <c r="C48" s="30"/>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="23"/>
       <c r="B49" s="23"/>
-      <c r="C49" s="28"/>
+      <c r="C49" s="30"/>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="23"/>
       <c r="B50" s="23"/>
-      <c r="C50" s="28"/>
+      <c r="C50" s="30"/>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="23"/>
       <c r="B51" s="23"/>
-      <c r="C51" s="28"/>
+      <c r="C51" s="30"/>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="23"/>
       <c r="B52" s="23"/>
-      <c r="C52" s="28"/>
+      <c r="C52" s="30"/>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="39"/>
-      <c r="B53" s="39"/>
+      <c r="A53" s="41"/>
+      <c r="B53" s="41"/>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="23"/>
@@ -9226,10 +9300,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
@@ -9339,6 +9413,70 @@
     <row r="20" ht="72" spans="1:1">
       <c r="A20" s="7" t="s">
         <v>181</v>
+      </c>
+    </row>
+    <row r="21" ht="100.8" spans="1:2">
+      <c r="A21" t="s">
+        <v>182</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B22" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="23" ht="57.6" spans="1:2">
+      <c r="A23" t="s">
+        <v>186</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="24" ht="72" spans="1:2">
+      <c r="A24" t="s">
+        <v>188</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" ht="86.4" spans="1:2">
+      <c r="A25" t="s">
+        <v>190</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="26" ht="43.2" spans="1:2">
+      <c r="A26" t="s">
+        <v>192</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="27" ht="28.8" spans="1:2">
+      <c r="A27" t="s">
+        <v>194</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="28" ht="43.2" spans="1:2">
+      <c r="A28" t="s">
+        <v>196</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -9360,17 +9498,17 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" s="22" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -9399,302 +9537,302 @@
   <sheetData>
     <row r="1" spans="2:3">
       <c r="B1" s="16" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="2:3">
       <c r="B2" s="17" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="17" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="17" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" s="17" t="s">
-        <v>191</v>
+        <v>207</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="2:3">
       <c r="B6" s="17" t="s">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="17" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" ht="43.2" spans="2:3">
       <c r="B8" s="17" t="s">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" s="18" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" ht="23.4" spans="2:2">
       <c r="B11" s="19" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="2:2">
       <c r="B12" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" t="s">
-        <v>200</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" s="20" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" s="20" t="s">
-        <v>202</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="2:2">
       <c r="B16" s="20" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="20" t="s">
-        <v>204</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="20" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="20" t="s">
-        <v>207</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="20" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" s="20" t="s">
-        <v>209</v>
+        <v>225</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" s="20" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" s="20" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
     </row>
     <row r="26" ht="23.4" spans="2:2">
       <c r="B26" s="19" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" s="20" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" s="20" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" s="20" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" s="20" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" s="20" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" s="20" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="20" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" s="20" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" s="20" t="s">
-        <v>224</v>
+        <v>240</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" s="20" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" s="20" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
     </row>
     <row r="40" spans="2:2">
       <c r="B40" t="s">
-        <v>227</v>
+        <v>243</v>
       </c>
     </row>
     <row r="41" ht="23.4" spans="2:2">
       <c r="B41" s="19" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
     </row>
     <row r="42" spans="2:2">
       <c r="B42" t="s">
-        <v>229</v>
+        <v>245</v>
       </c>
     </row>
     <row r="43" spans="2:2">
       <c r="B43" s="20" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
     </row>
     <row r="44" spans="2:2">
       <c r="B44" s="20" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
     </row>
     <row r="45" spans="2:2">
       <c r="B45" s="20" t="s">
-        <v>232</v>
+        <v>248</v>
       </c>
     </row>
     <row r="46" spans="2:2">
       <c r="B46" s="20" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
     </row>
     <row r="47" spans="2:2">
       <c r="B47" t="s">
-        <v>234</v>
+        <v>250</v>
       </c>
     </row>
     <row r="48" spans="2:2">
       <c r="B48" s="21" t="s">
-        <v>235</v>
+        <v>251</v>
       </c>
     </row>
     <row r="49" spans="2:2">
       <c r="B49" s="21" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50" s="21" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
     </row>
     <row r="51" spans="2:2">
       <c r="B51" s="21" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
     </row>
     <row r="52" spans="2:2">
       <c r="B52" t="s">
-        <v>239</v>
+        <v>255</v>
       </c>
     </row>
     <row r="54" ht="13" customHeight="1"/>
     <row r="55" ht="22" customHeight="1" spans="2:2">
       <c r="B55" s="19" t="s">
-        <v>240</v>
+        <v>256</v>
       </c>
     </row>
     <row r="56" spans="2:2">
       <c r="B56" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
     </row>
     <row r="57" spans="2:2">
       <c r="B57" s="20" t="s">
-        <v>242</v>
+        <v>258</v>
       </c>
     </row>
     <row r="58" spans="2:2">
@@ -9709,17 +9847,17 @@
     </row>
     <row r="60" spans="2:2">
       <c r="B60" s="20" t="s">
-        <v>243</v>
+        <v>259</v>
       </c>
     </row>
     <row r="61" spans="2:2">
       <c r="B61" s="20" t="s">
-        <v>244</v>
+        <v>260</v>
       </c>
     </row>
     <row r="62" spans="2:2">
       <c r="B62" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -9741,7 +9879,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="12" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -9756,7 +9894,7 @@
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
       <c r="N1" s="14" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="O1" s="15"/>
       <c r="P1" s="15"/>
@@ -9998,7 +10136,7 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="12" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -10184,7 +10322,7 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="13" t="s">
-        <v>249</v>
+        <v>265</v>
       </c>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>

</xml_diff>

<commit_message>
15-12-25 updated & doing revisions
</commit_message>
<xml_diff>
--- a/JavaPrograms/Work Done.xlsx
+++ b/JavaPrograms/Work Done.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8280" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="8280" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="DSA plan" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="442">
   <si>
     <r>
       <rPr>
@@ -773,6 +773,90 @@
 Why use it? It prevents your server from crashing due to bad inputs. It automates 50 lines of "if/else" validation code for you.</t>
   </si>
   <si>
+    <t>Why use a class here?</t>
+  </si>
+  <si>
+    <t>In Java, a Class is a big thing with methods and logic. In this specific Python context (Pydantic), a Class is just a Form Template.
+Python
+class CodeRequest(BaseModel):
+    code: str
+Translation: "Hey API, I am creating a form called CodeRequest. It has exactly ONE blank space to fill in, labeled code. And that space MUST contain text (str)."
+If we didn't use a class, we would have to manually parse the JSON body, check if the key exists, check if it's a string... messy. The Class defines the Shape of the data.</t>
+  </si>
+  <si>
+    <t>What is async?</t>
+  </si>
+  <si>
+    <t>This is the most important concept for modern web servers.
+Synchronous (The Old Way):
+You order coffee.
+The Barista stands there, staring at the machine for 2 minutes. 😐
+The line behind you waits. No one else can order until you get your coffee.
+Result: Slow.
+Asynchronous (async - The New Way):
+You order coffee.
+The Barista hits the button on the machine.
+While the coffee brews, the Barista turns around and takes the next person's order. ⚡
+When your coffee is done, they hand it to you.
+Result: Fast.
+In our code:
+Python
+@app.post("/review")
+async def review_code(request: CodeRequest):
+    # ... calling Google Gemini ...
+Calling Google Gemini takes time (maybe 2 seconds).
+Without async: Your server freezes for 2 seconds. No one else can use it.
+With async: Your server sends the request to Google, and while it waits for the answer, it can handle other users.</t>
+  </si>
+  <si>
+    <t>The Mental Model: The "Digital Restaurant" 🍔You know Java, so you know "Functions." But an API is different.Think of your computer as a Restaurant.1. The Server (uvicorn) = The Kitchen Staff 👨‍🍳Your Python script is just a recipe book. It does nothing by itself.Uvicorn is the team of chefs. They show up, turn on the lights, and wait for orders.That is why the terminal hangs. They are standing there, waiting.2. The App (app = FastAPI()) = The Front Counter 🏪This is where customers (users) walk up to talk to you.If you didn't have this, the chefs (Uvicorn) wouldn't know who to talk to.3. The Decorator (@app.post("/review")) = The Menu Board 📜This is the most confusing part for new Python devs.The Symbol: @ means "Decorate this function."The Concept: Imagine you have a function make_burger().In a normal script, you call it.In an API, you stick a sign on it: "Order Here for Burgers."@app.post("/review") tells the server: "If a customer comes to the /review window, run THIS specific function."4. JSON ({"code": "..."}) = The Order Ticket 📝Computers don't speak English. They speak JSON (JavaScript Object Notation).It is just a fancy text format that looks like a Dictionary.Key: What is it? ("code")Value: The actual data. ("print hello")The "Why" Behind The ToolsYou asked for the deeper reasoning. Here is the engineering reality.ToolWhy do we use it?The "Java Way" (Comparison)FastAPIIt is the fastest Python framework today. It writes the documentation for you automatically.Like Spring Boot, but 10x less code.UvicornPython is slow. Uvicorn is a "wrapper" written in C++ that makes Python run fast on the web.Like Tomcat in Java.Decorators (@)To attach "metadata" to a function without changing the code inside it.Like Annotations (@Override, @GetMapping) in Java.</t>
+  </si>
+  <si>
+    <t>Why does QuickSelect run faster than QuickSort?
+ans: QuickSort sorts both sides of the pivot
+QuickSelect only cares about one index
+So after partition:
+If pivot is at target index → DONE
+Else → recurse into only one side
+Complexity difference
+QuickSort → T(n) = T(left) + T(right)
+QuickSelect → T(n) = T(one side only)
+👉 That’s why average O(n) instead of O(n log n) 
+“QuickSelect is faster because it avoids unnecessary recursion and only explores the partition that contains the target element.”
+When would you prefer Merge Sort over QuickSort?
+ans. I prefer Merge Sort when I need guaranteed O(n log n) performance or stability, especially for linked lists or external sorting.  
+You prefer Merge Sort when:
+1️⃣ Guaranteed performance matters
+Merge Sort is always O(n log n)
+QuickSort can degrade to O(n²)
+2️⃣ Stability is required
+Merge Sort is stable
+QuickSort is not stable
+3️⃣ External sorting / large data
+Works well when data doesn’t fit in memory
+4️⃣ Linked Lists
+Merge Sort works beautifully on linked lists
+QuickSort doesn’t
+Why does Binary Search on Answer work?
+Your answer: Binary Search on Answer works because:
+The answer space is monotonic
+Meaning:
+If a value works, all bigger (or smaller) values also work
+OR
+If a value fails, all smaller (or bigger) values fail
+Example: Koko Eating Bananas
+Eating speed = x
+If Koko can eat at speed x
+→ she can eat at any speed &gt; x
+That’s a monotonic yes/no function.
+Pattern
+Define search space (low → high)
+Define can(mid)
+Use binary search on that space
+Interview-ready line
+“Binary Search on Answer works because the feasibility function is monotonic, allowing us to binary search the solution space.”</t>
+  </si>
+  <si>
     <t>Recall</t>
   </si>
   <si>
@@ -800,6 +884,15 @@
     <t>Selection Sort , Bubble Sort
 Rotate array                                                                                                                                                   Check if a number is palindrome **
 Find factorial of n</t>
+  </si>
+  <si>
+    <t>New Rule for You
+For every algorithm, you must be able to answer:
+What problem does it solve?
+Why does it work?
+What breaks it?
+Time + space?
+When would I choose it over alternatives?</t>
   </si>
   <si>
     <t>Questions</t>
@@ -2781,6 +2874,307 @@
 Otherwise create node and recurse</t>
   </si>
   <si>
+    <t>1️⃣ Bubble Sort
+Why it works
+Repeatedly swaps adjacent elements if they’re in the wrong order
+Largest element “bubbles” to the end each pass
+Time
+Best: O(n) (already sorted, with optimization)
+Avg/Worst: O(n²)
+Space
+O(1)
+When NOT to use
+Almost always in interviews
+Only useful for teaching or tiny inputs
+👉 Interview line:
+“Bubble sort is simple but inefficient for large datasets.”
+2️⃣ Selection Sort
+Why it works
+Selects the minimum element and puts it in the correct position
+Time
+Always O(n²)
+Space
+O(1)
+When NOT to use
+When stability matters
+When data is large
+👉 Interview line:
+“Selection sort minimizes swaps but is still quadratic.”
+3️⃣ Insertion Sort
+Why it works
+Builds sorted array one element at a time
+Inserts element into correct position in the sorted prefix
+Time
+Best: O(n) (nearly sorted)
+Worst: O(n²)
+Space
+O(1)
+When NOT to use
+Large unsorted datasets
+👉 Interview gold:
+“Insertion sort is efficient for nearly sorted arrays.”
+4️⃣ Merge Sort
+Why it works
+Divide array until single elements
+Merge sorted halves
+Time
+Always O(n log n)
+Space
+O(n)
+When NOT to use
+When memory is constrained
+In-place requirement
+👉 Interview line:
+“Merge sort guarantees O(n log n) but uses extra memory.”
+5️⃣ Merge Two Sorted Arrays
+Why it works
+Two pointers pick the smaller element each time
+Time
+O(n + m)
+Space
+O(n + m)
+When NOT to use
+When in-place merge is required (needs different logic)
+PART 3 — QuickSort Family (This is where interviews care)
+6️⃣ QuickSort (Lomuto)
+Why it works
+Picks last element as pivot
+Ensures all smaller elements are left of pivot
+Time
+Avg: O(n log n)
+Worst: O(n²)
+Space
+O(log n) recursion
+When NOT to use
+Already sorted arrays
+When duplicates are heavy
+👉 Interview line:
+“Lomuto is simple but sensitive to pivot choice.”
+7️⃣ QuickSort (Hoare)
+Why it works
+Uses two pointers moving inward
+Swaps elements that are on the wrong side
+Time
+Avg: O(n log n)
+Better constant factors than Lomuto
+Space
+O(log n)
+When NOT to use
+When implementation simplicity matters
+👉 Interview line:
+“Hoare partition is more efficient but trickier.”
+8️⃣ QuickSort (DNF – Dutch National Flag)
+Why it works
+Splits array into &lt; pivot, = pivot, &gt; pivot
+Handles duplicates efficiently
+Time
+Avg: O(n log n)
+Avoids duplicate-heavy worst cases
+Space
+O(log n)
+When NOT to use
+When duplicates are rare (extra complexity not needed)
+👉 Interview killer line:
+“DNF is ideal when many duplicates exist.”
+PART 4 — Selection / Partition Patterns
+QuickSelect (Kth Smallest/Largest)
+Why it works
+Same partition logic as QuickSort
+Only recurse into ONE side
+Time
+Avg: O(n)
+Worst: O(n²)
+Space
+O(1) extra
+When NOT to use
+When worst-case guarantees are required
+Top K Largest / Smallest
+Why
+Partition until kth index
+Everything beyond is result
+👉 Interview:
+“More efficient than sorting the entire array.”
+Count Inversions
+Why
+During merge, count when left &gt; right
+Time
+O(n log n)
+Space
+O(n)
+PART 5 — Trees &amp; Binary Search on Answer (High-level)
+You already code these well, so interview explanation is simple:
+Level Order → BFS using queue
+Right Side View → last node per level
+Max Depth → DFS height
+Balanced Tree → height difference ≤ 1
+Diameter → longest path through any node
+Invert Tree → swap left/right recursively
+Path Sum → DFS accumulating sum
+Binary Search on Answer:
+“Search on solution space instead of array.”
+That single sentence covers:
+Koko
+Split Array
+Ship Packages
+Median of Two Arrays
+PART 6 — New Rule (Very Important)
+From now on, every revision includes a quiz.
+Example quiz I’ll ask you:
+“Why does QuickSelect run faster than QuickSort?”
+“When would you prefer Merge Sort over QuickSort?”
+“Why does Binary Search on Answer work?”
+No code. Only thinking.</t>
+  </si>
+  <si>
+    <t>Big-O hierarchy (time &amp; space) — what’s good vs bad
+Think of Big-O as how pain grows when input grows
+From best → worst 👇
+🟢 Excellent (very fast)
+O(1) — constant
+→ Doesn’t care about input size
+Example: array access, hashmap get
+🟢 Very good
+O(log n)
+→ Cuts problem in half every step
+Example: Binary Search
+🟡 Good / acceptable
+O(n)
+→ Linear scan
+Example: one loop over array
+🟡 Still good (industry standard)
+O(n log n)
+→ Best possible for comparison sorting
+Example: Merge Sort, QuickSort (avg)
+🔴 Bad (avoid if possible)
+O(n²)
+→ Nested loops
+Example: Bubble / Selection / worst QuickSort
+🔴🔴 Very bad
+O(2ⁿ), O(n!)
+→ Explodes fast
+Example: brute force recursion
+📌 Interview rule of thumb
+Aim for O(n) or O(n log n)
+O(n²) only if constraints are small
+O(1) space is a bonus, not mandatory</t>
+  </si>
+  <si>
+    <t>DFS vs BFS</t>
+  </si>
+  <si>
+    <t>Your answer:
+Conceptually right. Analogy is good.
+Verdict: ✅ Correct (needs tightening)
+Interview-ready version:
+DFS explores as deep as possible before backtracking, which is useful for problems like path-related questions, height, balance, and recursion-based logic.
+BFS explores level by level using a queue, which is ideal for level order traversal, shortest path in trees, and width-based problems.</t>
+  </si>
+  <si>
+    <t>Why Level Order needs a queue</t>
+  </si>
+  <si>
+    <t>BFS needs FIFO order
+Queue preserves insertion order
+Recursion alone cannot guarantee level separation
+Interview-ready answer:
+Level order traversal requires a queue because BFS processes nodes in FIFO order.
+This ensures all nodes at a level are processed before moving to the next level, which recursion alone cannot guarantee.</t>
+  </si>
+  <si>
+    <t>Right Side View (one sentence)</t>
+  </si>
+  <si>
+    <t>At each level, the last node visited during BFS represents the node visible from the right side.</t>
+  </si>
+  <si>
+    <t>Max Depth vs Diameter</t>
+  </si>
+  <si>
+    <t>orrect explanation:
+Max Depth: longest path from root to leaf
+Diameter: longest path between any two nodes (may not pass through root)
+Interview-ready answer:
+Maximum depth measures height from root to leaf, whereas diameter measures the longest path between any two nodes in the tree, which may or may not pass through the root.</t>
+  </si>
+  <si>
+    <t>Why Balanced Tree needs bottom-up DFS</t>
+  </si>
+  <si>
+    <t>Your answer:
+Correct intuition, weak explanation.
+Verdict: ⚠️ Half correct
+Correct reasoning:
+Height must be known before checking balance
+Bottom-up avoids recomputation
+Interview-ready answer:
+Balanced Binary Tree requires bottom-up DFS because we must compute the height of subtrees before checking balance.
+A top-down approach would repeatedly recompute heights, leading to O(n²) time.</t>
+  </si>
+  <si>
+    <t>Why Path Sum subtracts value</t>
+  </si>
+  <si>
+    <t>We subtract the node value so that each recursive call checks whether the remaining required sum can be achieved down that path.
+This ensures we only consider root-to-leaf paths.</t>
+  </si>
+  <si>
+    <t>Path Sum II — why copy path</t>
+  </si>
+  <si>
+    <t>We copy the path list because it is mutable.
+Without copying, backtracking would modify paths already stored in the result, causing incorrect answers.</t>
+  </si>
+  <si>
+    <t>Invert Binary Tree</t>
+  </si>
+  <si>
+    <t>Correct explanation:
+Recursive subproblem: invert left and right subtrees
+Then swap them
+Interview-ready answer:
+Invert Binary Tree is a classic recursion problem because each subtree can be inverted independently.
+The recursive subproblem is to invert the left and right subtrees, then swap them.</t>
+  </si>
+  <si>
+    <t>Same Tree</t>
+  </si>
+  <si>
+    <t>Correct 3 conditions:
+Both nodes are null → true
+One is null, other is not → false
+Values match AND left subtrees match AND right subtrees match
+Interview-ready answer:
+Two trees are the same if their root values match and both left and right subtrees are recursively identical.</t>
+  </si>
+  <si>
+    <t>Lowest Common Ancestor</t>
+  </si>
+  <si>
+    <t>If left and right recursive calls both return non-null, it means one node was found in each subtree, so the current node is their lowest common ancestor.</t>
+  </si>
+  <si>
+    <t>Max Path Sum — why Math.max(0, ...)</t>
+  </si>
+  <si>
+    <t>Correct explanation:
+Negative path sums reduce the total, so we discard them by taking max with 0.
+Without this, negative values could incorrectly lower the maximum path sum.</t>
+  </si>
+  <si>
+    <t>Why return only one side in Max Path Sum</t>
+  </si>
+  <si>
+    <t>When returning to the parent, a path can only extend in one direction (left or right).
+Using both would create a fork, which is invalid for a single path.</t>
+  </si>
+  <si>
+    <t>Why HashMap for inorder</t>
+  </si>
+  <si>
+    <t>The HashMap allows O(1) lookup of root index in inorder traversal.
+Without it, each lookup would be O(n), degrading overall complexity to O(n²).</t>
+  </si>
+  <si>
     <t>Space Complexity</t>
   </si>
   <si>
@@ -4075,9 +4469,6 @@
   </si>
   <si>
     <t>track longest left+right path</t>
-  </si>
-  <si>
-    <t>Same Tree</t>
   </si>
   <si>
     <t>check structure + value same</t>
@@ -4951,7 +5342,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5072,8 +5463,17 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
@@ -5101,9 +5501,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
@@ -5784,246 +6181,246 @@
   </cols>
   <sheetData>
     <row r="1" ht="90" customHeight="1" spans="1:6">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="66" t="s">
+      <c r="B1" s="67"/>
+      <c r="C1" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="67"/>
-      <c r="E1" s="68" t="s">
+      <c r="D1" s="69"/>
+      <c r="E1" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="68"/>
+      <c r="F1" s="70"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="71" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="23"/>
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="71"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="23"/>
       <c r="B4" s="23"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="23"/>
       <c r="B5" s="23"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="23"/>
       <c r="B6" s="23"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="23"/>
       <c r="B7" s="23"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="69" t="s">
+      <c r="A9" s="71" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="25"/>
-      <c r="C9" s="76" t="s">
+      <c r="C9" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="77"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="25"/>
       <c r="B10" s="25"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="25"/>
       <c r="B11" s="25"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="79"/>
-      <c r="E11" s="68"/>
-      <c r="F11" s="68"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="25"/>
       <c r="B12" s="25"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="79"/>
-      <c r="E12" s="68"/>
-      <c r="F12" s="68"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="25"/>
       <c r="B13" s="25"/>
-      <c r="C13" s="78"/>
-      <c r="D13" s="79"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="68"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="25"/>
       <c r="B14" s="25"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="70"/>
     </row>
     <row r="15" ht="15" customHeight="1" spans="1:6">
       <c r="A15" s="25"/>
       <c r="B15" s="25"/>
-      <c r="C15" s="80"/>
-      <c r="D15" s="81"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="68"/>
+      <c r="C15" s="82"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="25"/>
       <c r="B16" s="25"/>
-      <c r="C16" s="82" t="s">
+      <c r="C16" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="83"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="68"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="70"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="25"/>
       <c r="B17" s="25"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="85"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="68"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="25"/>
       <c r="B18" s="25"/>
-      <c r="C18" s="84"/>
-      <c r="D18" s="85"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="68"/>
+      <c r="C18" s="86"/>
+      <c r="D18" s="87"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="69" t="s">
+      <c r="A19" s="71" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="23"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="85"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="68"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="87"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="70"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="23"/>
       <c r="B20" s="23"/>
-      <c r="C20" s="84"/>
-      <c r="D20" s="85"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="68"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="87"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="23"/>
       <c r="B21" s="23"/>
-      <c r="C21" s="84"/>
-      <c r="D21" s="85"/>
-      <c r="E21" s="68"/>
-      <c r="F21" s="68"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="70"/>
+      <c r="F21" s="70"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="23"/>
       <c r="B22" s="23"/>
-      <c r="C22" s="84"/>
-      <c r="D22" s="85"/>
+      <c r="C22" s="86"/>
+      <c r="D22" s="87"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="23"/>
       <c r="B23" s="23"/>
-      <c r="C23" s="86"/>
-      <c r="D23" s="87"/>
+      <c r="C23" s="88"/>
+      <c r="D23" s="89"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="23"/>
       <c r="B24" s="23"/>
-      <c r="C24" s="88" t="s">
+      <c r="C24" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="89"/>
+      <c r="D24" s="91"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="23"/>
       <c r="B25" s="23"/>
-      <c r="C25" s="90"/>
-      <c r="D25" s="91"/>
+      <c r="C25" s="92"/>
+      <c r="D25" s="93"/>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="23"/>
       <c r="B26" s="23"/>
-      <c r="C26" s="90"/>
-      <c r="D26" s="91"/>
+      <c r="C26" s="92"/>
+      <c r="D26" s="93"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="23"/>
       <c r="B27" s="23"/>
-      <c r="C27" s="90"/>
-      <c r="D27" s="91"/>
+      <c r="C27" s="92"/>
+      <c r="D27" s="93"/>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="23"/>
       <c r="B28" s="23"/>
-      <c r="C28" s="92"/>
-      <c r="D28" s="93"/>
+      <c r="C28" s="94"/>
+      <c r="D28" s="95"/>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="23"/>
@@ -6038,7 +6435,7 @@
       <c r="D30" s="29"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="69" t="s">
+      <c r="A31" s="71" t="s">
         <v>10</v>
       </c>
       <c r="B31" s="25"/>
@@ -6094,7 +6491,7 @@
       <c r="D39" s="29"/>
     </row>
     <row r="40" ht="18" customHeight="1" spans="1:4">
-      <c r="A40" s="69" t="s">
+      <c r="A40" s="71" t="s">
         <v>11</v>
       </c>
       <c r="B40" s="25"/>
@@ -6156,7 +6553,7 @@
       <c r="D49" s="29"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="69" t="s">
+      <c r="A50" s="71" t="s">
         <v>12</v>
       </c>
       <c r="B50" s="25"/>
@@ -6212,7 +6609,7 @@
       <c r="D58" s="29"/>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="69" t="s">
+      <c r="A59" s="71" t="s">
         <v>13</v>
       </c>
       <c r="B59" s="23"/>
@@ -6268,7 +6665,7 @@
       <c r="D67" s="29"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="69" t="s">
+      <c r="A68" s="71" t="s">
         <v>14</v>
       </c>
       <c r="B68" s="23"/>
@@ -6330,7 +6727,7 @@
       <c r="D77" s="29"/>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="69" t="s">
+      <c r="A78" s="71" t="s">
         <v>15</v>
       </c>
       <c r="B78" s="23"/>
@@ -6392,7 +6789,7 @@
       <c r="D87" s="29"/>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="69" t="s">
+      <c r="A88" s="71" t="s">
         <v>16</v>
       </c>
       <c r="B88" s="23"/>
@@ -6448,7 +6845,7 @@
       <c r="D96" s="29"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="69" t="s">
+      <c r="A97" s="71" t="s">
         <v>17</v>
       </c>
       <c r="B97" s="25"/>
@@ -6504,7 +6901,7 @@
       <c r="D105" s="29"/>
     </row>
     <row r="106" spans="1:4">
-      <c r="A106" s="69" t="s">
+      <c r="A106" s="71" t="s">
         <v>18</v>
       </c>
       <c r="B106" s="23"/>
@@ -6603,10 +7000,10 @@
   <sheetData>
     <row r="1" ht="409" customHeight="1" spans="1:2">
       <c r="A1" s="7" t="s">
-        <v>299</v>
+        <v>334</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>300</v>
+        <v>335</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -6757,18 +7154,18 @@
     </row>
     <row r="2" ht="409.5" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>301</v>
+        <v>336</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>302</v>
+        <v>337</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>303</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" ht="409.5" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>304</v>
+        <v>339</v>
       </c>
       <c r="C3"/>
     </row>
@@ -6817,32 +7214,32 @@
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="1" t="s">
-        <v>305</v>
+        <v>340</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="1" t="s">
-        <v>306</v>
+        <v>341</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="1" t="s">
-        <v>307</v>
+        <v>342</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="10" t="s">
-        <v>308</v>
+        <v>343</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="1" t="s">
-        <v>309</v>
+        <v>344</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="1" t="s">
-        <v>310</v>
+        <v>345</v>
       </c>
     </row>
     <row r="36" ht="23.4" spans="1:1">
@@ -6850,177 +7247,177 @@
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="1" t="s">
-        <v>311</v>
+        <v>346</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="1" t="s">
-        <v>312</v>
+        <v>347</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="1" t="s">
-        <v>313</v>
+        <v>348</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="1" t="s">
-        <v>314</v>
+        <v>349</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="1" t="s">
-        <v>315</v>
+        <v>350</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="1" t="s">
-        <v>316</v>
+        <v>351</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="1" t="s">
-        <v>317</v>
+        <v>352</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="1" t="s">
-        <v>318</v>
+        <v>353</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="1" t="s">
-        <v>319</v>
+        <v>354</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="1" t="s">
-        <v>320</v>
+        <v>355</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="10" t="s">
-        <v>321</v>
+        <v>356</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="1" t="s">
-        <v>322</v>
+        <v>357</v>
       </c>
     </row>
     <row r="60" ht="23.4" spans="1:1">
       <c r="A60" s="9" t="s">
-        <v>323</v>
+        <v>358</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="1" t="s">
-        <v>324</v>
+        <v>359</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="1" t="s">
-        <v>325</v>
+        <v>360</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="1" t="s">
-        <v>326</v>
+        <v>361</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="1" t="s">
-        <v>327</v>
+        <v>362</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="1" t="s">
-        <v>328</v>
+        <v>363</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="1" t="s">
-        <v>329</v>
+        <v>364</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="1" t="s">
-        <v>330</v>
+        <v>365</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="1" t="s">
-        <v>331</v>
+        <v>366</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="1" t="s">
-        <v>332</v>
+        <v>367</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="1" t="s">
-        <v>333</v>
+        <v>368</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="10" t="s">
-        <v>334</v>
+        <v>369</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="1" t="s">
-        <v>335</v>
+        <v>370</v>
       </c>
     </row>
     <row r="86" ht="23.4" spans="1:1">
       <c r="A86" s="9" t="s">
-        <v>336</v>
+        <v>371</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="1" t="s">
-        <v>337</v>
+        <v>372</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="1" t="s">
-        <v>338</v>
+        <v>373</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="1" t="s">
-        <v>339</v>
+        <v>374</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="1" t="s">
-        <v>340</v>
+        <v>375</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" s="1" t="s">
-        <v>341</v>
+        <v>376</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" s="1" t="s">
-        <v>342</v>
+        <v>377</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="1" t="s">
-        <v>343</v>
+        <v>378</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" s="1" t="s">
-        <v>344</v>
+        <v>379</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="1" t="s">
-        <v>345</v>
+        <v>380</v>
       </c>
     </row>
     <row r="103" spans="1:1">
@@ -7030,12 +7427,12 @@
     </row>
     <row r="105" spans="1:1">
       <c r="A105" s="1" t="s">
-        <v>346</v>
+        <v>381</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" s="1" t="s">
-        <v>221</v>
+        <v>256</v>
       </c>
     </row>
     <row r="108" spans="1:1">
@@ -7043,12 +7440,12 @@
     </row>
     <row r="109" spans="1:1">
       <c r="A109" s="1" t="s">
-        <v>347</v>
+        <v>382</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" s="1" t="s">
-        <v>348</v>
+        <v>383</v>
       </c>
     </row>
     <row r="112" ht="23.4" spans="1:1">
@@ -7056,42 +7453,42 @@
     </row>
     <row r="113" spans="1:1">
       <c r="A113" s="1" t="s">
-        <v>349</v>
+        <v>384</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" s="1" t="s">
-        <v>350</v>
+        <v>385</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" s="1" t="s">
-        <v>351</v>
+        <v>386</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" s="1" t="s">
-        <v>352</v>
+        <v>387</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" s="1" t="s">
-        <v>353</v>
+        <v>388</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" s="1" t="s">
-        <v>354</v>
+        <v>389</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" s="1" t="s">
-        <v>355</v>
+        <v>390</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" s="1" t="s">
-        <v>356</v>
+        <v>391</v>
       </c>
     </row>
     <row r="128" spans="1:1">
@@ -7099,12 +7496,12 @@
     </row>
     <row r="129" spans="1:1">
       <c r="A129" s="1" t="s">
-        <v>357</v>
+        <v>392</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" s="1" t="s">
-        <v>358</v>
+        <v>393</v>
       </c>
     </row>
     <row r="132" ht="23.4" spans="1:1">
@@ -7112,62 +7509,62 @@
     </row>
     <row r="133" spans="1:1">
       <c r="A133" s="1" t="s">
-        <v>359</v>
+        <v>394</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" s="1" t="s">
-        <v>360</v>
+        <v>395</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" s="1" t="s">
-        <v>361</v>
+        <v>396</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" s="1" t="s">
-        <v>362</v>
+        <v>397</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" s="1" t="s">
-        <v>363</v>
+        <v>398</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" s="1" t="s">
-        <v>364</v>
+        <v>399</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" s="1" t="s">
-        <v>365</v>
+        <v>400</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" s="1" t="s">
-        <v>366</v>
+        <v>401</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" s="1" t="s">
-        <v>367</v>
+        <v>402</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" s="10" t="s">
-        <v>368</v>
+        <v>403</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" s="1" t="s">
-        <v>369</v>
+        <v>404</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" s="1" t="s">
-        <v>370</v>
+        <v>405</v>
       </c>
     </row>
     <row r="154" ht="23.4" spans="1:1">
@@ -7175,62 +7572,62 @@
     </row>
     <row r="156" spans="1:1">
       <c r="A156" s="1" t="s">
-        <v>371</v>
+        <v>406</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" s="1" t="s">
-        <v>372</v>
+        <v>407</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" s="1" t="s">
-        <v>373</v>
+        <v>408</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" s="1" t="s">
-        <v>374</v>
+        <v>409</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" s="1" t="s">
-        <v>375</v>
+        <v>410</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" s="1" t="s">
-        <v>376</v>
+        <v>411</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" s="1" t="s">
-        <v>377</v>
+        <v>412</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" s="1" t="s">
-        <v>378</v>
+        <v>413</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" s="1" t="s">
-        <v>379</v>
+        <v>414</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" s="10" t="s">
-        <v>380</v>
+        <v>415</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" s="1" t="s">
-        <v>381</v>
+        <v>416</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" s="1" t="s">
-        <v>382</v>
+        <v>417</v>
       </c>
     </row>
     <row r="180" spans="1:1">
@@ -7240,7 +7637,7 @@
     </row>
     <row r="182" spans="1:1">
       <c r="A182" s="1" t="s">
-        <v>383</v>
+        <v>418</v>
       </c>
     </row>
     <row r="184" spans="1:1">
@@ -7250,122 +7647,122 @@
     </row>
     <row r="186" spans="1:1">
       <c r="A186" s="1" t="s">
-        <v>384</v>
+        <v>419</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" s="1" t="s">
-        <v>385</v>
+        <v>420</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" s="1" t="s">
-        <v>386</v>
+        <v>421</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" s="1" t="s">
-        <v>387</v>
+        <v>422</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" s="1" t="s">
-        <v>388</v>
+        <v>423</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" s="1" t="s">
-        <v>389</v>
+        <v>424</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" s="1" t="s">
-        <v>390</v>
+        <v>425</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" s="1" t="s">
-        <v>391</v>
+        <v>426</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" s="1" t="s">
-        <v>392</v>
+        <v>427</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" s="1" t="s">
-        <v>393</v>
+        <v>428</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" s="1" t="s">
-        <v>394</v>
+        <v>429</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" s="1" t="s">
-        <v>395</v>
+        <v>430</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" s="1" t="s">
-        <v>396</v>
+        <v>431</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" s="1" t="s">
-        <v>397</v>
+        <v>432</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" s="1" t="s">
-        <v>398</v>
+        <v>433</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" s="1" t="s">
-        <v>399</v>
+        <v>434</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" s="1" t="s">
-        <v>400</v>
+        <v>435</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" s="1" t="s">
-        <v>401</v>
+        <v>236</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" s="1" t="s">
-        <v>402</v>
+        <v>436</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" s="1" t="s">
-        <v>403</v>
+        <v>437</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" s="1" t="s">
-        <v>404</v>
+        <v>438</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" s="1" t="s">
-        <v>405</v>
+        <v>439</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" s="1" t="s">
-        <v>406</v>
+        <v>440</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" s="1" t="s">
-        <v>407</v>
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -7405,7 +7802,7 @@
       <c r="D1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="54" t="s">
         <v>23</v>
       </c>
     </row>
@@ -7413,31 +7810,31 @@
       <c r="A2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="53">
+      <c r="B2" s="55">
         <v>45976</v>
       </c>
-      <c r="C2" s="54">
+      <c r="C2" s="56">
         <v>45983</v>
       </c>
       <c r="D2" s="23">
         <v>4</v>
       </c>
-      <c r="E2" s="55"/>
+      <c r="E2" s="57"/>
     </row>
     <row r="3" ht="115.2" spans="1:5">
       <c r="A3" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="53">
+      <c r="B3" s="55">
         <v>45976</v>
       </c>
-      <c r="C3" s="54">
+      <c r="C3" s="56">
         <v>45983</v>
       </c>
       <c r="D3" s="23">
         <v>4</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="58" t="s">
         <v>26</v>
       </c>
     </row>
@@ -7445,16 +7842,16 @@
       <c r="A4" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="53">
+      <c r="B4" s="55">
         <v>45976</v>
       </c>
-      <c r="C4" s="54">
+      <c r="C4" s="56">
         <v>45983</v>
       </c>
       <c r="D4" s="23">
         <v>3</v>
       </c>
-      <c r="E4" s="57" t="s">
+      <c r="E4" s="59" t="s">
         <v>28</v>
       </c>
     </row>
@@ -7462,125 +7859,125 @@
       <c r="A5" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="53">
+      <c r="B5" s="55">
         <v>45976</v>
       </c>
-      <c r="C5" s="54">
+      <c r="C5" s="56">
         <v>45983</v>
       </c>
       <c r="D5" s="23">
         <v>2</v>
       </c>
-      <c r="E5" s="58"/>
+      <c r="E5" s="60"/>
     </row>
     <row r="6" ht="115.2" spans="1:5">
       <c r="A6" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="53">
+      <c r="B6" s="55">
         <v>45976</v>
       </c>
-      <c r="C6" s="54">
+      <c r="C6" s="56">
         <v>45983</v>
       </c>
       <c r="D6" s="23">
         <v>2</v>
       </c>
-      <c r="E6" s="58"/>
+      <c r="E6" s="60"/>
     </row>
     <row r="7" ht="129.6" spans="1:5">
       <c r="A7" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="53">
+      <c r="B7" s="55">
         <v>45976</v>
       </c>
-      <c r="C7" s="54">
+      <c r="C7" s="56">
         <v>45983</v>
       </c>
       <c r="D7" s="23">
         <v>2</v>
       </c>
-      <c r="E7" s="58"/>
-    </row>
-    <row r="8" s="51" customFormat="1" ht="144" spans="1:5">
-      <c r="A8" s="59" t="s">
+      <c r="E7" s="60"/>
+    </row>
+    <row r="8" s="53" customFormat="1" ht="144" spans="1:5">
+      <c r="A8" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="54">
+      <c r="B8" s="56">
         <v>45976</v>
       </c>
-      <c r="C8" s="54">
+      <c r="C8" s="56">
         <v>45983</v>
       </c>
-      <c r="D8" s="60">
+      <c r="D8" s="62">
         <v>2</v>
       </c>
-      <c r="E8" s="61"/>
-    </row>
-    <row r="9" s="51" customFormat="1" ht="158.4" spans="1:5">
-      <c r="A9" s="59" t="s">
+      <c r="E8" s="63"/>
+    </row>
+    <row r="9" s="53" customFormat="1" ht="158.4" spans="1:5">
+      <c r="A9" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="54">
+      <c r="B9" s="56">
         <v>45976</v>
       </c>
-      <c r="C9" s="54">
+      <c r="C9" s="56">
         <v>45983</v>
       </c>
-      <c r="D9" s="60">
+      <c r="D9" s="62">
         <v>1</v>
       </c>
-      <c r="E9" s="62"/>
-    </row>
-    <row r="10" s="51" customFormat="1" spans="1:5">
-      <c r="A10" s="60" t="s">
+      <c r="E9" s="64"/>
+    </row>
+    <row r="10" s="53" customFormat="1" spans="1:5">
+      <c r="A10" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="54">
+      <c r="B10" s="56">
         <v>45976</v>
       </c>
-      <c r="C10" s="54">
+      <c r="C10" s="56">
         <v>45983</v>
       </c>
-      <c r="D10" s="60">
+      <c r="D10" s="62">
         <v>1</v>
       </c>
-      <c r="E10" s="63" t="s">
+      <c r="E10" s="65" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" s="51" customFormat="1" spans="1:5">
-      <c r="A11" s="60" t="s">
+    <row r="11" s="53" customFormat="1" spans="1:5">
+      <c r="A11" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="54">
+      <c r="B11" s="56">
         <v>45976</v>
       </c>
-      <c r="C11" s="54">
+      <c r="C11" s="56">
         <v>45983</v>
       </c>
-      <c r="D11" s="60">
+      <c r="D11" s="62">
         <v>1</v>
       </c>
-      <c r="E11" s="63" t="s">
+      <c r="E11" s="65" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" s="51" customFormat="1" spans="1:5">
-      <c r="A12" s="60" t="s">
+    <row r="12" s="53" customFormat="1" spans="1:5">
+      <c r="A12" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="54">
+      <c r="B12" s="56">
         <v>45976</v>
       </c>
-      <c r="C12" s="54">
+      <c r="C12" s="56">
         <v>45983</v>
       </c>
-      <c r="D12" s="60">
+      <c r="D12" s="62">
         <v>1</v>
       </c>
-      <c r="E12" s="63" t="s">
+      <c r="E12" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7588,16 +7985,16 @@
       <c r="A13" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="54">
+      <c r="B13" s="56">
         <v>45977</v>
       </c>
-      <c r="C13" s="54">
+      <c r="C13" s="56">
         <v>45982</v>
       </c>
       <c r="D13" s="23">
         <v>1</v>
       </c>
-      <c r="E13" s="63" t="s">
+      <c r="E13" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7605,16 +8002,16 @@
       <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="54">
+      <c r="B14" s="56">
         <v>45980</v>
       </c>
-      <c r="C14" s="54">
+      <c r="C14" s="56">
         <v>45982</v>
       </c>
       <c r="D14" s="23">
         <v>1</v>
       </c>
-      <c r="E14" s="63" t="s">
+      <c r="E14" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7622,16 +8019,16 @@
       <c r="A15" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="54">
+      <c r="B15" s="56">
         <v>45980</v>
       </c>
-      <c r="C15" s="54">
+      <c r="C15" s="56">
         <v>45982</v>
       </c>
       <c r="D15" s="23">
         <v>1</v>
       </c>
-      <c r="E15" s="63" t="s">
+      <c r="E15" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7639,16 +8036,16 @@
       <c r="A16" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="54">
+      <c r="B16" s="56">
         <v>45980</v>
       </c>
-      <c r="C16" s="54">
+      <c r="C16" s="56">
         <v>45982</v>
       </c>
       <c r="D16" s="23">
         <v>1</v>
       </c>
-      <c r="E16" s="63" t="s">
+      <c r="E16" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7656,16 +8053,16 @@
       <c r="A17" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="54">
+      <c r="B17" s="56">
         <v>45980</v>
       </c>
-      <c r="C17" s="54">
+      <c r="C17" s="56">
         <v>45982</v>
       </c>
       <c r="D17" s="23">
         <v>1</v>
       </c>
-      <c r="E17" s="63" t="s">
+      <c r="E17" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7673,16 +8070,16 @@
       <c r="A18" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="54">
+      <c r="B18" s="56">
         <v>45981</v>
       </c>
-      <c r="C18" s="54">
+      <c r="C18" s="56">
         <v>45983</v>
       </c>
       <c r="D18" s="23">
         <v>1</v>
       </c>
-      <c r="E18" s="63" t="s">
+      <c r="E18" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7690,16 +8087,16 @@
       <c r="A19" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="54">
+      <c r="B19" s="56">
         <v>45982</v>
       </c>
-      <c r="C19" s="54">
+      <c r="C19" s="56">
         <v>45984</v>
       </c>
       <c r="D19" s="23">
         <v>1</v>
       </c>
-      <c r="E19" s="63" t="s">
+      <c r="E19" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7707,16 +8104,16 @@
       <c r="A20" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="54">
+      <c r="B20" s="56">
         <v>45983</v>
       </c>
-      <c r="C20" s="54">
+      <c r="C20" s="56">
         <v>45985</v>
       </c>
       <c r="D20" s="23">
         <v>1</v>
       </c>
-      <c r="E20" s="63" t="s">
+      <c r="E20" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7724,16 +8121,16 @@
       <c r="A21" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="54">
+      <c r="B21" s="56">
         <v>45986</v>
       </c>
-      <c r="C21" s="54">
+      <c r="C21" s="56">
         <v>45987</v>
       </c>
       <c r="D21" s="23">
         <v>1</v>
       </c>
-      <c r="E21" s="63" t="s">
+      <c r="E21" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7741,16 +8138,16 @@
       <c r="A22" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="54">
+      <c r="B22" s="56">
         <v>45986</v>
       </c>
-      <c r="C22" s="54">
+      <c r="C22" s="56">
         <v>45987</v>
       </c>
       <c r="D22" s="23">
         <v>1</v>
       </c>
-      <c r="E22" s="63" t="s">
+      <c r="E22" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7758,16 +8155,16 @@
       <c r="A23" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="54">
+      <c r="B23" s="56">
         <v>45986</v>
       </c>
-      <c r="C23" s="54">
+      <c r="C23" s="56">
         <v>45987</v>
       </c>
       <c r="D23" s="23">
         <v>1</v>
       </c>
-      <c r="E23" s="63" t="s">
+      <c r="E23" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7775,16 +8172,16 @@
       <c r="A24" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="54">
+      <c r="B24" s="56">
         <v>45986</v>
       </c>
-      <c r="C24" s="54">
+      <c r="C24" s="56">
         <v>45987</v>
       </c>
       <c r="D24" s="23">
         <v>1</v>
       </c>
-      <c r="E24" s="63" t="s">
+      <c r="E24" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7792,16 +8189,16 @@
       <c r="A25" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="54">
+      <c r="B25" s="56">
         <v>45986</v>
       </c>
-      <c r="C25" s="54">
+      <c r="C25" s="56">
         <v>45987</v>
       </c>
       <c r="D25" s="23">
         <v>1</v>
       </c>
-      <c r="E25" s="63" t="s">
+      <c r="E25" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7809,16 +8206,16 @@
       <c r="A26" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="54">
+      <c r="B26" s="56">
         <v>45986</v>
       </c>
-      <c r="C26" s="54">
+      <c r="C26" s="56">
         <v>45987</v>
       </c>
       <c r="D26" s="23">
         <v>1</v>
       </c>
-      <c r="E26" s="63" t="s">
+      <c r="E26" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7826,16 +8223,16 @@
       <c r="A27" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="54">
+      <c r="B27" s="56">
         <v>45986</v>
       </c>
-      <c r="C27" s="54">
+      <c r="C27" s="56">
         <v>45987</v>
       </c>
       <c r="D27" s="23">
         <v>1</v>
       </c>
-      <c r="E27" s="63" t="s">
+      <c r="E27" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7843,16 +8240,16 @@
       <c r="A28" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="54">
+      <c r="B28" s="56">
         <v>45986</v>
       </c>
-      <c r="C28" s="54">
+      <c r="C28" s="56">
         <v>45987</v>
       </c>
       <c r="D28" s="23">
         <v>1</v>
       </c>
-      <c r="E28" s="63" t="s">
+      <c r="E28" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7860,16 +8257,16 @@
       <c r="A29" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="54">
+      <c r="B29" s="56">
         <v>45986</v>
       </c>
-      <c r="C29" s="54">
+      <c r="C29" s="56">
         <v>45987</v>
       </c>
       <c r="D29" s="23">
         <v>1</v>
       </c>
-      <c r="E29" s="63" t="s">
+      <c r="E29" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7877,16 +8274,16 @@
       <c r="A30" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="54">
+      <c r="B30" s="56">
         <v>45986</v>
       </c>
-      <c r="C30" s="54">
+      <c r="C30" s="56">
         <v>45987</v>
       </c>
       <c r="D30" s="23">
         <v>1</v>
       </c>
-      <c r="E30" s="63" t="s">
+      <c r="E30" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7894,16 +8291,16 @@
       <c r="A31" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="54">
+      <c r="B31" s="56">
         <v>45992</v>
       </c>
-      <c r="C31" s="54">
+      <c r="C31" s="56">
         <v>45993</v>
       </c>
       <c r="D31" s="23">
         <v>1</v>
       </c>
-      <c r="E31" s="63" t="s">
+      <c r="E31" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7911,16 +8308,16 @@
       <c r="A32" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="54">
+      <c r="B32" s="56">
         <v>45992</v>
       </c>
-      <c r="C32" s="54">
+      <c r="C32" s="56">
         <v>45993</v>
       </c>
       <c r="D32" s="23">
         <v>1</v>
       </c>
-      <c r="E32" s="63" t="s">
+      <c r="E32" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7928,16 +8325,16 @@
       <c r="A33" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="54">
+      <c r="B33" s="56">
         <v>45992</v>
       </c>
-      <c r="C33" s="54">
+      <c r="C33" s="56">
         <v>45993</v>
       </c>
       <c r="D33" s="23">
         <v>1</v>
       </c>
-      <c r="E33" s="63" t="s">
+      <c r="E33" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -7945,16 +8342,16 @@
       <c r="A34" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="54">
+      <c r="B34" s="56">
         <v>45993</v>
       </c>
-      <c r="C34" s="54">
+      <c r="C34" s="56">
         <v>45993</v>
       </c>
       <c r="D34" s="23">
         <v>1</v>
       </c>
-      <c r="E34" s="63" t="s">
+      <c r="E34" s="65" t="s">
         <v>35</v>
       </c>
     </row>
@@ -8561,33 +8958,33 @@
   <sheetPr/>
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="18.1111111111111" customWidth="1"/>
+    <col min="1" max="1" width="24.7777777777778" customWidth="1"/>
     <col min="2" max="2" width="57.6666666666667" customWidth="1"/>
     <col min="3" max="3" width="121.777777777778" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="50" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" ht="409.5" spans="1:3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="52" t="s">
         <v>64</v>
       </c>
       <c r="C2" s="30" t="s">
@@ -8630,39 +9027,49 @@
       <c r="A7" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="40" t="s">
         <v>73</v>
       </c>
       <c r="C7" s="29"/>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
+    <row r="8" ht="158.4" spans="1:3">
+      <c r="A8" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>75</v>
+      </c>
       <c r="C8" s="29"/>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="29"/>
-      <c r="B9" s="29"/>
+    <row r="9" ht="345.6" spans="1:3">
+      <c r="A9" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>77</v>
+      </c>
       <c r="C9" s="29"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" ht="403.2" spans="1:3">
       <c r="A10" s="29"/>
-      <c r="B10" s="29"/>
+      <c r="B10" s="40" t="s">
+        <v>78</v>
+      </c>
       <c r="C10" s="29"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="29"/>
-      <c r="B11" s="29"/>
       <c r="C11" s="29"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="29"/>
-      <c r="B12" s="29"/>
       <c r="C12" s="29"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" ht="409.5" spans="1:3">
       <c r="A13" s="29"/>
-      <c r="B13" s="29"/>
+      <c r="B13" s="40" t="s">
+        <v>79</v>
+      </c>
       <c r="C13" s="29"/>
     </row>
     <row r="14" spans="1:3">
@@ -8879,13 +9286,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="59.7777777777778" customWidth="1"/>
     <col min="2" max="2" width="79.7777777777778" customWidth="1"/>
@@ -8893,52 +9300,57 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="27" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="42">
+      <c r="A2" s="45">
         <v>45962</v>
       </c>
       <c r="B2" s="29"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="43" t="s">
-        <v>76</v>
+        <v>81</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="43" t="s">
-        <v>78</v>
+        <v>83</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" s="43" t="s">
-        <v>80</v>
+        <v>85</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="44">
+      <c r="A6" s="47">
         <v>45969</v>
       </c>
       <c r="B6" s="29"/>
     </row>
-    <row r="7" s="41" customFormat="1" ht="57.6" spans="1:2">
-      <c r="A7" s="45" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="46" t="s">
-        <v>82</v>
+    <row r="7" s="44" customFormat="1" ht="57.6" spans="1:2">
+      <c r="A7" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="49" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" ht="187.2" spans="1:1">
+      <c r="A10" s="43" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -8952,8 +9364,8 @@
   <sheetPr/>
   <dimension ref="A1:D87"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -8966,10 +9378,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="27" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="C1" s="28" t="s">
         <v>62</v>
@@ -8977,144 +9389,144 @@
     </row>
     <row r="2" ht="201.6" spans="1:3">
       <c r="A2" s="29" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" ht="100.8" spans="1:3">
       <c r="A3" s="29" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" ht="72" spans="1:3">
       <c r="A4" s="31" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="C4" s="29"/>
     </row>
     <row r="5" ht="129.6" spans="1:3">
       <c r="A5" s="30" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" ht="129.6" spans="1:4">
       <c r="A6" s="30" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" ht="158.4" spans="1:3">
       <c r="A7" s="23" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" ht="86.4" spans="1:3">
       <c r="A8" s="25" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="C8" s="29"/>
     </row>
     <row r="9" ht="129.6" spans="1:3">
       <c r="A9" s="25" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="C9" s="29"/>
     </row>
     <row r="10" ht="129.6" spans="1:3">
       <c r="A10" s="23" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="C10" s="29"/>
     </row>
     <row r="11" ht="158.4" spans="1:3">
       <c r="A11" s="23" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="C11" s="29"/>
     </row>
     <row r="12" ht="115.2" spans="1:3">
       <c r="A12" s="25" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" ht="158.4" spans="1:3">
       <c r="A13" s="23" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" ht="158.4" spans="1:3">
       <c r="A14" s="23" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="C14" s="30"/>
     </row>
     <row r="15" ht="43.2" spans="1:3">
       <c r="A15" s="23" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="C15" s="30"/>
     </row>
@@ -9123,10 +9535,10 @@
         <v>34</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" ht="172.8" spans="1:3">
@@ -9134,10 +9546,10 @@
         <v>36</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" ht="409.5" spans="1:4">
@@ -9145,13 +9557,13 @@
         <v>37</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" ht="409.5" spans="1:4">
@@ -9159,423 +9571,479 @@
         <v>38</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" ht="409.5" spans="1:4">
       <c r="A20" s="23" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" ht="174" customHeight="1" spans="1:3">
       <c r="A21" s="23" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C21" s="29"/>
     </row>
     <row r="22" ht="187.2" spans="1:3">
       <c r="A22" s="23" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="C22" s="29"/>
     </row>
     <row r="23" ht="244.8" spans="1:3">
       <c r="A23" s="23" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="C23" s="29"/>
     </row>
     <row r="24" ht="158.4" spans="1:3">
       <c r="A24" s="23" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="C24" s="29"/>
     </row>
     <row r="25" ht="100.8" spans="1:3">
       <c r="A25" s="23" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="C25" s="29"/>
     </row>
     <row r="26" ht="409" customHeight="1" spans="1:3">
       <c r="A26" s="23" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" ht="57.6" spans="1:3">
       <c r="A27" s="23" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="C27" s="29"/>
     </row>
     <row r="28" ht="409.5" spans="1:4">
       <c r="A28" s="23" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" ht="244.8" spans="1:3">
       <c r="A29" s="23" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" ht="244.8" spans="1:3">
       <c r="A30" s="23" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="C30" s="29"/>
     </row>
     <row r="31" ht="187.2" spans="1:3">
       <c r="A31" s="23" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="C31" s="29"/>
     </row>
     <row r="32" ht="259.2" spans="1:3">
       <c r="A32" s="35" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="B32" s="36" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="C32" s="29"/>
     </row>
     <row r="33" ht="345.6" spans="1:3">
       <c r="A33" s="35" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="B33" s="36" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="C33" s="29"/>
     </row>
     <row r="34" ht="100.8" spans="1:3">
       <c r="A34" s="23" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="C34" s="29"/>
     </row>
     <row r="35" ht="72" spans="1:3">
       <c r="A35" s="23" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="C35" s="29"/>
     </row>
     <row r="36" ht="409" customHeight="1" spans="1:3">
       <c r="A36" s="23" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" ht="187.2" spans="1:3">
       <c r="A37" s="23" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="C37" s="38"/>
     </row>
     <row r="38" ht="288" spans="1:3">
       <c r="A38" s="23" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="C38" s="39"/>
     </row>
     <row r="39" ht="216" spans="1:3">
       <c r="A39" s="23" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="C39" s="29"/>
     </row>
     <row r="40" ht="100.8" spans="1:3">
       <c r="A40" s="25" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="C40" s="29"/>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="23" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="B41" s="23"/>
       <c r="C41" s="29"/>
     </row>
     <row r="42" ht="144" spans="1:3">
       <c r="A42" s="25" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="B42" s="25" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="43" ht="57.6" spans="1:3">
       <c r="A43" s="25" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="C43" s="29"/>
     </row>
     <row r="44" ht="273.6" spans="1:3">
       <c r="A44" s="25" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="C44" s="29"/>
     </row>
     <row r="45" ht="172.8" spans="1:3">
       <c r="A45" s="23" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="C45" s="30" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
     </row>
     <row r="46" ht="43.2" spans="1:3">
       <c r="A46" s="23" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C46" s="29"/>
     </row>
     <row r="47" ht="144" spans="1:3">
       <c r="A47" s="23" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="C47" s="29"/>
     </row>
     <row r="48" ht="72" spans="1:3">
       <c r="A48" s="23" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="C48" s="29"/>
     </row>
     <row r="49" ht="57.6" spans="1:3">
       <c r="A49" s="23" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="B49" s="25" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C49" s="29"/>
     </row>
     <row r="50" ht="28.8" spans="1:3">
       <c r="A50" s="23" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="B50" s="25" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="C50" s="29"/>
     </row>
     <row r="51" ht="230.4" spans="1:3">
       <c r="A51" s="23" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="C51" s="29"/>
     </row>
     <row r="52" ht="158.4" spans="1:3">
       <c r="A52" s="23" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="C52" s="29"/>
     </row>
     <row r="53" ht="129.6" spans="1:3">
       <c r="A53" s="23" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="B53" s="25" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="C53" s="29"/>
     </row>
     <row r="54" ht="409.5" spans="1:3">
       <c r="A54" s="23" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="B54" s="25" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="C54" s="29"/>
     </row>
     <row r="55" ht="201.6" spans="1:3">
       <c r="A55" s="23" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="C55" s="30" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="56" ht="409.5" spans="1:3">
       <c r="A56" s="23"/>
-      <c r="B56" s="23"/>
+      <c r="B56" s="40" t="s">
+        <v>218</v>
+      </c>
       <c r="C56" s="29"/>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" ht="409.5" spans="1:3">
       <c r="A57" s="23"/>
-      <c r="B57" s="23"/>
+      <c r="B57" s="40" t="s">
+        <v>219</v>
+      </c>
       <c r="C57" s="29"/>
     </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="23"/>
-      <c r="B58" s="23"/>
+    <row r="58" ht="158.4" spans="1:3">
+      <c r="A58" t="s">
+        <v>220</v>
+      </c>
+      <c r="B58" s="25" t="s">
+        <v>221</v>
+      </c>
       <c r="C58" s="29"/>
     </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="23"/>
-      <c r="B59" s="23"/>
+    <row r="59" ht="158.4" spans="1:3">
+      <c r="A59" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="B59" s="25" t="s">
+        <v>223</v>
+      </c>
       <c r="C59" s="29"/>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="23"/>
-      <c r="B60" s="23"/>
+      <c r="A60" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="B60" s="23" t="s">
+        <v>225</v>
+      </c>
       <c r="C60" s="29"/>
     </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="40"/>
-      <c r="B61" s="40"/>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="23"/>
-      <c r="B62" s="23"/>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="23"/>
-      <c r="B63" s="23"/>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="23"/>
-      <c r="B64" s="23"/>
-    </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="23"/>
-      <c r="B65" s="23"/>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" s="23"/>
-      <c r="B66" s="23"/>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" s="23"/>
-      <c r="B67" s="23"/>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="23"/>
-      <c r="B68" s="23"/>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" s="23"/>
-      <c r="B69" s="23"/>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="23"/>
-      <c r="B70" s="23"/>
+    <row r="61" ht="144" spans="1:2">
+      <c r="A61" s="41" t="s">
+        <v>226</v>
+      </c>
+      <c r="B61" s="42" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="62" ht="230.4" spans="1:2">
+      <c r="A62" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="B62" s="25" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="63" ht="43.2" spans="1:2">
+      <c r="A63" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="B63" s="25" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="64" ht="28.8" spans="1:2">
+      <c r="A64" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="B64" s="25" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="65" ht="144" spans="1:2">
+      <c r="A65" t="s">
+        <v>234</v>
+      </c>
+      <c r="B65" s="25" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="66" ht="158.4" spans="1:2">
+      <c r="A66" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="B66" s="25" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="67" ht="28.8" spans="1:2">
+      <c r="A67" t="s">
+        <v>238</v>
+      </c>
+      <c r="B67" s="43" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="68" ht="57.6" spans="1:2">
+      <c r="A68" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="B68" s="25" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="69" ht="28.8" spans="1:2">
+      <c r="A69" t="s">
+        <v>242</v>
+      </c>
+      <c r="B69" s="25" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="70" ht="28.8" spans="1:2">
+      <c r="A70" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="B70" s="25" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="23"/>
@@ -9671,72 +10139,72 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="23" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="23" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="24" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="25" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="25" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="23" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="25" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="25" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="23" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="23" t="s">
-        <v>211</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="25" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="23" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="23" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="23" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:1">
@@ -9754,7 +10222,7 @@
         <v>38</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>212</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -9764,76 +10232,76 @@
     </row>
     <row r="19" ht="72" spans="1:1">
       <c r="A19" s="7" t="s">
-        <v>213</v>
+        <v>248</v>
       </c>
     </row>
     <row r="20" ht="72" spans="1:1">
       <c r="A20" s="7" t="s">
-        <v>214</v>
+        <v>249</v>
       </c>
     </row>
     <row r="21" ht="100.8" spans="1:2">
       <c r="A21" t="s">
-        <v>215</v>
+        <v>250</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>216</v>
+        <v>251</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="26" t="s">
-        <v>217</v>
+        <v>252</v>
       </c>
       <c r="B22" t="s">
-        <v>218</v>
+        <v>253</v>
       </c>
     </row>
     <row r="23" ht="57.6" spans="1:2">
       <c r="A23" t="s">
-        <v>219</v>
+        <v>254</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>220</v>
+        <v>255</v>
       </c>
     </row>
     <row r="24" ht="72" spans="1:2">
       <c r="A24" t="s">
-        <v>221</v>
+        <v>256</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>222</v>
+        <v>257</v>
       </c>
     </row>
     <row r="25" ht="86.4" spans="1:2">
       <c r="A25" t="s">
-        <v>223</v>
+        <v>258</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>224</v>
+        <v>259</v>
       </c>
     </row>
     <row r="26" ht="43.2" spans="1:2">
       <c r="A26" t="s">
-        <v>225</v>
+        <v>260</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>226</v>
+        <v>261</v>
       </c>
     </row>
     <row r="27" ht="28.8" spans="1:2">
       <c r="A27" t="s">
-        <v>227</v>
+        <v>262</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>228</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" ht="43.2" spans="1:2">
       <c r="A28" t="s">
-        <v>229</v>
+        <v>264</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>230</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -9855,17 +10323,17 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" s="22" t="s">
-        <v>231</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>232</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>233</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -9894,302 +10362,302 @@
   <sheetData>
     <row r="1" spans="2:3">
       <c r="B1" s="16" t="s">
-        <v>234</v>
+        <v>269</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>235</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="2:3">
       <c r="B2" s="17" t="s">
-        <v>236</v>
+        <v>271</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>237</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="17" t="s">
-        <v>238</v>
+        <v>273</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>237</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="17" t="s">
-        <v>239</v>
+        <v>274</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>237</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5" spans="2:3">
       <c r="B5" s="17" t="s">
-        <v>240</v>
+        <v>275</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>237</v>
+        <v>272</v>
       </c>
     </row>
     <row r="6" spans="2:3">
       <c r="B6" s="17" t="s">
-        <v>241</v>
+        <v>276</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>237</v>
+        <v>272</v>
       </c>
     </row>
     <row r="7" spans="2:3">
       <c r="B7" s="17" t="s">
-        <v>242</v>
+        <v>277</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>237</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" ht="43.2" spans="2:3">
       <c r="B8" s="17" t="s">
-        <v>243</v>
+        <v>278</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>244</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" s="18" t="s">
-        <v>245</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>246</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" ht="23.4" spans="2:2">
       <c r="B11" s="19" t="s">
-        <v>247</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" spans="2:2">
       <c r="B12" t="s">
-        <v>248</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" t="s">
-        <v>249</v>
+        <v>284</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" s="20" t="s">
-        <v>250</v>
+        <v>285</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" s="20" t="s">
-        <v>251</v>
+        <v>286</v>
       </c>
     </row>
     <row r="16" spans="2:2">
       <c r="B16" s="20" t="s">
-        <v>252</v>
+        <v>287</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="20" t="s">
-        <v>253</v>
+        <v>288</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="20" t="s">
-        <v>254</v>
+        <v>289</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>255</v>
+        <v>290</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="20" t="s">
-        <v>256</v>
+        <v>291</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="20" t="s">
-        <v>257</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" s="20" t="s">
-        <v>258</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" s="20" t="s">
-        <v>259</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" s="20" t="s">
-        <v>260</v>
+        <v>295</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>261</v>
+        <v>296</v>
       </c>
     </row>
     <row r="26" ht="23.4" spans="2:2">
       <c r="B26" s="19" t="s">
-        <v>262</v>
+        <v>297</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>263</v>
+        <v>298</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" s="20" t="s">
-        <v>264</v>
+        <v>299</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" s="20" t="s">
-        <v>265</v>
+        <v>300</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" s="20" t="s">
-        <v>266</v>
+        <v>301</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" s="20" t="s">
-        <v>267</v>
+        <v>302</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" s="20" t="s">
-        <v>268</v>
+        <v>303</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>269</v>
+        <v>304</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" s="20" t="s">
-        <v>270</v>
+        <v>305</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="20" t="s">
-        <v>271</v>
+        <v>306</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" s="20" t="s">
-        <v>272</v>
+        <v>307</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" s="20" t="s">
-        <v>273</v>
+        <v>308</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" s="20" t="s">
-        <v>274</v>
+        <v>309</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" s="20" t="s">
-        <v>275</v>
+        <v>310</v>
       </c>
     </row>
     <row r="40" spans="2:2">
       <c r="B40" t="s">
-        <v>276</v>
+        <v>311</v>
       </c>
     </row>
     <row r="41" ht="23.4" spans="2:2">
       <c r="B41" s="19" t="s">
-        <v>277</v>
+        <v>312</v>
       </c>
     </row>
     <row r="42" spans="2:2">
       <c r="B42" t="s">
-        <v>278</v>
+        <v>313</v>
       </c>
     </row>
     <row r="43" spans="2:2">
       <c r="B43" s="20" t="s">
-        <v>279</v>
+        <v>314</v>
       </c>
     </row>
     <row r="44" spans="2:2">
       <c r="B44" s="20" t="s">
-        <v>280</v>
+        <v>315</v>
       </c>
     </row>
     <row r="45" spans="2:2">
       <c r="B45" s="20" t="s">
-        <v>281</v>
+        <v>316</v>
       </c>
     </row>
     <row r="46" spans="2:2">
       <c r="B46" s="20" t="s">
-        <v>282</v>
+        <v>317</v>
       </c>
     </row>
     <row r="47" spans="2:2">
       <c r="B47" t="s">
-        <v>283</v>
+        <v>318</v>
       </c>
     </row>
     <row r="48" spans="2:2">
       <c r="B48" s="21" t="s">
-        <v>284</v>
+        <v>319</v>
       </c>
     </row>
     <row r="49" spans="2:2">
       <c r="B49" s="21" t="s">
-        <v>285</v>
+        <v>320</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50" s="21" t="s">
-        <v>286</v>
+        <v>321</v>
       </c>
     </row>
     <row r="51" spans="2:2">
       <c r="B51" s="21" t="s">
-        <v>287</v>
+        <v>322</v>
       </c>
     </row>
     <row r="52" spans="2:2">
       <c r="B52" t="s">
-        <v>288</v>
+        <v>323</v>
       </c>
     </row>
     <row r="54" ht="13" customHeight="1"/>
     <row r="55" ht="22" customHeight="1" spans="2:2">
       <c r="B55" s="19" t="s">
-        <v>289</v>
+        <v>324</v>
       </c>
     </row>
     <row r="56" spans="2:2">
       <c r="B56" t="s">
-        <v>290</v>
+        <v>325</v>
       </c>
     </row>
     <row r="57" spans="2:2">
       <c r="B57" s="20" t="s">
-        <v>291</v>
+        <v>326</v>
       </c>
     </row>
     <row r="58" spans="2:2">
@@ -10199,22 +10667,22 @@
     </row>
     <row r="59" spans="2:2">
       <c r="B59" s="20" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
     </row>
     <row r="60" spans="2:2">
       <c r="B60" s="20" t="s">
-        <v>292</v>
+        <v>327</v>
       </c>
     </row>
     <row r="61" spans="2:2">
       <c r="B61" s="20" t="s">
-        <v>293</v>
+        <v>328</v>
       </c>
     </row>
     <row r="62" spans="2:2">
       <c r="B62" t="s">
-        <v>294</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -10236,7 +10704,7 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="12" t="s">
-        <v>295</v>
+        <v>330</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -10251,7 +10719,7 @@
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
       <c r="N1" s="14" t="s">
-        <v>296</v>
+        <v>331</v>
       </c>
       <c r="O1" s="15"/>
       <c r="P1" s="15"/>
@@ -10493,7 +10961,7 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="12" t="s">
-        <v>297</v>
+        <v>332</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -10679,7 +11147,7 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="13" t="s">
-        <v>298</v>
+        <v>333</v>
       </c>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>

</xml_diff>

<commit_message>
23-12-25 Revision Topic - Trees maxDepth, diameterOfBT, balancedTree, LCA (lowestCommonAncestor), pathSum, pathSum2, RightSideViewTree, SameTree, invertTree, BuildTreePreIn
</commit_message>
<xml_diff>
--- a/JavaPrograms/Work Done.xlsx
+++ b/JavaPrograms/Work Done.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8280" firstSheet="4" activeTab="11"/>
+    <workbookView windowWidth="23040" windowHeight="9000" firstSheet="4" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="DSA plan" sheetId="4" r:id="rId1"/>
@@ -8085,8 +8085,8 @@
   <sheetPr/>
   <dimension ref="C2:C96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -8095,7 +8095,7 @@
     <col min="3" max="3" width="144.666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="409.5" spans="3:3">
+    <row r="2" spans="3:3">
       <c r="C2" s="1" t="s">
         <v>454</v>
       </c>

</xml_diff>